<commit_message>
Updated BGR model - 2025-07-29 00:57
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F4944D1-35ED-4760-844B-0C03D6AB66C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9535F261-0B84-4B77-B15E-9E3602F5AC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -304,7 +304,7 @@
     <t>BGR</t>
   </si>
   <si>
-    <t>Electricity Trade Data (TWh)</t>
+    <t>Electricity Trade Data (TWh) - Source: UNSD</t>
   </si>
   <si>
     <t>ISO</t>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 06:19
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9535F261-0B84-4B77-B15E-9E3602F5AC08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8484D292-961E-4364-900A-BD7985E31203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,9 @@
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
 <metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
+  <metadataTypes count="2">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
   <futureMetadata name="XLDAPR" count="1">
     <bk>
@@ -47,16 +48,40 @@
       </extLst>
     </bk>
   </futureMetadata>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+    <bk>
+      <rc t="2" v="1"/>
+    </bk>
+  </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="86">
   <si>
     <t>bioenergy</t>
   </si>
@@ -381,6 +406,72 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>13</v>
+    <v>3</v>
+  </rv>
+  <rv s="1">
+    <v>13</v>
+    <v>1</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="subType" t="i"/>
+  </s>
+  <s t="_error">
+    <k n="errorType" t="i"/>
+    <k n="propagated" t="b"/>
+  </s>
+</rvStructures>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -781,14 +872,14 @@
       <c r="P4" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" s="4" cm="1">
+      <c r="Q4" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="Q4">MAX(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MAX(_xlpm.r))), historical_data!$C$24:$C$30=$P4))</f>
-        <v>0.50828415182197206</v>
+        <v>#VALUE!</v>
       </c>
       <c r="R4" s="4"/>
-      <c r="S4" s="4" cm="1">
+      <c r="S4" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="S4">MIN(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MIN(_xlpm.r))), historical_data!$C$24:$C$30=$P4))</f>
-        <v>0.25824553878597789</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="5" spans="2:36" x14ac:dyDescent="0.45">
@@ -811,17 +902,17 @@
       <c r="P5" t="s">
         <v>2</v>
       </c>
-      <c r="Q5" s="4" cm="1">
+      <c r="Q5" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="Q5">MAX(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MAX(_xlpm.r))), historical_data!$C$24:$C$30=$P5))</f>
-        <v>0.29014459665144599</v>
-      </c>
-      <c r="R5" s="4">
+        <v>#VALUE!</v>
+      </c>
+      <c r="R5" s="4" t="e" vm="2">
         <f>IF(Q5&gt;0.7,Q5,0.7)</f>
-        <v>0.7</v>
-      </c>
-      <c r="S5" s="4" cm="1">
+        <v>#VALUE!</v>
+      </c>
+      <c r="S5" s="4" t="e" cm="1" vm="1">
         <f t="array" ref="S5">MIN(_xlfn._xlws.FILTER(_xlfn.BYROW(historical_data!$D$24:$AA$30, _xlfn.LAMBDA(_xlpm.r, MIN(_xlpm.r))), historical_data!$C$24:$C$30=$P5))</f>
-        <v>0.14840182648401828</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.45">
@@ -931,9 +1022,9 @@
       <c r="X8">
         <v>1</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8" s="3" t="e" vm="2">
         <f>-Q4*$Q$1*8.76</f>
-        <v>-4.8978260869565231</v>
+        <v>#VALUE!</v>
       </c>
       <c r="Z8" s="3"/>
       <c r="AA8">
@@ -951,9 +1042,9 @@
       <c r="AF8">
         <v>1</v>
       </c>
-      <c r="AG8" s="3">
+      <c r="AG8" s="3" t="e" vm="2">
         <f>-S4*$S$1*8.76</f>
-        <v>-2.0360078277886497</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AI8">
         <v>0</v>
@@ -975,13 +1066,13 @@
       <c r="X9">
         <v>1</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9" s="3" t="e" vm="2">
         <f>-Q5*$Q$1*8.76</f>
-        <v>-2.7958333333333334</v>
-      </c>
-      <c r="Z9" s="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="Z9" s="3" t="e" vm="2">
         <f>-R5*$Q$1*8.76</f>
-        <v>-6.7451999999999996</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AA9">
         <v>0</v>
@@ -998,9 +1089,9 @@
       <c r="AF9">
         <v>1</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AG9" s="3" t="e" vm="2">
         <f>-S5*$S$1*8.76</f>
-        <v>-1.1700000000000004</v>
+        <v>#VALUE!</v>
       </c>
       <c r="AI9">
         <v>0</v>
@@ -1172,7 +1263,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA35"/>
+  <dimension ref="A1:AA47"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="U26" sqref="U26"/>
@@ -1656,852 +1747,801 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17">
+        <v>2000</v>
+      </c>
+      <c r="C17">
+        <v>2001</v>
+      </c>
+      <c r="D17">
+        <v>2002</v>
+      </c>
+      <c r="E17">
+        <v>2003</v>
+      </c>
+      <c r="F17">
+        <v>2004</v>
+      </c>
+      <c r="G17">
+        <v>2005</v>
+      </c>
+      <c r="H17">
+        <v>2006</v>
+      </c>
+      <c r="I17">
+        <v>2007</v>
+      </c>
+      <c r="J17">
+        <v>2008</v>
+      </c>
+      <c r="K17">
+        <v>2009</v>
+      </c>
+      <c r="L17">
+        <v>2010</v>
+      </c>
+      <c r="M17">
+        <v>2011</v>
+      </c>
+      <c r="N17">
+        <v>2012</v>
+      </c>
+      <c r="O17">
+        <v>2013</v>
+      </c>
+      <c r="P17">
+        <v>2014</v>
+      </c>
+      <c r="Q17">
+        <v>2015</v>
+      </c>
+      <c r="R17">
+        <v>2016</v>
+      </c>
+      <c r="S17">
+        <v>2017</v>
+      </c>
+      <c r="T17">
+        <v>2018</v>
+      </c>
+      <c r="U17">
+        <v>2019</v>
+      </c>
+      <c r="V17">
+        <v>2020</v>
+      </c>
+      <c r="W17">
+        <v>2021</v>
+      </c>
+      <c r="X17">
+        <v>2022</v>
+      </c>
+      <c r="Y17">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0.22831050228310504</v>
+      </c>
+      <c r="K18">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="L18">
+        <v>0.45662100456621008</v>
+      </c>
+      <c r="M18">
+        <v>0.68493150684931503</v>
+      </c>
+      <c r="N18">
+        <v>0.7990867579908677</v>
+      </c>
+      <c r="O18">
+        <v>0.41856925418569257</v>
+      </c>
+      <c r="P18">
+        <v>0.57077625570776258</v>
+      </c>
+      <c r="Q18">
+        <v>0.61643835616438358</v>
+      </c>
+      <c r="R18">
+        <v>0.66590563165905636</v>
+      </c>
+      <c r="S18">
+        <v>0.91324200913242015</v>
+      </c>
+      <c r="T18">
+        <v>2.5603392041748205</v>
+      </c>
+      <c r="U18">
+        <v>3.4627092846270933</v>
+      </c>
+      <c r="V18">
+        <v>3.8812785388127851</v>
+      </c>
+      <c r="W18">
+        <v>5.9132420091324196</v>
+      </c>
+      <c r="X18">
+        <v>5.1141552511415531</v>
+      </c>
+      <c r="Y18">
+        <v>4.9771689497716896</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>0.34409073920603195</v>
+      </c>
+      <c r="C19">
+        <v>0.39609028421001313</v>
+      </c>
+      <c r="D19">
+        <v>0.34896569655015519</v>
+      </c>
+      <c r="E19">
+        <v>0.3908090804205463</v>
+      </c>
+      <c r="F19">
+        <v>0.3922789539227895</v>
+      </c>
+      <c r="G19">
+        <v>0.38314653383146535</v>
+      </c>
+      <c r="H19">
+        <v>0.396222498962225</v>
+      </c>
+      <c r="I19">
+        <v>0.46430053964300544</v>
+      </c>
+      <c r="J19">
+        <v>0.48111249481112495</v>
+      </c>
+      <c r="K19">
+        <v>0.42782873873654675</v>
+      </c>
+      <c r="L19">
+        <v>0.45844586648499153</v>
+      </c>
+      <c r="M19">
+        <v>0.49726171897578175</v>
+      </c>
+      <c r="N19">
+        <v>0.41309028379862439</v>
+      </c>
+      <c r="O19">
+        <v>0.36227010141320837</v>
+      </c>
+      <c r="P19">
+        <v>0.41231328844516674</v>
+      </c>
+      <c r="Q19">
+        <v>0.50828415182197206</v>
+      </c>
+      <c r="R19">
+        <v>0.4369935206742831</v>
+      </c>
+      <c r="S19">
+        <v>0.46734400271649285</v>
+      </c>
+      <c r="T19">
+        <v>0.41685655309224456</v>
+      </c>
+      <c r="U19">
+        <v>0.38424076705180099</v>
+      </c>
+      <c r="V19">
+        <v>0.30180771877150181</v>
+      </c>
+      <c r="W19">
+        <v>0.38178341330902782</v>
+      </c>
+      <c r="X19">
+        <v>0.48677943686388042</v>
+      </c>
+      <c r="Y19">
+        <v>0.25824553878597789</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>0.19642930601834707</v>
+      </c>
+      <c r="C20">
+        <v>0.19642930601834707</v>
+      </c>
+      <c r="D20">
+        <v>0.1583775556378296</v>
+      </c>
+      <c r="E20">
+        <v>0.18100292072894811</v>
+      </c>
+      <c r="F20">
+        <v>0.15323542720802993</v>
+      </c>
+      <c r="G20">
+        <v>0.1779176436710683</v>
+      </c>
+      <c r="H20">
+        <v>0.22213994816734542</v>
+      </c>
+      <c r="I20">
+        <v>0.23228111971411552</v>
+      </c>
+      <c r="J20">
+        <v>0.23426642842962081</v>
+      </c>
+      <c r="K20">
+        <v>0.19456025411951558</v>
+      </c>
+      <c r="L20">
+        <v>0.19555290847726822</v>
+      </c>
+      <c r="M20">
+        <v>0.19786910197869106</v>
+      </c>
+      <c r="N20">
+        <v>0.22450532724505329</v>
+      </c>
+      <c r="O20">
+        <v>0.2226027397260274</v>
+      </c>
+      <c r="P20">
+        <v>0.20357686453576868</v>
+      </c>
+      <c r="Q20">
+        <v>0.17694063926940642</v>
+      </c>
+      <c r="R20">
+        <v>0.1950152207001522</v>
+      </c>
+      <c r="S20">
+        <v>0.18359969558599698</v>
+      </c>
+      <c r="T20">
+        <v>0.19216133942161343</v>
+      </c>
+      <c r="U20">
+        <v>0.20452815829528159</v>
+      </c>
+      <c r="V20">
+        <v>0.21784627092846273</v>
+      </c>
+      <c r="W20">
+        <v>0.29014459665144599</v>
+      </c>
+      <c r="X20">
+        <v>0.1950152207001522</v>
+      </c>
+      <c r="Y20">
+        <v>0.14840182648401828</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21">
+        <v>0.29434148088459128</v>
+      </c>
+      <c r="C21">
+        <v>0.22423352902804958</v>
+      </c>
+      <c r="D21">
+        <v>0.22408253001860307</v>
+      </c>
+      <c r="E21">
+        <v>0.20686315206863154</v>
+      </c>
+      <c r="F21">
+        <v>0.18103408514367419</v>
+      </c>
+      <c r="G21">
+        <v>0.24791291914579586</v>
+      </c>
+      <c r="H21">
+        <v>0.2427240440939071</v>
+      </c>
+      <c r="I21">
+        <v>0.16072605011472321</v>
+      </c>
+      <c r="J21">
+        <v>0.1502326182476092</v>
+      </c>
+      <c r="K21">
+        <v>0.18296846327828276</v>
+      </c>
+      <c r="L21">
+        <v>0.26339491433119683</v>
+      </c>
+      <c r="M21">
+        <v>0.14626141552511415</v>
+      </c>
+      <c r="N21">
+        <v>0.15647142182333496</v>
+      </c>
+      <c r="O21">
+        <v>0.19708855325293684</v>
+      </c>
+      <c r="P21">
+        <v>0.22250599798777185</v>
+      </c>
+      <c r="Q21">
+        <v>0.27329541057193724</v>
+      </c>
+      <c r="R21">
+        <v>0.18767897221577279</v>
+      </c>
+      <c r="S21">
+        <v>0.12870890865760704</v>
+      </c>
+      <c r="T21">
+        <v>0.23422292564900221</v>
+      </c>
+      <c r="U21">
+        <v>0.13325692663137406</v>
+      </c>
+      <c r="V21">
+        <v>0.12825410686023031</v>
+      </c>
+      <c r="W21">
+        <v>0.21921446633557101</v>
+      </c>
+      <c r="X21">
+        <v>0.17145847997545438</v>
+      </c>
+      <c r="Y21">
+        <v>0.14032522966412186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22">
+        <v>0.58791571267802401</v>
+      </c>
+      <c r="C22">
+        <v>0.632219592016247</v>
+      </c>
+      <c r="D22">
+        <v>0.84860999194198217</v>
+      </c>
+      <c r="E22">
+        <v>0.72522159548751008</v>
+      </c>
+      <c r="F22">
+        <v>0.70591592801504166</v>
+      </c>
+      <c r="G22">
+        <v>0.78271890948160072</v>
+      </c>
+      <c r="H22">
+        <v>0.81797273704002138</v>
+      </c>
+      <c r="I22">
+        <v>0.88425019931869253</v>
+      </c>
+      <c r="J22">
+        <v>0.95250175158850958</v>
+      </c>
+      <c r="K22">
+        <v>0.92169795366142393</v>
+      </c>
+      <c r="L22">
+        <v>0.92109395762363799</v>
+      </c>
+      <c r="M22">
+        <v>0.98511753762895304</v>
+      </c>
+      <c r="N22">
+        <v>0.94312558272968505</v>
+      </c>
+      <c r="O22">
+        <v>0.81695954983626218</v>
+      </c>
+      <c r="P22">
+        <v>0.91497163414971638</v>
+      </c>
+      <c r="Q22">
+        <v>0.88672109220054429</v>
+      </c>
+      <c r="R22">
+        <v>0.91440094569223274</v>
+      </c>
+      <c r="S22">
+        <v>0.90107317525438657</v>
+      </c>
+      <c r="T22">
+        <v>0.91608169199663791</v>
+      </c>
+      <c r="U22">
+        <v>0.94050296462891025</v>
+      </c>
+      <c r="V22">
+        <v>0.9444785206388151</v>
+      </c>
+      <c r="W22">
+        <v>0.93652740861900541</v>
+      </c>
+      <c r="X22">
+        <v>0.93482359890047495</v>
+      </c>
+      <c r="Y22">
+        <v>0.91778550171516859</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>65535</v>
+      </c>
+      <c r="C23">
+        <v>65535</v>
+      </c>
+      <c r="D23">
+        <v>65535</v>
+      </c>
+      <c r="E23">
+        <v>65535</v>
+      </c>
+      <c r="F23">
+        <v>65535</v>
+      </c>
+      <c r="G23">
+        <v>65535</v>
+      </c>
+      <c r="H23">
+        <v>65535</v>
+      </c>
+      <c r="I23">
+        <v>65535</v>
+      </c>
+      <c r="J23">
+        <v>65535</v>
+      </c>
+      <c r="K23">
+        <v>65535</v>
+      </c>
+      <c r="L23">
+        <v>65535</v>
+      </c>
+      <c r="M23">
+        <v>65535</v>
+      </c>
+      <c r="N23">
+        <v>65535</v>
+      </c>
+      <c r="O23">
+        <v>65535</v>
+      </c>
+      <c r="P23">
+        <v>65535</v>
+      </c>
+      <c r="Q23">
+        <v>65535</v>
+      </c>
+      <c r="R23">
+        <v>65535</v>
+      </c>
+      <c r="S23">
+        <v>65535</v>
+      </c>
+      <c r="T23">
+        <v>65535</v>
+      </c>
+      <c r="U23">
+        <v>65535</v>
+      </c>
+      <c r="V23">
+        <v>65535</v>
+      </c>
+      <c r="W23">
+        <v>65535</v>
+      </c>
+      <c r="X23">
+        <v>65535</v>
+      </c>
+      <c r="Y23">
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="L24">
+        <v>3.8051750380517509E-2</v>
+      </c>
+      <c r="M24">
+        <v>7.6103500761035017E-2</v>
+      </c>
+      <c r="N24">
+        <v>9.6783799880881469E-2</v>
+      </c>
+      <c r="O24">
+        <v>0.1525728837372673</v>
+      </c>
+      <c r="P24">
+        <v>0.13964622955180209</v>
+      </c>
+      <c r="Q24">
+        <v>0.15294587046149752</v>
+      </c>
+      <c r="R24">
+        <v>0.1540541738706388</v>
+      </c>
+      <c r="S24">
+        <v>0.15516247727978011</v>
+      </c>
+      <c r="T24">
+        <v>0.14851265682493239</v>
+      </c>
+      <c r="U24">
+        <v>0.15586582367404284</v>
+      </c>
+      <c r="V24">
+        <v>0.15255292652552924</v>
+      </c>
+      <c r="W24">
+        <v>0.13213245604573401</v>
+      </c>
+      <c r="X24">
+        <v>0.13711751430220961</v>
+      </c>
+      <c r="Y24">
+        <v>0.13667567483614451</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>7.6103500761035017E-2</v>
+      </c>
+      <c r="I25">
+        <v>0.19025875190258754</v>
+      </c>
+      <c r="J25">
+        <v>0.12453300124533001</v>
+      </c>
+      <c r="K25">
+        <v>8.3022000830220002E-2</v>
+      </c>
+      <c r="L25">
+        <v>0.15841953219644023</v>
+      </c>
+      <c r="M25">
+        <v>0.18180280737358362</v>
+      </c>
+      <c r="N25">
+        <v>0.20480795057749127</v>
+      </c>
+      <c r="O25">
+        <v>0.22998925597636316</v>
+      </c>
+      <c r="P25">
+        <v>0.21689497716894979</v>
+      </c>
+      <c r="Q25">
+        <v>0.23646444879321593</v>
+      </c>
+      <c r="R25">
+        <v>0.23157208088714937</v>
+      </c>
+      <c r="S25">
+        <v>0.24461839530332682</v>
+      </c>
+      <c r="T25">
+        <v>0.21526418786692761</v>
+      </c>
+      <c r="U25">
+        <v>0.21526418786692761</v>
+      </c>
+      <c r="V25">
+        <v>0.24135681669928247</v>
+      </c>
+      <c r="W25">
+        <v>0.23320287018917157</v>
+      </c>
+      <c r="X25">
+        <v>0.23483365949119375</v>
+      </c>
+      <c r="Y25">
+        <v>0.25277234181343772</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>43</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B29" t="s">
         <v>4</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C29" t="s">
         <v>5</v>
       </c>
-      <c r="D17">
+      <c r="D29">
         <v>2000</v>
       </c>
-      <c r="E17">
+      <c r="E29">
         <v>2001</v>
       </c>
-      <c r="F17">
+      <c r="F29">
         <v>2002</v>
       </c>
-      <c r="G17">
+      <c r="G29">
         <v>2003</v>
       </c>
-      <c r="H17">
+      <c r="H29">
         <v>2004</v>
       </c>
-      <c r="I17">
+      <c r="I29">
         <v>2005</v>
       </c>
-      <c r="J17">
+      <c r="J29">
         <v>2006</v>
       </c>
-      <c r="K17">
+      <c r="K29">
         <v>2007</v>
       </c>
-      <c r="L17">
+      <c r="L29">
         <v>2008</v>
       </c>
-      <c r="M17">
+      <c r="M29">
         <v>2009</v>
       </c>
-      <c r="N17">
+      <c r="N29">
         <v>2010</v>
       </c>
-      <c r="O17">
+      <c r="O29">
         <v>2011</v>
       </c>
-      <c r="P17">
+      <c r="P29">
         <v>2012</v>
       </c>
-      <c r="Q17">
+      <c r="Q29">
         <v>2013</v>
       </c>
-      <c r="R17">
+      <c r="R29">
         <v>2014</v>
       </c>
-      <c r="S17">
+      <c r="S29">
         <v>2015</v>
       </c>
-      <c r="T17">
+      <c r="T29">
         <v>2016</v>
       </c>
-      <c r="U17">
+      <c r="U29">
         <v>2017</v>
       </c>
-      <c r="V17">
+      <c r="V29">
         <v>2018</v>
       </c>
-      <c r="W17">
+      <c r="W29">
         <v>2019</v>
       </c>
-      <c r="X17">
+      <c r="X29">
         <v>2020</v>
       </c>
-      <c r="Y17">
+      <c r="Y29">
         <v>2021</v>
       </c>
-      <c r="Z17">
+      <c r="Z29">
         <v>2022</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>44</v>
-      </c>
-      <c r="B18" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18" t="s">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0.30441400304414001</v>
-      </c>
-      <c r="M18">
-        <v>0.10147133434804669</v>
-      </c>
-      <c r="N18">
-        <v>0.40447488584474894</v>
-      </c>
-      <c r="O18">
-        <v>0.5811540058115402</v>
-      </c>
-      <c r="P18">
-        <v>0.53816046966731901</v>
-      </c>
-      <c r="Q18">
-        <v>0.37067553048616708</v>
-      </c>
-      <c r="R18">
-        <v>0.57077625570776258</v>
-      </c>
-      <c r="S18">
-        <v>0.57500422797226458</v>
-      </c>
-      <c r="T18">
-        <v>0.70696146759593048</v>
-      </c>
-      <c r="U18">
-        <v>0.86924428402751963</v>
-      </c>
-      <c r="V18">
-        <v>2.5863099724480505</v>
-      </c>
-      <c r="W18">
-        <v>3.6549813955986812</v>
-      </c>
-      <c r="X18">
-        <v>4.036889720525596</v>
-      </c>
-      <c r="Y18">
-        <v>6.2453375126974553</v>
-      </c>
-      <c r="Z18">
-        <v>3.2548137163984849</v>
-      </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>44</v>
-      </c>
-      <c r="B19" t="s">
-        <v>81</v>
-      </c>
-      <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <v>0.17918731176527739</v>
-      </c>
-      <c r="E19">
-        <v>0.14535545467936098</v>
-      </c>
-      <c r="F19">
-        <v>0.15845780240593327</v>
-      </c>
-      <c r="G19">
-        <v>0.1498316039834055</v>
-      </c>
-      <c r="H19">
-        <v>0.1347902156764661</v>
-      </c>
-      <c r="I19">
-        <v>0.18958653994151151</v>
-      </c>
-      <c r="J19">
-        <v>0.18353719344825822</v>
-      </c>
-      <c r="K19">
-        <v>0.12836507928947488</v>
-      </c>
-      <c r="L19">
-        <v>0.12535509016122517</v>
-      </c>
-      <c r="M19">
-        <v>0.15416139825537606</v>
-      </c>
-      <c r="N19">
-        <v>0.21319901365069094</v>
-      </c>
-      <c r="O19">
-        <v>0.13556538436675425</v>
-      </c>
-      <c r="P19">
-        <v>0.1426745416205524</v>
-      </c>
-      <c r="Q19">
-        <v>0.17089921406444017</v>
-      </c>
-      <c r="R19">
-        <v>0.18308207829936693</v>
-      </c>
-      <c r="S19">
-        <v>0.21797454043557021</v>
-      </c>
-      <c r="T19">
-        <v>0.16178813238750592</v>
-      </c>
-      <c r="U19">
-        <v>0.11826549026371555</v>
-      </c>
-      <c r="V19">
-        <v>0.18320015783762453</v>
-      </c>
-      <c r="W19">
-        <v>0.11430375923833559</v>
-      </c>
-      <c r="X19">
-        <v>0.11225524213694742</v>
-      </c>
-      <c r="Y19">
-        <v>0.1716829439171017</v>
-      </c>
-      <c r="Z19">
-        <v>0.13069358514235713</v>
-      </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s">
-        <v>81</v>
-      </c>
-      <c r="C20" t="s">
-        <v>13</v>
-      </c>
-      <c r="D20">
-        <v>0.58751816400088952</v>
-      </c>
-      <c r="E20">
-        <v>0.63195855763612019</v>
-      </c>
-      <c r="F20">
-        <v>0.84807034848805107</v>
-      </c>
-      <c r="G20">
-        <v>0.72468873612271401</v>
-      </c>
-      <c r="H20">
-        <v>0.70518756353607848</v>
-      </c>
-      <c r="I20">
-        <v>0.78226961776024206</v>
-      </c>
-      <c r="J20">
-        <v>0.81749754243287398</v>
-      </c>
-      <c r="K20">
-        <v>0.88349648121868596</v>
-      </c>
-      <c r="L20">
-        <v>0.95119319991890894</v>
-      </c>
-      <c r="M20">
-        <v>0.92048229990249752</v>
-      </c>
-      <c r="N20">
-        <v>0.92005994960757642</v>
-      </c>
-      <c r="O20">
-        <v>0.98431753019201262</v>
-      </c>
-      <c r="P20">
-        <v>0.94540432280661413</v>
-      </c>
-      <c r="Q20">
-        <v>0.81619276686525755</v>
-      </c>
-      <c r="R20">
-        <v>0.91711461765215874</v>
-      </c>
-      <c r="S20">
-        <v>0.88913935610658323</v>
-      </c>
-      <c r="T20">
-        <v>0.91556341739152636</v>
-      </c>
-      <c r="U20">
-        <v>0.90218624426321981</v>
-      </c>
-      <c r="V20">
-        <v>0.91672584775055033</v>
-      </c>
-      <c r="W20">
-        <v>0.942110199083116</v>
-      </c>
-      <c r="X20">
-        <v>0.94612082701666678</v>
-      </c>
-      <c r="Y20">
-        <v>0.9382181082323805</v>
-      </c>
-      <c r="Z20">
-        <v>0.93680249206717758</v>
-      </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>44</v>
-      </c>
-      <c r="B21" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3</v>
-      </c>
-      <c r="D21">
-        <v>1.3728687025740881E-2</v>
-      </c>
-      <c r="E21">
-        <v>8.9246408872480296E-3</v>
-      </c>
-      <c r="F21">
-        <v>1.4064542368890371E-2</v>
-      </c>
-      <c r="G21">
-        <v>1.3440969291696423E-2</v>
-      </c>
-      <c r="H21">
-        <v>1.4367639360976603E-2</v>
-      </c>
-      <c r="I21">
-        <v>1.06544901065449E-2</v>
-      </c>
-      <c r="J21">
-        <v>6.8721033906174785E-3</v>
-      </c>
-      <c r="K21">
-        <v>1.3383397499030053E-2</v>
-      </c>
-      <c r="L21">
-        <v>6.8134032678754683E-3</v>
-      </c>
-      <c r="M21">
-        <v>8.974387151398696E-3</v>
-      </c>
-      <c r="N21">
-        <v>1.0171012962918537E-2</v>
-      </c>
-      <c r="O21">
-        <v>4.0275281549390085E-3</v>
-      </c>
-      <c r="P21">
-        <v>5.4770281784942507E-3</v>
-      </c>
-      <c r="Q21">
-        <v>5.9193423561722108E-3</v>
-      </c>
-      <c r="R21">
-        <v>5.7979529360833674E-3</v>
-      </c>
-      <c r="S21">
-        <v>5.9440758150922698E-3</v>
-      </c>
-      <c r="T21">
-        <v>1.0672682178439969E-2</v>
-      </c>
-      <c r="U21">
-        <v>1.3166338195431674E-2</v>
-      </c>
-      <c r="V21">
-        <v>1.0273264456408587E-2</v>
-      </c>
-      <c r="W21">
-        <v>1.1459284473580975E-2</v>
-      </c>
-      <c r="X21">
-        <v>1.0273784895450284E-2</v>
-      </c>
-      <c r="Y21">
-        <v>1.1799059936493149E-2</v>
-      </c>
-      <c r="Z21">
-        <v>1.5180712412366853E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>81</v>
-      </c>
-      <c r="C22" t="s">
-        <v>14</v>
-      </c>
-      <c r="K22">
-        <v>0.22831050228310501</v>
-      </c>
-      <c r="L22">
-        <v>0.1906392694063927</v>
-      </c>
-      <c r="M22">
-        <v>0.18647260273972602</v>
-      </c>
-      <c r="N22">
-        <v>6.7876712328767116E-2</v>
-      </c>
-      <c r="O22">
-        <v>7.476575935480044E-2</v>
-      </c>
-      <c r="P22">
-        <v>9.6412405035707568E-2</v>
-      </c>
-      <c r="Q22">
-        <v>0.15293804193529958</v>
-      </c>
-      <c r="R22">
-        <v>0.13941040865139273</v>
-      </c>
-      <c r="S22">
-        <v>0.1534278778672068</v>
-      </c>
-      <c r="T22">
-        <v>0.15383140488540142</v>
-      </c>
-      <c r="U22">
-        <v>0.15538589047072227</v>
-      </c>
-      <c r="V22">
-        <v>0.14838111835914639</v>
-      </c>
-      <c r="W22">
-        <v>0.15491400651998427</v>
-      </c>
-      <c r="X22">
-        <v>0.15239085998651261</v>
-      </c>
-      <c r="Y22">
-        <v>0.13133926069138591</v>
-      </c>
-      <c r="Z22">
-        <v>0.13764325363624622</v>
-      </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>44</v>
-      </c>
-      <c r="B23" t="s">
-        <v>81</v>
-      </c>
-      <c r="C23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23">
-        <v>0.11415525114155251</v>
-      </c>
-      <c r="I23">
-        <v>6.5453767123287668E-2</v>
-      </c>
-      <c r="J23">
-        <v>8.4758159986470502E-2</v>
-      </c>
-      <c r="K23">
-        <v>0.17808980213089803</v>
-      </c>
-      <c r="L23">
-        <v>0.12192381639029079</v>
-      </c>
-      <c r="M23">
-        <v>8.1248714467892558E-2</v>
-      </c>
-      <c r="N23">
-        <v>0.15938903548169775</v>
-      </c>
-      <c r="O23">
-        <v>0.18169781142649755</v>
-      </c>
-      <c r="P23">
-        <v>0.2058669391554197</v>
-      </c>
-      <c r="Q23">
-        <v>0.22956604290766625</v>
-      </c>
-      <c r="R23">
-        <v>0.2172995015710637</v>
-      </c>
-      <c r="S23">
-        <v>0.23704950320418605</v>
-      </c>
-      <c r="T23">
-        <v>0.23271503321770831</v>
-      </c>
-      <c r="U23">
-        <v>0.24584659524473154</v>
-      </c>
-      <c r="V23">
-        <v>0.21529025081619735</v>
-      </c>
-      <c r="W23">
-        <v>0.21381996798613462</v>
-      </c>
-      <c r="X23">
-        <v>0.23992922634315969</v>
-      </c>
-      <c r="Y23">
-        <v>0.2323315222455867</v>
-      </c>
-      <c r="Z23">
-        <v>0.24297964087912982</v>
-      </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>43</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27">
-        <v>2000</v>
-      </c>
-      <c r="E27">
-        <v>2001</v>
-      </c>
-      <c r="F27">
-        <v>2002</v>
-      </c>
-      <c r="G27">
-        <v>2003</v>
-      </c>
-      <c r="H27">
-        <v>2004</v>
-      </c>
-      <c r="I27">
-        <v>2005</v>
-      </c>
-      <c r="J27">
-        <v>2006</v>
-      </c>
-      <c r="K27">
-        <v>2007</v>
-      </c>
-      <c r="L27">
-        <v>2008</v>
-      </c>
-      <c r="M27">
-        <v>2009</v>
-      </c>
-      <c r="N27">
-        <v>2010</v>
-      </c>
-      <c r="O27">
-        <v>2011</v>
-      </c>
-      <c r="P27">
-        <v>2012</v>
-      </c>
-      <c r="Q27">
-        <v>2013</v>
-      </c>
-      <c r="R27">
-        <v>2014</v>
-      </c>
-      <c r="S27">
-        <v>2015</v>
-      </c>
-      <c r="T27">
-        <v>2016</v>
-      </c>
-      <c r="U27">
-        <v>2017</v>
-      </c>
-      <c r="V27">
-        <v>2018</v>
-      </c>
-      <c r="W27">
-        <v>2019</v>
-      </c>
-      <c r="X27">
-        <v>2020</v>
-      </c>
-      <c r="Y27">
-        <v>2021</v>
-      </c>
-      <c r="Z27">
-        <v>2022</v>
-      </c>
-      <c r="AA27">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" t="s">
-        <v>81</v>
-      </c>
-      <c r="C28" t="s">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
-      </c>
-      <c r="K28">
-        <v>0</v>
-      </c>
-      <c r="L28">
-        <v>0.22831050228310504</v>
-      </c>
-      <c r="M28">
-        <v>0.11415525114155252</v>
-      </c>
-      <c r="N28">
-        <v>0.45662100456621008</v>
-      </c>
-      <c r="O28">
-        <v>0.68493150684931503</v>
-      </c>
-      <c r="P28">
-        <v>0.7990867579908677</v>
-      </c>
-      <c r="Q28">
-        <v>0.41856925418569257</v>
-      </c>
-      <c r="R28">
-        <v>0.57077625570776258</v>
-      </c>
-      <c r="S28">
-        <v>0.61643835616438358</v>
-      </c>
-      <c r="T28">
-        <v>0.66590563165905636</v>
-      </c>
-      <c r="U28">
-        <v>0.91324200913242015</v>
-      </c>
-      <c r="V28">
-        <v>2.5603392041748205</v>
-      </c>
-      <c r="W28">
-        <v>3.4627092846270933</v>
-      </c>
-      <c r="X28">
-        <v>3.8812785388127851</v>
-      </c>
-      <c r="Y28">
-        <v>5.9132420091324196</v>
-      </c>
-      <c r="Z28">
-        <v>5.1141552511415531</v>
-      </c>
-      <c r="AA28">
-        <v>4.9771689497716896</v>
-      </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>46</v>
-      </c>
-      <c r="B29" t="s">
-        <v>81</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>0.34409073920603195</v>
-      </c>
-      <c r="E29">
-        <v>0.39609028421001313</v>
-      </c>
-      <c r="F29">
-        <v>0.34896569655015519</v>
-      </c>
-      <c r="G29">
-        <v>0.3908090804205463</v>
-      </c>
-      <c r="H29">
-        <v>0.3922789539227895</v>
-      </c>
-      <c r="I29">
-        <v>0.38314653383146535</v>
-      </c>
-      <c r="J29">
-        <v>0.396222498962225</v>
-      </c>
-      <c r="K29">
-        <v>0.46430053964300544</v>
-      </c>
-      <c r="L29">
-        <v>0.48111249481112495</v>
-      </c>
-      <c r="M29">
-        <v>0.42782873873654675</v>
-      </c>
-      <c r="N29">
-        <v>0.45844586648499153</v>
-      </c>
-      <c r="O29">
-        <v>0.49726171897578175</v>
-      </c>
-      <c r="P29">
-        <v>0.41309028379862439</v>
-      </c>
-      <c r="Q29">
-        <v>0.36227010141320837</v>
-      </c>
-      <c r="R29">
-        <v>0.41231328844516674</v>
-      </c>
-      <c r="S29">
-        <v>0.50828415182197206</v>
-      </c>
-      <c r="T29">
-        <v>0.4369935206742831</v>
-      </c>
-      <c r="U29">
-        <v>0.46734400271649285</v>
-      </c>
-      <c r="V29">
-        <v>0.41685655309224456</v>
-      </c>
-      <c r="W29">
-        <v>0.38424076705180099</v>
-      </c>
-      <c r="X29">
-        <v>0.30180771877150181</v>
-      </c>
-      <c r="Y29">
-        <v>0.38178341330902782</v>
-      </c>
-      <c r="Z29">
-        <v>0.48677943686388042</v>
-      </c>
-      <c r="AA29">
-        <v>0.25824553878597789</v>
-      </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>46</v>
       </c>
       <c r="B30" t="s">
         <v>81</v>
       </c>
       <c r="C30" t="s">
-        <v>2</v>
-      </c>
-      <c r="D30">
-        <v>0.19642930601834707</v>
-      </c>
-      <c r="E30">
-        <v>0.19642930601834707</v>
-      </c>
-      <c r="F30">
-        <v>0.1583775556378296</v>
-      </c>
-      <c r="G30">
-        <v>0.18100292072894811</v>
-      </c>
-      <c r="H30">
-        <v>0.15323542720802993</v>
-      </c>
-      <c r="I30">
-        <v>0.1779176436710683</v>
-      </c>
-      <c r="J30">
-        <v>0.22213994816734542</v>
-      </c>
-      <c r="K30">
-        <v>0.23228111971411552</v>
+        <v>0</v>
       </c>
       <c r="L30">
-        <v>0.23426642842962081</v>
+        <v>0.30441400304414001</v>
       </c>
       <c r="M30">
-        <v>0.19456025411951558</v>
+        <v>0.10147133434804669</v>
       </c>
       <c r="N30">
-        <v>0.19555290847726822</v>
+        <v>0.40447488584474894</v>
       </c>
       <c r="O30">
-        <v>0.19786910197869106</v>
+        <v>0.5811540058115402</v>
       </c>
       <c r="P30">
-        <v>0.22450532724505329</v>
+        <v>0.53816046966731901</v>
       </c>
       <c r="Q30">
-        <v>0.2226027397260274</v>
+        <v>0.37067553048616708</v>
       </c>
       <c r="R30">
-        <v>0.20357686453576868</v>
+        <v>0.57077625570776258</v>
       </c>
       <c r="S30">
-        <v>0.17694063926940642</v>
+        <v>0.57500422797226458</v>
       </c>
       <c r="T30">
-        <v>0.1950152207001522</v>
+        <v>0.70696146759593048</v>
       </c>
       <c r="U30">
-        <v>0.18359969558599698</v>
+        <v>0.86924428402751963</v>
       </c>
       <c r="V30">
-        <v>0.19216133942161343</v>
+        <v>2.5863099724480505</v>
       </c>
       <c r="W30">
-        <v>0.20452815829528159</v>
+        <v>3.6549813955986812</v>
       </c>
       <c r="X30">
-        <v>0.21784627092846273</v>
+        <v>4.036889720525596</v>
       </c>
       <c r="Y30">
-        <v>0.29014459665144599</v>
+        <v>6.2453375126974553</v>
       </c>
       <c r="Z30">
-        <v>0.1950152207001522</v>
-      </c>
-      <c r="AA30">
-        <v>0.14840182648401828</v>
-      </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
+        <v>3.2548137163984849</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s">
         <v>81</v>
@@ -2510,81 +2550,78 @@
         <v>12</v>
       </c>
       <c r="D31">
-        <v>0.29434148088459128</v>
+        <v>0.17918731176527739</v>
       </c>
       <c r="E31">
-        <v>0.22423352902804958</v>
+        <v>0.14535545467936098</v>
       </c>
       <c r="F31">
-        <v>0.22408253001860307</v>
+        <v>0.15845780240593327</v>
       </c>
       <c r="G31">
-        <v>0.20686315206863154</v>
+        <v>0.1498316039834055</v>
       </c>
       <c r="H31">
-        <v>0.18103408514367419</v>
+        <v>0.1347902156764661</v>
       </c>
       <c r="I31">
-        <v>0.24791291914579586</v>
+        <v>0.18958653994151151</v>
       </c>
       <c r="J31">
-        <v>0.2427240440939071</v>
+        <v>0.18353719344825822</v>
       </c>
       <c r="K31">
-        <v>0.16072605011472321</v>
+        <v>0.12836507928947488</v>
       </c>
       <c r="L31">
-        <v>0.1502326182476092</v>
+        <v>0.12535509016122517</v>
       </c>
       <c r="M31">
-        <v>0.18296846327828276</v>
+        <v>0.15416139825537606</v>
       </c>
       <c r="N31">
-        <v>0.26339491433119683</v>
+        <v>0.21319901365069094</v>
       </c>
       <c r="O31">
-        <v>0.14626141552511415</v>
+        <v>0.13556538436675425</v>
       </c>
       <c r="P31">
-        <v>0.15647142182333496</v>
+        <v>0.1426745416205524</v>
       </c>
       <c r="Q31">
-        <v>0.19708855325293684</v>
+        <v>0.17089921406444017</v>
       </c>
       <c r="R31">
-        <v>0.22250599798777185</v>
+        <v>0.18308207829936693</v>
       </c>
       <c r="S31">
-        <v>0.27329541057193724</v>
+        <v>0.21797454043557021</v>
       </c>
       <c r="T31">
-        <v>0.18767897221577279</v>
+        <v>0.16178813238750592</v>
       </c>
       <c r="U31">
-        <v>0.12870890865760704</v>
+        <v>0.11826549026371555</v>
       </c>
       <c r="V31">
-        <v>0.23422292564900221</v>
+        <v>0.18320015783762453</v>
       </c>
       <c r="W31">
-        <v>0.13325692663137406</v>
+        <v>0.11430375923833559</v>
       </c>
       <c r="X31">
-        <v>0.12825410686023031</v>
+        <v>0.11225524213694742</v>
       </c>
       <c r="Y31">
-        <v>0.21921446633557101</v>
+        <v>0.1716829439171017</v>
       </c>
       <c r="Z31">
-        <v>0.17145847997545438</v>
-      </c>
-      <c r="AA31">
-        <v>0.14032522966412186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
+        <v>0.13069358514235713</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B32" t="s">
         <v>81</v>
@@ -2593,81 +2630,78 @@
         <v>13</v>
       </c>
       <c r="D32">
-        <v>0.58791571267802401</v>
+        <v>0.58751816400088952</v>
       </c>
       <c r="E32">
-        <v>0.632219592016247</v>
+        <v>0.63195855763612019</v>
       </c>
       <c r="F32">
-        <v>0.84860999194198217</v>
+        <v>0.84807034848805107</v>
       </c>
       <c r="G32">
-        <v>0.72522159548751008</v>
+        <v>0.72468873612271401</v>
       </c>
       <c r="H32">
-        <v>0.70591592801504166</v>
+        <v>0.70518756353607848</v>
       </c>
       <c r="I32">
-        <v>0.78271890948160072</v>
+        <v>0.78226961776024206</v>
       </c>
       <c r="J32">
-        <v>0.81797273704002138</v>
+        <v>0.81749754243287398</v>
       </c>
       <c r="K32">
-        <v>0.88425019931869253</v>
+        <v>0.88349648121868596</v>
       </c>
       <c r="L32">
-        <v>0.95250175158850958</v>
+        <v>0.95119319991890894</v>
       </c>
       <c r="M32">
-        <v>0.92169795366142393</v>
+        <v>0.92048229990249752</v>
       </c>
       <c r="N32">
-        <v>0.92109395762363799</v>
+        <v>0.92005994960757642</v>
       </c>
       <c r="O32">
-        <v>0.98511753762895304</v>
+        <v>0.98431753019201262</v>
       </c>
       <c r="P32">
-        <v>0.94312558272968505</v>
+        <v>0.94540432280661413</v>
       </c>
       <c r="Q32">
-        <v>0.81695954983626218</v>
+        <v>0.81619276686525755</v>
       </c>
       <c r="R32">
-        <v>0.91497163414971638</v>
+        <v>0.91711461765215874</v>
       </c>
       <c r="S32">
-        <v>0.88672109220054429</v>
+        <v>0.88913935610658323</v>
       </c>
       <c r="T32">
-        <v>0.91440094569223274</v>
+        <v>0.91556341739152636</v>
       </c>
       <c r="U32">
-        <v>0.90107317525438657</v>
+        <v>0.90218624426321981</v>
       </c>
       <c r="V32">
-        <v>0.91608169199663791</v>
+        <v>0.91672584775055033</v>
       </c>
       <c r="W32">
-        <v>0.94050296462891025</v>
+        <v>0.942110199083116</v>
       </c>
       <c r="X32">
-        <v>0.9444785206388151</v>
+        <v>0.94612082701666678</v>
       </c>
       <c r="Y32">
-        <v>0.93652740861900541</v>
+        <v>0.9382181082323805</v>
       </c>
       <c r="Z32">
-        <v>0.93482359890047495</v>
-      </c>
-      <c r="AA32">
-        <v>0.91778550171516859</v>
+        <v>0.93680249206717758</v>
       </c>
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
         <v>81</v>
@@ -2676,81 +2710,78 @@
         <v>3</v>
       </c>
       <c r="D33">
-        <v>65535</v>
+        <v>1.3728687025740881E-2</v>
       </c>
       <c r="E33">
-        <v>65535</v>
+        <v>8.9246408872480296E-3</v>
       </c>
       <c r="F33">
-        <v>65535</v>
+        <v>1.4064542368890371E-2</v>
       </c>
       <c r="G33">
-        <v>65535</v>
+        <v>1.3440969291696423E-2</v>
       </c>
       <c r="H33">
-        <v>65535</v>
+        <v>1.4367639360976603E-2</v>
       </c>
       <c r="I33">
-        <v>65535</v>
+        <v>1.06544901065449E-2</v>
       </c>
       <c r="J33">
-        <v>65535</v>
+        <v>6.8721033906174785E-3</v>
       </c>
       <c r="K33">
-        <v>65535</v>
+        <v>1.3383397499030053E-2</v>
       </c>
       <c r="L33">
-        <v>65535</v>
+        <v>6.8134032678754683E-3</v>
       </c>
       <c r="M33">
-        <v>65535</v>
+        <v>8.974387151398696E-3</v>
       </c>
       <c r="N33">
-        <v>65535</v>
+        <v>1.0171012962918537E-2</v>
       </c>
       <c r="O33">
-        <v>65535</v>
+        <v>4.0275281549390085E-3</v>
       </c>
       <c r="P33">
-        <v>65535</v>
+        <v>5.4770281784942507E-3</v>
       </c>
       <c r="Q33">
-        <v>65535</v>
+        <v>5.9193423561722108E-3</v>
       </c>
       <c r="R33">
-        <v>65535</v>
+        <v>5.7979529360833674E-3</v>
       </c>
       <c r="S33">
-        <v>65535</v>
+        <v>5.9440758150922698E-3</v>
       </c>
       <c r="T33">
-        <v>65535</v>
+        <v>1.0672682178439969E-2</v>
       </c>
       <c r="U33">
-        <v>65535</v>
+        <v>1.3166338195431674E-2</v>
       </c>
       <c r="V33">
-        <v>65535</v>
+        <v>1.0273264456408587E-2</v>
       </c>
       <c r="W33">
-        <v>65535</v>
+        <v>1.1459284473580975E-2</v>
       </c>
       <c r="X33">
-        <v>65535</v>
+        <v>1.0273784895450284E-2</v>
       </c>
       <c r="Y33">
-        <v>65535</v>
+        <v>1.1799059936493149E-2</v>
       </c>
       <c r="Z33">
-        <v>65535</v>
-      </c>
-      <c r="AA33">
-        <v>65535</v>
+        <v>1.5180712412366853E-2</v>
       </c>
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B34" t="s">
         <v>81</v>
@@ -2758,52 +2789,58 @@
       <c r="C34" t="s">
         <v>14</v>
       </c>
+      <c r="K34">
+        <v>0.22831050228310501</v>
+      </c>
+      <c r="L34">
+        <v>0.1906392694063927</v>
+      </c>
+      <c r="M34">
+        <v>0.18647260273972602</v>
+      </c>
       <c r="N34">
-        <v>3.8051750380517509E-2</v>
+        <v>6.7876712328767116E-2</v>
       </c>
       <c r="O34">
-        <v>7.6103500761035017E-2</v>
+        <v>7.476575935480044E-2</v>
       </c>
       <c r="P34">
-        <v>9.6783799880881469E-2</v>
+        <v>9.6412405035707568E-2</v>
       </c>
       <c r="Q34">
-        <v>0.1525728837372673</v>
+        <v>0.15293804193529958</v>
       </c>
       <c r="R34">
-        <v>0.13964622955180209</v>
+        <v>0.13941040865139273</v>
       </c>
       <c r="S34">
-        <v>0.15294587046149752</v>
+        <v>0.1534278778672068</v>
       </c>
       <c r="T34">
-        <v>0.1540541738706388</v>
+        <v>0.15383140488540142</v>
       </c>
       <c r="U34">
-        <v>0.15516247727978011</v>
+        <v>0.15538589047072227</v>
       </c>
       <c r="V34">
-        <v>0.14851265682493239</v>
+        <v>0.14838111835914639</v>
       </c>
       <c r="W34">
-        <v>0.15586582367404284</v>
+        <v>0.15491400651998427</v>
       </c>
       <c r="X34">
-        <v>0.15255292652552924</v>
+        <v>0.15239085998651261</v>
       </c>
       <c r="Y34">
-        <v>0.13213245604573401</v>
+        <v>0.13133926069138591</v>
       </c>
       <c r="Z34">
-        <v>0.13711751430220961</v>
-      </c>
-      <c r="AA34">
-        <v>0.13667567483614451</v>
+        <v>0.13764325363624622</v>
       </c>
     </row>
     <row r="35" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B35" t="s">
         <v>81</v>
@@ -2811,61 +2848,768 @@
       <c r="C35" t="s">
         <v>15</v>
       </c>
+      <c r="H35">
+        <v>0.11415525114155251</v>
+      </c>
       <c r="I35">
+        <v>6.5453767123287668E-2</v>
+      </c>
+      <c r="J35">
+        <v>8.4758159986470502E-2</v>
+      </c>
+      <c r="K35">
+        <v>0.17808980213089803</v>
+      </c>
+      <c r="L35">
+        <v>0.12192381639029079</v>
+      </c>
+      <c r="M35">
+        <v>8.1248714467892558E-2</v>
+      </c>
+      <c r="N35">
+        <v>0.15938903548169775</v>
+      </c>
+      <c r="O35">
+        <v>0.18169781142649755</v>
+      </c>
+      <c r="P35">
+        <v>0.2058669391554197</v>
+      </c>
+      <c r="Q35">
+        <v>0.22956604290766625</v>
+      </c>
+      <c r="R35">
+        <v>0.2172995015710637</v>
+      </c>
+      <c r="S35">
+        <v>0.23704950320418605</v>
+      </c>
+      <c r="T35">
+        <v>0.23271503321770831</v>
+      </c>
+      <c r="U35">
+        <v>0.24584659524473154</v>
+      </c>
+      <c r="V35">
+        <v>0.21529025081619735</v>
+      </c>
+      <c r="W35">
+        <v>0.21381996798613462</v>
+      </c>
+      <c r="X35">
+        <v>0.23992922634315969</v>
+      </c>
+      <c r="Y35">
+        <v>0.2323315222455867</v>
+      </c>
+      <c r="Z35">
+        <v>0.24297964087912982</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>2000</v>
+      </c>
+      <c r="E39">
+        <v>2001</v>
+      </c>
+      <c r="F39">
+        <v>2002</v>
+      </c>
+      <c r="G39">
+        <v>2003</v>
+      </c>
+      <c r="H39">
+        <v>2004</v>
+      </c>
+      <c r="I39">
+        <v>2005</v>
+      </c>
+      <c r="J39">
+        <v>2006</v>
+      </c>
+      <c r="K39">
+        <v>2007</v>
+      </c>
+      <c r="L39">
+        <v>2008</v>
+      </c>
+      <c r="M39">
+        <v>2009</v>
+      </c>
+      <c r="N39">
+        <v>2010</v>
+      </c>
+      <c r="O39">
+        <v>2011</v>
+      </c>
+      <c r="P39">
+        <v>2012</v>
+      </c>
+      <c r="Q39">
+        <v>2013</v>
+      </c>
+      <c r="R39">
+        <v>2014</v>
+      </c>
+      <c r="S39">
+        <v>2015</v>
+      </c>
+      <c r="T39">
+        <v>2016</v>
+      </c>
+      <c r="U39">
+        <v>2017</v>
+      </c>
+      <c r="V39">
+        <v>2018</v>
+      </c>
+      <c r="W39">
+        <v>2019</v>
+      </c>
+      <c r="X39">
+        <v>2020</v>
+      </c>
+      <c r="Y39">
+        <v>2021</v>
+      </c>
+      <c r="Z39">
+        <v>2022</v>
+      </c>
+      <c r="AA39">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>46</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
         <v>0</v>
       </c>
-      <c r="J35">
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+      <c r="I40">
+        <v>0</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40">
+        <v>0</v>
+      </c>
+      <c r="L40">
+        <v>0.22831050228310504</v>
+      </c>
+      <c r="M40">
+        <v>0.11415525114155252</v>
+      </c>
+      <c r="N40">
+        <v>0.45662100456621008</v>
+      </c>
+      <c r="O40">
+        <v>0.68493150684931503</v>
+      </c>
+      <c r="P40">
+        <v>0.7990867579908677</v>
+      </c>
+      <c r="Q40">
+        <v>0.41856925418569257</v>
+      </c>
+      <c r="R40">
+        <v>0.57077625570776258</v>
+      </c>
+      <c r="S40">
+        <v>0.61643835616438358</v>
+      </c>
+      <c r="T40">
+        <v>0.66590563165905636</v>
+      </c>
+      <c r="U40">
+        <v>0.91324200913242015</v>
+      </c>
+      <c r="V40">
+        <v>2.5603392041748205</v>
+      </c>
+      <c r="W40">
+        <v>3.4627092846270933</v>
+      </c>
+      <c r="X40">
+        <v>3.8812785388127851</v>
+      </c>
+      <c r="Y40">
+        <v>5.9132420091324196</v>
+      </c>
+      <c r="Z40">
+        <v>5.1141552511415531</v>
+      </c>
+      <c r="AA40">
+        <v>4.9771689497716896</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>0.34409073920603195</v>
+      </c>
+      <c r="E41">
+        <v>0.39609028421001313</v>
+      </c>
+      <c r="F41">
+        <v>0.34896569655015519</v>
+      </c>
+      <c r="G41">
+        <v>0.3908090804205463</v>
+      </c>
+      <c r="H41">
+        <v>0.3922789539227895</v>
+      </c>
+      <c r="I41">
+        <v>0.38314653383146535</v>
+      </c>
+      <c r="J41">
+        <v>0.396222498962225</v>
+      </c>
+      <c r="K41">
+        <v>0.46430053964300544</v>
+      </c>
+      <c r="L41">
+        <v>0.48111249481112495</v>
+      </c>
+      <c r="M41">
+        <v>0.42782873873654675</v>
+      </c>
+      <c r="N41">
+        <v>0.45844586648499153</v>
+      </c>
+      <c r="O41">
+        <v>0.49726171897578175</v>
+      </c>
+      <c r="P41">
+        <v>0.41309028379862439</v>
+      </c>
+      <c r="Q41">
+        <v>0.36227010141320837</v>
+      </c>
+      <c r="R41">
+        <v>0.41231328844516674</v>
+      </c>
+      <c r="S41">
+        <v>0.50828415182197206</v>
+      </c>
+      <c r="T41">
+        <v>0.4369935206742831</v>
+      </c>
+      <c r="U41">
+        <v>0.46734400271649285</v>
+      </c>
+      <c r="V41">
+        <v>0.41685655309224456</v>
+      </c>
+      <c r="W41">
+        <v>0.38424076705180099</v>
+      </c>
+      <c r="X41">
+        <v>0.30180771877150181</v>
+      </c>
+      <c r="Y41">
+        <v>0.38178341330902782</v>
+      </c>
+      <c r="Z41">
+        <v>0.48677943686388042</v>
+      </c>
+      <c r="AA41">
+        <v>0.25824553878597789</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>46</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42">
+        <v>0.19642930601834707</v>
+      </c>
+      <c r="E42">
+        <v>0.19642930601834707</v>
+      </c>
+      <c r="F42">
+        <v>0.1583775556378296</v>
+      </c>
+      <c r="G42">
+        <v>0.18100292072894811</v>
+      </c>
+      <c r="H42">
+        <v>0.15323542720802993</v>
+      </c>
+      <c r="I42">
+        <v>0.1779176436710683</v>
+      </c>
+      <c r="J42">
+        <v>0.22213994816734542</v>
+      </c>
+      <c r="K42">
+        <v>0.23228111971411552</v>
+      </c>
+      <c r="L42">
+        <v>0.23426642842962081</v>
+      </c>
+      <c r="M42">
+        <v>0.19456025411951558</v>
+      </c>
+      <c r="N42">
+        <v>0.19555290847726822</v>
+      </c>
+      <c r="O42">
+        <v>0.19786910197869106</v>
+      </c>
+      <c r="P42">
+        <v>0.22450532724505329</v>
+      </c>
+      <c r="Q42">
+        <v>0.2226027397260274</v>
+      </c>
+      <c r="R42">
+        <v>0.20357686453576868</v>
+      </c>
+      <c r="S42">
+        <v>0.17694063926940642</v>
+      </c>
+      <c r="T42">
+        <v>0.1950152207001522</v>
+      </c>
+      <c r="U42">
+        <v>0.18359969558599698</v>
+      </c>
+      <c r="V42">
+        <v>0.19216133942161343</v>
+      </c>
+      <c r="W42">
+        <v>0.20452815829528159</v>
+      </c>
+      <c r="X42">
+        <v>0.21784627092846273</v>
+      </c>
+      <c r="Y42">
+        <v>0.29014459665144599</v>
+      </c>
+      <c r="Z42">
+        <v>0.1950152207001522</v>
+      </c>
+      <c r="AA42">
+        <v>0.14840182648401828</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>46</v>
+      </c>
+      <c r="B43" t="s">
+        <v>81</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43">
+        <v>0.29434148088459128</v>
+      </c>
+      <c r="E43">
+        <v>0.22423352902804958</v>
+      </c>
+      <c r="F43">
+        <v>0.22408253001860307</v>
+      </c>
+      <c r="G43">
+        <v>0.20686315206863154</v>
+      </c>
+      <c r="H43">
+        <v>0.18103408514367419</v>
+      </c>
+      <c r="I43">
+        <v>0.24791291914579586</v>
+      </c>
+      <c r="J43">
+        <v>0.2427240440939071</v>
+      </c>
+      <c r="K43">
+        <v>0.16072605011472321</v>
+      </c>
+      <c r="L43">
+        <v>0.1502326182476092</v>
+      </c>
+      <c r="M43">
+        <v>0.18296846327828276</v>
+      </c>
+      <c r="N43">
+        <v>0.26339491433119683</v>
+      </c>
+      <c r="O43">
+        <v>0.14626141552511415</v>
+      </c>
+      <c r="P43">
+        <v>0.15647142182333496</v>
+      </c>
+      <c r="Q43">
+        <v>0.19708855325293684</v>
+      </c>
+      <c r="R43">
+        <v>0.22250599798777185</v>
+      </c>
+      <c r="S43">
+        <v>0.27329541057193724</v>
+      </c>
+      <c r="T43">
+        <v>0.18767897221577279</v>
+      </c>
+      <c r="U43">
+        <v>0.12870890865760704</v>
+      </c>
+      <c r="V43">
+        <v>0.23422292564900221</v>
+      </c>
+      <c r="W43">
+        <v>0.13325692663137406</v>
+      </c>
+      <c r="X43">
+        <v>0.12825410686023031</v>
+      </c>
+      <c r="Y43">
+        <v>0.21921446633557101</v>
+      </c>
+      <c r="Z43">
+        <v>0.17145847997545438</v>
+      </c>
+      <c r="AA43">
+        <v>0.14032522966412186</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" t="s">
+        <v>81</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44">
+        <v>0.58791571267802401</v>
+      </c>
+      <c r="E44">
+        <v>0.632219592016247</v>
+      </c>
+      <c r="F44">
+        <v>0.84860999194198217</v>
+      </c>
+      <c r="G44">
+        <v>0.72522159548751008</v>
+      </c>
+      <c r="H44">
+        <v>0.70591592801504166</v>
+      </c>
+      <c r="I44">
+        <v>0.78271890948160072</v>
+      </c>
+      <c r="J44">
+        <v>0.81797273704002138</v>
+      </c>
+      <c r="K44">
+        <v>0.88425019931869253</v>
+      </c>
+      <c r="L44">
+        <v>0.95250175158850958</v>
+      </c>
+      <c r="M44">
+        <v>0.92169795366142393</v>
+      </c>
+      <c r="N44">
+        <v>0.92109395762363799</v>
+      </c>
+      <c r="O44">
+        <v>0.98511753762895304</v>
+      </c>
+      <c r="P44">
+        <v>0.94312558272968505</v>
+      </c>
+      <c r="Q44">
+        <v>0.81695954983626218</v>
+      </c>
+      <c r="R44">
+        <v>0.91497163414971638</v>
+      </c>
+      <c r="S44">
+        <v>0.88672109220054429</v>
+      </c>
+      <c r="T44">
+        <v>0.91440094569223274</v>
+      </c>
+      <c r="U44">
+        <v>0.90107317525438657</v>
+      </c>
+      <c r="V44">
+        <v>0.91608169199663791</v>
+      </c>
+      <c r="W44">
+        <v>0.94050296462891025</v>
+      </c>
+      <c r="X44">
+        <v>0.9444785206388151</v>
+      </c>
+      <c r="Y44">
+        <v>0.93652740861900541</v>
+      </c>
+      <c r="Z44">
+        <v>0.93482359890047495</v>
+      </c>
+      <c r="AA44">
+        <v>0.91778550171516859</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>65535</v>
+      </c>
+      <c r="E45">
+        <v>65535</v>
+      </c>
+      <c r="F45">
+        <v>65535</v>
+      </c>
+      <c r="G45">
+        <v>65535</v>
+      </c>
+      <c r="H45">
+        <v>65535</v>
+      </c>
+      <c r="I45">
+        <v>65535</v>
+      </c>
+      <c r="J45">
+        <v>65535</v>
+      </c>
+      <c r="K45">
+        <v>65535</v>
+      </c>
+      <c r="L45">
+        <v>65535</v>
+      </c>
+      <c r="M45">
+        <v>65535</v>
+      </c>
+      <c r="N45">
+        <v>65535</v>
+      </c>
+      <c r="O45">
+        <v>65535</v>
+      </c>
+      <c r="P45">
+        <v>65535</v>
+      </c>
+      <c r="Q45">
+        <v>65535</v>
+      </c>
+      <c r="R45">
+        <v>65535</v>
+      </c>
+      <c r="S45">
+        <v>65535</v>
+      </c>
+      <c r="T45">
+        <v>65535</v>
+      </c>
+      <c r="U45">
+        <v>65535</v>
+      </c>
+      <c r="V45">
+        <v>65535</v>
+      </c>
+      <c r="W45">
+        <v>65535</v>
+      </c>
+      <c r="X45">
+        <v>65535</v>
+      </c>
+      <c r="Y45">
+        <v>65535</v>
+      </c>
+      <c r="Z45">
+        <v>65535</v>
+      </c>
+      <c r="AA45">
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" t="s">
+        <v>14</v>
+      </c>
+      <c r="N46">
+        <v>3.8051750380517509E-2</v>
+      </c>
+      <c r="O46">
         <v>7.6103500761035017E-2</v>
       </c>
-      <c r="K35">
+      <c r="P46">
+        <v>9.6783799880881469E-2</v>
+      </c>
+      <c r="Q46">
+        <v>0.1525728837372673</v>
+      </c>
+      <c r="R46">
+        <v>0.13964622955180209</v>
+      </c>
+      <c r="S46">
+        <v>0.15294587046149752</v>
+      </c>
+      <c r="T46">
+        <v>0.1540541738706388</v>
+      </c>
+      <c r="U46">
+        <v>0.15516247727978011</v>
+      </c>
+      <c r="V46">
+        <v>0.14851265682493239</v>
+      </c>
+      <c r="W46">
+        <v>0.15586582367404284</v>
+      </c>
+      <c r="X46">
+        <v>0.15255292652552924</v>
+      </c>
+      <c r="Y46">
+        <v>0.13213245604573401</v>
+      </c>
+      <c r="Z46">
+        <v>0.13711751430220961</v>
+      </c>
+      <c r="AA46">
+        <v>0.13667567483614451</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>7.6103500761035017E-2</v>
+      </c>
+      <c r="K47">
         <v>0.19025875190258754</v>
       </c>
-      <c r="L35">
+      <c r="L47">
         <v>0.12453300124533001</v>
       </c>
-      <c r="M35">
+      <c r="M47">
         <v>8.3022000830220002E-2</v>
       </c>
-      <c r="N35">
+      <c r="N47">
         <v>0.15841953219644023</v>
       </c>
-      <c r="O35">
+      <c r="O47">
         <v>0.18180280737358362</v>
       </c>
-      <c r="P35">
+      <c r="P47">
         <v>0.20480795057749127</v>
       </c>
-      <c r="Q35">
+      <c r="Q47">
         <v>0.22998925597636316</v>
       </c>
-      <c r="R35">
+      <c r="R47">
         <v>0.21689497716894979</v>
       </c>
-      <c r="S35">
+      <c r="S47">
         <v>0.23646444879321593</v>
       </c>
-      <c r="T35">
+      <c r="T47">
         <v>0.23157208088714937</v>
       </c>
-      <c r="U35">
+      <c r="U47">
         <v>0.24461839530332682</v>
       </c>
-      <c r="V35">
+      <c r="V47">
         <v>0.21526418786692761</v>
       </c>
-      <c r="W35">
+      <c r="W47">
         <v>0.21526418786692761</v>
       </c>
-      <c r="X35">
+      <c r="X47">
         <v>0.24135681669928247</v>
       </c>
-      <c r="Y35">
+      <c r="Y47">
         <v>0.23320287018917157</v>
       </c>
-      <c r="Z35">
+      <c r="Z47">
         <v>0.23483365949119375</v>
       </c>
-      <c r="AA35">
+      <c r="AA47">
         <v>0.25277234181343772</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 06:25
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8484D292-961E-4364-900A-BD7985E31203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90376F09-7BA1-4ED3-B5E8-8ECE594A46C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="88">
   <si>
     <t>bioenergy</t>
   </si>
@@ -339,6 +339,12 @@
   </si>
   <si>
     <t>Import</t>
+  </si>
+  <si>
+    <t>EMBER Capacity (GW)</t>
+  </si>
+  <si>
+    <t>EMBER Generation (TWh)</t>
   </si>
 </sst>
 </file>
@@ -1263,7 +1269,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:AA47"/>
+  <dimension ref="A1:Z59"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="U26" sqref="U26"/>
@@ -1750,7 +1756,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1827,7 +1833,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1904,7 +1910,7 @@
         <v>4.9771689497716896</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -1981,7 +1987,7 @@
         <v>0.25824553878597789</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2058,7 +2064,7 @@
         <v>0.14840182648401828</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -2135,7 +2141,7 @@
         <v>0.14032522966412186</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>13</v>
       </c>
@@ -2212,7 +2218,7 @@
         <v>0.91778550171516859</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>3</v>
       </c>
@@ -2289,7 +2295,7 @@
         <v>65535</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>14</v>
       </c>
@@ -2336,7 +2342,7 @@
         <v>0.13667567483614451</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>15</v>
       </c>
@@ -2398,1219 +2404,1908 @@
         <v>0.25277234181343772</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>2000</v>
+      </c>
+      <c r="C29">
+        <v>2001</v>
+      </c>
+      <c r="D29">
+        <v>2002</v>
+      </c>
+      <c r="E29">
+        <v>2003</v>
+      </c>
+      <c r="F29">
+        <v>2004</v>
+      </c>
+      <c r="G29">
+        <v>2005</v>
+      </c>
+      <c r="H29">
+        <v>2006</v>
+      </c>
+      <c r="I29">
+        <v>2007</v>
+      </c>
+      <c r="J29">
+        <v>2008</v>
+      </c>
+      <c r="K29">
+        <v>2009</v>
+      </c>
+      <c r="L29">
+        <v>2010</v>
+      </c>
+      <c r="M29">
+        <v>2011</v>
+      </c>
+      <c r="N29">
+        <v>2012</v>
+      </c>
+      <c r="O29">
+        <v>2013</v>
+      </c>
+      <c r="P29">
+        <v>2014</v>
+      </c>
+      <c r="Q29">
+        <v>2015</v>
+      </c>
+      <c r="R29">
+        <v>2016</v>
+      </c>
+      <c r="S29">
+        <v>2017</v>
+      </c>
+      <c r="T29">
+        <v>2018</v>
+      </c>
+      <c r="U29">
+        <v>2019</v>
+      </c>
+      <c r="V29">
+        <v>2020</v>
+      </c>
+      <c r="W29">
+        <v>2021</v>
+      </c>
+      <c r="X29">
+        <v>2022</v>
+      </c>
+      <c r="Y29">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>0.05</v>
+      </c>
+      <c r="C30">
+        <v>0.05</v>
+      </c>
+      <c r="D30">
+        <v>0.05</v>
+      </c>
+      <c r="E30">
+        <v>0.01</v>
+      </c>
+      <c r="F30">
+        <v>0.01</v>
+      </c>
+      <c r="G30">
+        <v>0.01</v>
+      </c>
+      <c r="H30">
+        <v>0.01</v>
+      </c>
+      <c r="I30">
+        <v>0.01</v>
+      </c>
+      <c r="J30">
+        <v>0.01</v>
+      </c>
+      <c r="K30">
+        <v>0.01</v>
+      </c>
+      <c r="L30">
+        <v>0.01</v>
+      </c>
+      <c r="M30">
+        <v>0.01</v>
+      </c>
+      <c r="N30">
+        <v>0.01</v>
+      </c>
+      <c r="O30">
+        <v>0.03</v>
+      </c>
+      <c r="P30">
+        <v>0.04</v>
+      </c>
+      <c r="Q30">
+        <v>0.05</v>
+      </c>
+      <c r="R30">
+        <v>0.06</v>
+      </c>
+      <c r="S30">
+        <v>0.05</v>
+      </c>
+      <c r="T30">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="U30">
+        <v>0.06</v>
+      </c>
+      <c r="V30">
+        <v>0.05</v>
+      </c>
+      <c r="W30">
+        <v>0.05</v>
+      </c>
+      <c r="X30">
+        <v>0.05</v>
+      </c>
+      <c r="Y30">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>5.62</v>
+      </c>
+      <c r="C31">
+        <v>5.62</v>
+      </c>
+      <c r="D31">
+        <v>5.62</v>
+      </c>
+      <c r="E31">
+        <v>5.62</v>
+      </c>
+      <c r="F31">
+        <v>5.5</v>
+      </c>
+      <c r="G31">
+        <v>5.5</v>
+      </c>
+      <c r="H31">
+        <v>5.5</v>
+      </c>
+      <c r="I31">
+        <v>5.5</v>
+      </c>
+      <c r="J31">
+        <v>5.5</v>
+      </c>
+      <c r="K31">
+        <v>5.63</v>
+      </c>
+      <c r="L31">
+        <v>5.63</v>
+      </c>
+      <c r="M31">
+        <v>6.32</v>
+      </c>
+      <c r="N31">
+        <v>6.32</v>
+      </c>
+      <c r="O31">
+        <v>6.11</v>
+      </c>
+      <c r="P31">
+        <v>5.9</v>
+      </c>
+      <c r="Q31">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="R31">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="S31">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="T31">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="U31">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="V31">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="W31">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="X31">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="Y31">
+        <v>5.1100000000000003</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>2</v>
+      </c>
+      <c r="B32">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C32">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D32">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E32">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F32">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G32">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="H32">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I32">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J32">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K32">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L32">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="M32">
+        <v>1.2</v>
+      </c>
+      <c r="N32">
+        <v>1.2</v>
+      </c>
+      <c r="O32">
+        <v>1.2</v>
+      </c>
+      <c r="P32">
+        <v>1.2</v>
+      </c>
+      <c r="Q32">
+        <v>1.2</v>
+      </c>
+      <c r="R32">
+        <v>1.2</v>
+      </c>
+      <c r="S32">
+        <v>1.2</v>
+      </c>
+      <c r="T32">
+        <v>1.2</v>
+      </c>
+      <c r="U32">
+        <v>1.2</v>
+      </c>
+      <c r="V32">
+        <v>1.2</v>
+      </c>
+      <c r="W32">
+        <v>1.2</v>
+      </c>
+      <c r="X32">
+        <v>1.2</v>
+      </c>
+      <c r="Y32">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>12</v>
+      </c>
+      <c r="B33">
+        <v>1.02</v>
+      </c>
+      <c r="C33">
+        <v>0.84</v>
+      </c>
+      <c r="D33">
+        <v>1.08</v>
+      </c>
+      <c r="E33">
+        <v>1.65</v>
+      </c>
+      <c r="F33">
+        <v>1.98</v>
+      </c>
+      <c r="G33">
+        <v>1.98</v>
+      </c>
+      <c r="H33">
+        <v>1.98</v>
+      </c>
+      <c r="I33">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="J33">
+        <v>2.12</v>
+      </c>
+      <c r="K33">
+        <v>2.14</v>
+      </c>
+      <c r="L33">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="M33">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="N33">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="O33">
+        <v>2.34</v>
+      </c>
+      <c r="P33">
+        <v>2.36</v>
+      </c>
+      <c r="Q33">
+        <v>2.36</v>
+      </c>
+      <c r="R33">
+        <v>2.36</v>
+      </c>
+      <c r="S33">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="T33">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="U33">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="V33">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="W33">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="X33">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="Y33">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34">
+        <v>3.53</v>
+      </c>
+      <c r="C34">
+        <v>3.53</v>
+      </c>
+      <c r="D34">
+        <v>2.72</v>
+      </c>
+      <c r="E34">
+        <v>2.72</v>
+      </c>
+      <c r="F34">
+        <v>2.72</v>
+      </c>
+      <c r="G34">
+        <v>2.72</v>
+      </c>
+      <c r="H34">
+        <v>2.72</v>
+      </c>
+      <c r="I34">
+        <v>1.89</v>
+      </c>
+      <c r="J34">
+        <v>1.89</v>
+      </c>
+      <c r="K34">
+        <v>1.89</v>
+      </c>
+      <c r="L34">
+        <v>1.89</v>
+      </c>
+      <c r="M34">
+        <v>1.89</v>
+      </c>
+      <c r="N34">
+        <v>1.91</v>
+      </c>
+      <c r="O34">
+        <v>1.98</v>
+      </c>
+      <c r="P34">
+        <v>1.98</v>
+      </c>
+      <c r="Q34">
+        <v>1.98</v>
+      </c>
+      <c r="R34">
+        <v>1.97</v>
+      </c>
+      <c r="S34">
+        <v>1.97</v>
+      </c>
+      <c r="T34">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="U34">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="V34">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="W34">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="X34">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="Y34">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B35">
+        <v>0</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
+      </c>
+      <c r="J35">
+        <v>0</v>
+      </c>
+      <c r="K35">
+        <v>0</v>
+      </c>
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>0</v>
+      </c>
+      <c r="O35">
+        <v>0</v>
+      </c>
+      <c r="P35">
+        <v>0</v>
+      </c>
+      <c r="Q35">
+        <v>0</v>
+      </c>
+      <c r="R35">
+        <v>0</v>
+      </c>
+      <c r="S35">
+        <v>0</v>
+      </c>
+      <c r="T35">
+        <v>0</v>
+      </c>
+      <c r="U35">
+        <v>0</v>
+      </c>
+      <c r="V35">
+        <v>0</v>
+      </c>
+      <c r="W35">
+        <v>0</v>
+      </c>
+      <c r="X35">
+        <v>0</v>
+      </c>
+      <c r="Y35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <v>0</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36">
+        <v>0</v>
+      </c>
+      <c r="L36">
+        <v>0.03</v>
+      </c>
+      <c r="M36">
+        <v>0.15</v>
+      </c>
+      <c r="N36">
+        <v>0.92</v>
+      </c>
+      <c r="O36">
+        <v>1.04</v>
+      </c>
+      <c r="P36">
+        <v>1.03</v>
+      </c>
+      <c r="Q36">
+        <v>1.03</v>
+      </c>
+      <c r="R36">
+        <v>1.03</v>
+      </c>
+      <c r="S36">
+        <v>1.03</v>
+      </c>
+      <c r="T36">
+        <v>1.03</v>
+      </c>
+      <c r="U36">
+        <v>1.04</v>
+      </c>
+      <c r="V36">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W36">
+        <v>1.27</v>
+      </c>
+      <c r="X36">
+        <v>1.74</v>
+      </c>
+      <c r="Y36">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0.01</v>
+      </c>
+      <c r="H37">
+        <v>0.03</v>
+      </c>
+      <c r="I37">
+        <v>0.03</v>
+      </c>
+      <c r="J37">
+        <v>0.11</v>
+      </c>
+      <c r="K37">
+        <v>0.33</v>
+      </c>
+      <c r="L37">
+        <v>0.49</v>
+      </c>
+      <c r="M37">
+        <v>0.54</v>
+      </c>
+      <c r="N37">
+        <v>0.68</v>
+      </c>
+      <c r="O37">
+        <v>0.68</v>
+      </c>
+      <c r="P37">
+        <v>0.7</v>
+      </c>
+      <c r="Q37">
+        <v>0.7</v>
+      </c>
+      <c r="R37">
+        <v>0.7</v>
+      </c>
+      <c r="S37">
+        <v>0.7</v>
+      </c>
+      <c r="T37">
+        <v>0.7</v>
+      </c>
+      <c r="U37">
+        <v>0.7</v>
+      </c>
+      <c r="V37">
+        <v>0.7</v>
+      </c>
+      <c r="W37">
+        <v>0.7</v>
+      </c>
+      <c r="X37">
+        <v>0.7</v>
+      </c>
+      <c r="Y37">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>2000</v>
+      </c>
+      <c r="C41">
+        <v>2001</v>
+      </c>
+      <c r="D41">
+        <v>2002</v>
+      </c>
+      <c r="E41">
+        <v>2003</v>
+      </c>
+      <c r="F41">
+        <v>2004</v>
+      </c>
+      <c r="G41">
+        <v>2005</v>
+      </c>
+      <c r="H41">
+        <v>2006</v>
+      </c>
+      <c r="I41">
+        <v>2007</v>
+      </c>
+      <c r="J41">
+        <v>2008</v>
+      </c>
+      <c r="K41">
+        <v>2009</v>
+      </c>
+      <c r="L41">
+        <v>2010</v>
+      </c>
+      <c r="M41">
+        <v>2011</v>
+      </c>
+      <c r="N41">
+        <v>2012</v>
+      </c>
+      <c r="O41">
+        <v>2013</v>
+      </c>
+      <c r="P41">
+        <v>2014</v>
+      </c>
+      <c r="Q41">
+        <v>2015</v>
+      </c>
+      <c r="R41">
+        <v>2016</v>
+      </c>
+      <c r="S41">
+        <v>2017</v>
+      </c>
+      <c r="T41">
+        <v>2018</v>
+      </c>
+      <c r="U41">
+        <v>2019</v>
+      </c>
+      <c r="V41">
+        <v>2020</v>
+      </c>
+      <c r="W41">
+        <v>2021</v>
+      </c>
+      <c r="X41">
+        <v>2022</v>
+      </c>
+      <c r="Y41">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>0</v>
+      </c>
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+      <c r="I42">
+        <v>0</v>
+      </c>
+      <c r="J42">
+        <v>0.02</v>
+      </c>
+      <c r="K42">
+        <v>0.01</v>
+      </c>
+      <c r="L42">
+        <v>0.04</v>
+      </c>
+      <c r="M42">
+        <v>0.06</v>
+      </c>
+      <c r="N42">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="O42">
+        <v>0.11</v>
+      </c>
+      <c r="P42">
+        <v>0.2</v>
+      </c>
+      <c r="Q42">
+        <v>0.27</v>
+      </c>
+      <c r="R42">
+        <v>0.35</v>
+      </c>
+      <c r="S42">
+        <v>0.4</v>
+      </c>
+      <c r="T42">
+        <v>1.57</v>
+      </c>
+      <c r="U42">
+        <v>1.82</v>
+      </c>
+      <c r="V42">
+        <v>1.7</v>
+      </c>
+      <c r="W42">
+        <v>2.59</v>
+      </c>
+      <c r="X42">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="Y42">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>16.940000000000001</v>
+      </c>
+      <c r="C43">
+        <v>19.5</v>
+      </c>
+      <c r="D43">
+        <v>17.18</v>
+      </c>
+      <c r="E43">
+        <v>19.239999999999998</v>
+      </c>
+      <c r="F43">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="G43">
+        <v>18.46</v>
+      </c>
+      <c r="H43">
+        <v>19.09</v>
+      </c>
+      <c r="I43">
+        <v>22.37</v>
+      </c>
+      <c r="J43">
+        <v>23.18</v>
+      </c>
+      <c r="K43">
+        <v>21.1</v>
+      </c>
+      <c r="L43">
+        <v>22.61</v>
+      </c>
+      <c r="M43">
+        <v>27.53</v>
+      </c>
+      <c r="N43">
+        <v>22.87</v>
+      </c>
+      <c r="O43">
+        <v>19.39</v>
+      </c>
+      <c r="P43">
+        <v>21.31</v>
+      </c>
+      <c r="Q43">
+        <v>22.53</v>
+      </c>
+      <c r="R43">
+        <v>19.37</v>
+      </c>
+      <c r="S43">
+        <v>20.92</v>
+      </c>
+      <c r="T43">
+        <v>18.66</v>
+      </c>
+      <c r="U43">
+        <v>17.2</v>
+      </c>
+      <c r="V43">
+        <v>13.51</v>
+      </c>
+      <c r="W43">
+        <v>17.09</v>
+      </c>
+      <c r="X43">
+        <v>21.79</v>
+      </c>
+      <c r="Y43">
+        <v>11.56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44">
+        <v>1.91</v>
+      </c>
+      <c r="C44">
+        <v>1.91</v>
+      </c>
+      <c r="D44">
+        <v>1.54</v>
+      </c>
+      <c r="E44">
+        <v>1.76</v>
+      </c>
+      <c r="F44">
+        <v>1.49</v>
+      </c>
+      <c r="G44">
+        <v>1.73</v>
+      </c>
+      <c r="H44">
+        <v>2.16</v>
+      </c>
+      <c r="I44">
+        <v>2.34</v>
+      </c>
+      <c r="J44">
+        <v>2.36</v>
+      </c>
+      <c r="K44">
+        <v>1.96</v>
+      </c>
+      <c r="L44">
+        <v>1.97</v>
+      </c>
+      <c r="M44">
+        <v>2.08</v>
+      </c>
+      <c r="N44">
+        <v>2.36</v>
+      </c>
+      <c r="O44">
+        <v>2.34</v>
+      </c>
+      <c r="P44">
+        <v>2.14</v>
+      </c>
+      <c r="Q44">
+        <v>1.86</v>
+      </c>
+      <c r="R44">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="S44">
+        <v>1.93</v>
+      </c>
+      <c r="T44">
+        <v>2.02</v>
+      </c>
+      <c r="U44">
+        <v>2.15</v>
+      </c>
+      <c r="V44">
+        <v>2.29</v>
+      </c>
+      <c r="W44">
+        <v>3.05</v>
+      </c>
+      <c r="X44">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="Y44">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45">
+        <v>2.63</v>
+      </c>
+      <c r="C45">
+        <v>1.65</v>
+      </c>
+      <c r="D45">
+        <v>2.12</v>
+      </c>
+      <c r="E45">
+        <v>2.99</v>
+      </c>
+      <c r="F45">
+        <v>3.14</v>
+      </c>
+      <c r="G45">
+        <v>4.3</v>
+      </c>
+      <c r="H45">
+        <v>4.21</v>
+      </c>
+      <c r="I45">
+        <v>2.83</v>
+      </c>
+      <c r="J45">
+        <v>2.79</v>
+      </c>
+      <c r="K45">
+        <v>3.43</v>
+      </c>
+      <c r="L45">
+        <v>5.03</v>
+      </c>
+      <c r="M45">
+        <v>2.87</v>
+      </c>
+      <c r="N45">
+        <v>3.18</v>
+      </c>
+      <c r="O45">
+        <v>4.04</v>
+      </c>
+      <c r="P45">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Q45">
+        <v>5.65</v>
+      </c>
+      <c r="R45">
+        <v>3.88</v>
+      </c>
+      <c r="S45">
+        <v>2.83</v>
+      </c>
+      <c r="T45">
+        <v>5.15</v>
+      </c>
+      <c r="U45">
+        <v>2.93</v>
+      </c>
+      <c r="V45">
+        <v>2.82</v>
+      </c>
+      <c r="W45">
+        <v>4.82</v>
+      </c>
+      <c r="X45">
+        <v>3.8</v>
+      </c>
+      <c r="Y45">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="46" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <v>18.18</v>
+      </c>
+      <c r="C46">
+        <v>19.55</v>
+      </c>
+      <c r="D46">
+        <v>20.22</v>
+      </c>
+      <c r="E46">
+        <v>17.28</v>
+      </c>
+      <c r="F46">
+        <v>16.82</v>
+      </c>
+      <c r="G46">
+        <v>18.649999999999999</v>
+      </c>
+      <c r="H46">
+        <v>19.489999999999998</v>
+      </c>
+      <c r="I46">
+        <v>14.64</v>
+      </c>
+      <c r="J46">
+        <v>15.77</v>
+      </c>
+      <c r="K46">
+        <v>15.26</v>
+      </c>
+      <c r="L46">
+        <v>15.25</v>
+      </c>
+      <c r="M46">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="N46">
+        <v>15.78</v>
+      </c>
+      <c r="O46">
+        <v>14.17</v>
+      </c>
+      <c r="P46">
+        <v>15.87</v>
+      </c>
+      <c r="Q46">
+        <v>15.38</v>
+      </c>
+      <c r="R46">
+        <v>15.78</v>
+      </c>
+      <c r="S46">
+        <v>15.55</v>
+      </c>
+      <c r="T46">
+        <v>16.13</v>
+      </c>
+      <c r="U46">
+        <v>16.559999999999999</v>
+      </c>
+      <c r="V46">
+        <v>16.63</v>
+      </c>
+      <c r="W46">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="X46">
+        <v>16.46</v>
+      </c>
+      <c r="Y46">
+        <v>16.16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>3</v>
+      </c>
+      <c r="B47">
+        <v>0.93</v>
+      </c>
+      <c r="C47">
+        <v>0.83</v>
+      </c>
+      <c r="D47">
+        <v>1.02</v>
+      </c>
+      <c r="E47">
+        <v>1.01</v>
+      </c>
+      <c r="F47">
+        <v>1.01</v>
+      </c>
+      <c r="G47">
+        <v>0.75</v>
+      </c>
+      <c r="H47">
+        <v>0.47</v>
+      </c>
+      <c r="I47">
+        <v>0.59</v>
+      </c>
+      <c r="J47">
+        <v>0.25</v>
+      </c>
+      <c r="K47">
+        <v>0.31</v>
+      </c>
+      <c r="L47">
+        <v>0.34</v>
+      </c>
+      <c r="M47">
+        <v>0.15</v>
+      </c>
+      <c r="N47">
+        <v>0.2</v>
+      </c>
+      <c r="O47">
+        <v>0.21</v>
+      </c>
+      <c r="P47">
+        <v>0.21</v>
+      </c>
+      <c r="Q47">
+        <v>0.19</v>
+      </c>
+      <c r="R47">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S47">
+        <v>0.31</v>
+      </c>
+      <c r="T47">
+        <v>0.32</v>
+      </c>
+      <c r="U47">
+        <v>0.32</v>
+      </c>
+      <c r="V47">
+        <v>0.24</v>
+      </c>
+      <c r="W47">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X47">
+        <v>0.35</v>
+      </c>
+      <c r="Y47">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48">
+        <v>0</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0.01</v>
+      </c>
+      <c r="M48">
+        <v>0.1</v>
+      </c>
+      <c r="N48">
+        <v>0.78</v>
+      </c>
+      <c r="O48">
+        <v>1.39</v>
+      </c>
+      <c r="P48">
+        <v>1.26</v>
+      </c>
+      <c r="Q48">
+        <v>1.38</v>
+      </c>
+      <c r="R48">
+        <v>1.39</v>
+      </c>
+      <c r="S48">
+        <v>1.4</v>
+      </c>
+      <c r="T48">
+        <v>1.34</v>
+      </c>
+      <c r="U48">
+        <v>1.42</v>
+      </c>
+      <c r="V48">
+        <v>1.47</v>
+      </c>
+      <c r="W48">
+        <v>1.47</v>
+      </c>
+      <c r="X48">
+        <v>2.09</v>
+      </c>
+      <c r="Y48">
+        <v>3.52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0.02</v>
+      </c>
+      <c r="I49">
+        <v>0.05</v>
+      </c>
+      <c r="J49">
+        <v>0.12</v>
+      </c>
+      <c r="K49">
+        <v>0.24</v>
+      </c>
+      <c r="L49">
+        <v>0.68</v>
+      </c>
+      <c r="M49">
+        <v>0.86</v>
+      </c>
+      <c r="N49">
+        <v>1.22</v>
+      </c>
+      <c r="O49">
+        <v>1.37</v>
+      </c>
+      <c r="P49">
+        <v>1.33</v>
+      </c>
+      <c r="Q49">
+        <v>1.45</v>
+      </c>
+      <c r="R49">
+        <v>1.42</v>
+      </c>
+      <c r="S49">
+        <v>1.5</v>
+      </c>
+      <c r="T49">
+        <v>1.32</v>
+      </c>
+      <c r="U49">
+        <v>1.32</v>
+      </c>
+      <c r="V49">
+        <v>1.48</v>
+      </c>
+      <c r="W49">
+        <v>1.43</v>
+      </c>
+      <c r="X49">
+        <v>1.44</v>
+      </c>
+      <c r="Y49">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A52" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A53" t="s">
         <v>43</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B53" t="s">
         <v>4</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C53" t="s">
         <v>5</v>
       </c>
-      <c r="D29">
+      <c r="D53">
         <v>2000</v>
       </c>
-      <c r="E29">
+      <c r="E53">
         <v>2001</v>
       </c>
-      <c r="F29">
+      <c r="F53">
         <v>2002</v>
       </c>
-      <c r="G29">
+      <c r="G53">
         <v>2003</v>
       </c>
-      <c r="H29">
+      <c r="H53">
         <v>2004</v>
       </c>
-      <c r="I29">
+      <c r="I53">
         <v>2005</v>
       </c>
-      <c r="J29">
+      <c r="J53">
         <v>2006</v>
       </c>
-      <c r="K29">
+      <c r="K53">
         <v>2007</v>
       </c>
-      <c r="L29">
+      <c r="L53">
         <v>2008</v>
       </c>
-      <c r="M29">
+      <c r="M53">
         <v>2009</v>
       </c>
-      <c r="N29">
+      <c r="N53">
         <v>2010</v>
       </c>
-      <c r="O29">
+      <c r="O53">
         <v>2011</v>
       </c>
-      <c r="P29">
+      <c r="P53">
         <v>2012</v>
       </c>
-      <c r="Q29">
+      <c r="Q53">
         <v>2013</v>
       </c>
-      <c r="R29">
+      <c r="R53">
         <v>2014</v>
       </c>
-      <c r="S29">
+      <c r="S53">
         <v>2015</v>
       </c>
-      <c r="T29">
+      <c r="T53">
         <v>2016</v>
       </c>
-      <c r="U29">
+      <c r="U53">
         <v>2017</v>
       </c>
-      <c r="V29">
+      <c r="V53">
         <v>2018</v>
       </c>
-      <c r="W29">
+      <c r="W53">
         <v>2019</v>
       </c>
-      <c r="X29">
+      <c r="X53">
         <v>2020</v>
       </c>
-      <c r="Y29">
+      <c r="Y53">
         <v>2021</v>
       </c>
-      <c r="Z29">
+      <c r="Z53">
         <v>2022</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>44</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B54" t="s">
         <v>81</v>
       </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
-      <c r="L30">
+      <c r="C54" t="s">
+        <v>0</v>
+      </c>
+      <c r="L54">
         <v>0.30441400304414001</v>
       </c>
-      <c r="M30">
+      <c r="M54">
         <v>0.10147133434804669</v>
       </c>
-      <c r="N30">
+      <c r="N54">
         <v>0.40447488584474894</v>
       </c>
-      <c r="O30">
+      <c r="O54">
         <v>0.5811540058115402</v>
       </c>
-      <c r="P30">
+      <c r="P54">
         <v>0.53816046966731901</v>
       </c>
-      <c r="Q30">
+      <c r="Q54">
         <v>0.37067553048616708</v>
       </c>
-      <c r="R30">
+      <c r="R54">
         <v>0.57077625570776258</v>
       </c>
-      <c r="S30">
+      <c r="S54">
         <v>0.57500422797226458</v>
       </c>
-      <c r="T30">
+      <c r="T54">
         <v>0.70696146759593048</v>
       </c>
-      <c r="U30">
+      <c r="U54">
         <v>0.86924428402751963</v>
       </c>
-      <c r="V30">
+      <c r="V54">
         <v>2.5863099724480505</v>
       </c>
-      <c r="W30">
+      <c r="W54">
         <v>3.6549813955986812</v>
       </c>
-      <c r="X30">
+      <c r="X54">
         <v>4.036889720525596</v>
       </c>
-      <c r="Y30">
+      <c r="Y54">
         <v>6.2453375126974553</v>
       </c>
-      <c r="Z30">
+      <c r="Z54">
         <v>3.2548137163984849</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>44</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B55" t="s">
         <v>81</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C55" t="s">
         <v>12</v>
       </c>
-      <c r="D31">
+      <c r="D55">
         <v>0.17918731176527739</v>
       </c>
-      <c r="E31">
+      <c r="E55">
         <v>0.14535545467936098</v>
       </c>
-      <c r="F31">
+      <c r="F55">
         <v>0.15845780240593327</v>
       </c>
-      <c r="G31">
+      <c r="G55">
         <v>0.1498316039834055</v>
       </c>
-      <c r="H31">
+      <c r="H55">
         <v>0.1347902156764661</v>
       </c>
-      <c r="I31">
+      <c r="I55">
         <v>0.18958653994151151</v>
       </c>
-      <c r="J31">
+      <c r="J55">
         <v>0.18353719344825822</v>
       </c>
-      <c r="K31">
+      <c r="K55">
         <v>0.12836507928947488</v>
       </c>
-      <c r="L31">
+      <c r="L55">
         <v>0.12535509016122517</v>
       </c>
-      <c r="M31">
+      <c r="M55">
         <v>0.15416139825537606</v>
       </c>
-      <c r="N31">
+      <c r="N55">
         <v>0.21319901365069094</v>
       </c>
-      <c r="O31">
+      <c r="O55">
         <v>0.13556538436675425</v>
       </c>
-      <c r="P31">
+      <c r="P55">
         <v>0.1426745416205524</v>
       </c>
-      <c r="Q31">
+      <c r="Q55">
         <v>0.17089921406444017</v>
       </c>
-      <c r="R31">
+      <c r="R55">
         <v>0.18308207829936693</v>
       </c>
-      <c r="S31">
+      <c r="S55">
         <v>0.21797454043557021</v>
       </c>
-      <c r="T31">
+      <c r="T55">
         <v>0.16178813238750592</v>
       </c>
-      <c r="U31">
+      <c r="U55">
         <v>0.11826549026371555</v>
       </c>
-      <c r="V31">
+      <c r="V55">
         <v>0.18320015783762453</v>
       </c>
-      <c r="W31">
+      <c r="W55">
         <v>0.11430375923833559</v>
       </c>
-      <c r="X31">
+      <c r="X55">
         <v>0.11225524213694742</v>
       </c>
-      <c r="Y31">
+      <c r="Y55">
         <v>0.1716829439171017</v>
       </c>
-      <c r="Z31">
+      <c r="Z55">
         <v>0.13069358514235713</v>
       </c>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>44</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B56" t="s">
         <v>81</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C56" t="s">
         <v>13</v>
       </c>
-      <c r="D32">
+      <c r="D56">
         <v>0.58751816400088952</v>
       </c>
-      <c r="E32">
+      <c r="E56">
         <v>0.63195855763612019</v>
       </c>
-      <c r="F32">
+      <c r="F56">
         <v>0.84807034848805107</v>
       </c>
-      <c r="G32">
+      <c r="G56">
         <v>0.72468873612271401</v>
       </c>
-      <c r="H32">
+      <c r="H56">
         <v>0.70518756353607848</v>
       </c>
-      <c r="I32">
+      <c r="I56">
         <v>0.78226961776024206</v>
       </c>
-      <c r="J32">
+      <c r="J56">
         <v>0.81749754243287398</v>
       </c>
-      <c r="K32">
+      <c r="K56">
         <v>0.88349648121868596</v>
       </c>
-      <c r="L32">
+      <c r="L56">
         <v>0.95119319991890894</v>
       </c>
-      <c r="M32">
+      <c r="M56">
         <v>0.92048229990249752</v>
       </c>
-      <c r="N32">
+      <c r="N56">
         <v>0.92005994960757642</v>
       </c>
-      <c r="O32">
+      <c r="O56">
         <v>0.98431753019201262</v>
       </c>
-      <c r="P32">
+      <c r="P56">
         <v>0.94540432280661413</v>
       </c>
-      <c r="Q32">
+      <c r="Q56">
         <v>0.81619276686525755</v>
       </c>
-      <c r="R32">
+      <c r="R56">
         <v>0.91711461765215874</v>
       </c>
-      <c r="S32">
+      <c r="S56">
         <v>0.88913935610658323</v>
       </c>
-      <c r="T32">
+      <c r="T56">
         <v>0.91556341739152636</v>
       </c>
-      <c r="U32">
+      <c r="U56">
         <v>0.90218624426321981</v>
       </c>
-      <c r="V32">
+      <c r="V56">
         <v>0.91672584775055033</v>
       </c>
-      <c r="W32">
+      <c r="W56">
         <v>0.942110199083116</v>
       </c>
-      <c r="X32">
+      <c r="X56">
         <v>0.94612082701666678</v>
       </c>
-      <c r="Y32">
+      <c r="Y56">
         <v>0.9382181082323805</v>
       </c>
-      <c r="Z32">
+      <c r="Z56">
         <v>0.93680249206717758</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
         <v>44</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B57" t="s">
         <v>81</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C57" t="s">
         <v>3</v>
       </c>
-      <c r="D33">
+      <c r="D57">
         <v>1.3728687025740881E-2</v>
       </c>
-      <c r="E33">
+      <c r="E57">
         <v>8.9246408872480296E-3</v>
       </c>
-      <c r="F33">
+      <c r="F57">
         <v>1.4064542368890371E-2</v>
       </c>
-      <c r="G33">
+      <c r="G57">
         <v>1.3440969291696423E-2</v>
       </c>
-      <c r="H33">
+      <c r="H57">
         <v>1.4367639360976603E-2</v>
       </c>
-      <c r="I33">
+      <c r="I57">
         <v>1.06544901065449E-2</v>
       </c>
-      <c r="J33">
+      <c r="J57">
         <v>6.8721033906174785E-3</v>
       </c>
-      <c r="K33">
+      <c r="K57">
         <v>1.3383397499030053E-2</v>
       </c>
-      <c r="L33">
+      <c r="L57">
         <v>6.8134032678754683E-3</v>
       </c>
-      <c r="M33">
+      <c r="M57">
         <v>8.974387151398696E-3</v>
       </c>
-      <c r="N33">
+      <c r="N57">
         <v>1.0171012962918537E-2</v>
       </c>
-      <c r="O33">
+      <c r="O57">
         <v>4.0275281549390085E-3</v>
       </c>
-      <c r="P33">
+      <c r="P57">
         <v>5.4770281784942507E-3</v>
       </c>
-      <c r="Q33">
+      <c r="Q57">
         <v>5.9193423561722108E-3</v>
       </c>
-      <c r="R33">
+      <c r="R57">
         <v>5.7979529360833674E-3</v>
       </c>
-      <c r="S33">
+      <c r="S57">
         <v>5.9440758150922698E-3</v>
       </c>
-      <c r="T33">
+      <c r="T57">
         <v>1.0672682178439969E-2</v>
       </c>
-      <c r="U33">
+      <c r="U57">
         <v>1.3166338195431674E-2</v>
       </c>
-      <c r="V33">
+      <c r="V57">
         <v>1.0273264456408587E-2</v>
       </c>
-      <c r="W33">
+      <c r="W57">
         <v>1.1459284473580975E-2</v>
       </c>
-      <c r="X33">
+      <c r="X57">
         <v>1.0273784895450284E-2</v>
       </c>
-      <c r="Y33">
+      <c r="Y57">
         <v>1.1799059936493149E-2</v>
       </c>
-      <c r="Z33">
+      <c r="Z57">
         <v>1.5180712412366853E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
         <v>44</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B58" t="s">
         <v>81</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C58" t="s">
         <v>14</v>
       </c>
-      <c r="K34">
+      <c r="K58">
         <v>0.22831050228310501</v>
       </c>
-      <c r="L34">
+      <c r="L58">
         <v>0.1906392694063927</v>
       </c>
-      <c r="M34">
+      <c r="M58">
         <v>0.18647260273972602</v>
       </c>
-      <c r="N34">
+      <c r="N58">
         <v>6.7876712328767116E-2</v>
       </c>
-      <c r="O34">
+      <c r="O58">
         <v>7.476575935480044E-2</v>
       </c>
-      <c r="P34">
+      <c r="P58">
         <v>9.6412405035707568E-2</v>
       </c>
-      <c r="Q34">
+      <c r="Q58">
         <v>0.15293804193529958</v>
       </c>
-      <c r="R34">
+      <c r="R58">
         <v>0.13941040865139273</v>
       </c>
-      <c r="S34">
+      <c r="S58">
         <v>0.1534278778672068</v>
       </c>
-      <c r="T34">
+      <c r="T58">
         <v>0.15383140488540142</v>
       </c>
-      <c r="U34">
+      <c r="U58">
         <v>0.15538589047072227</v>
       </c>
-      <c r="V34">
+      <c r="V58">
         <v>0.14838111835914639</v>
       </c>
-      <c r="W34">
+      <c r="W58">
         <v>0.15491400651998427</v>
       </c>
-      <c r="X34">
+      <c r="X58">
         <v>0.15239085998651261</v>
       </c>
-      <c r="Y34">
+      <c r="Y58">
         <v>0.13133926069138591</v>
       </c>
-      <c r="Z34">
+      <c r="Z58">
         <v>0.13764325363624622</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>44</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B59" t="s">
         <v>81</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C59" t="s">
         <v>15</v>
       </c>
-      <c r="H35">
+      <c r="H59">
         <v>0.11415525114155251</v>
       </c>
-      <c r="I35">
+      <c r="I59">
         <v>6.5453767123287668E-2</v>
       </c>
-      <c r="J35">
+      <c r="J59">
         <v>8.4758159986470502E-2</v>
       </c>
-      <c r="K35">
+      <c r="K59">
         <v>0.17808980213089803</v>
       </c>
-      <c r="L35">
+      <c r="L59">
         <v>0.12192381639029079</v>
       </c>
-      <c r="M35">
+      <c r="M59">
         <v>8.1248714467892558E-2</v>
       </c>
-      <c r="N35">
+      <c r="N59">
         <v>0.15938903548169775</v>
       </c>
-      <c r="O35">
+      <c r="O59">
         <v>0.18169781142649755</v>
       </c>
-      <c r="P35">
+      <c r="P59">
         <v>0.2058669391554197</v>
       </c>
-      <c r="Q35">
+      <c r="Q59">
         <v>0.22956604290766625</v>
       </c>
-      <c r="R35">
+      <c r="R59">
         <v>0.2172995015710637</v>
       </c>
-      <c r="S35">
+      <c r="S59">
         <v>0.23704950320418605</v>
       </c>
-      <c r="T35">
+      <c r="T59">
         <v>0.23271503321770831</v>
       </c>
-      <c r="U35">
+      <c r="U59">
         <v>0.24584659524473154</v>
       </c>
-      <c r="V35">
+      <c r="V59">
         <v>0.21529025081619735</v>
       </c>
-      <c r="W35">
+      <c r="W59">
         <v>0.21381996798613462</v>
       </c>
-      <c r="X35">
+      <c r="X59">
         <v>0.23992922634315969</v>
       </c>
-      <c r="Y35">
+      <c r="Y59">
         <v>0.2323315222455867</v>
       </c>
-      <c r="Z35">
+      <c r="Z59">
         <v>0.24297964087912982</v>
-      </c>
-    </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
-      <c r="B39" t="s">
-        <v>4</v>
-      </c>
-      <c r="C39" t="s">
-        <v>5</v>
-      </c>
-      <c r="D39">
-        <v>2000</v>
-      </c>
-      <c r="E39">
-        <v>2001</v>
-      </c>
-      <c r="F39">
-        <v>2002</v>
-      </c>
-      <c r="G39">
-        <v>2003</v>
-      </c>
-      <c r="H39">
-        <v>2004</v>
-      </c>
-      <c r="I39">
-        <v>2005</v>
-      </c>
-      <c r="J39">
-        <v>2006</v>
-      </c>
-      <c r="K39">
-        <v>2007</v>
-      </c>
-      <c r="L39">
-        <v>2008</v>
-      </c>
-      <c r="M39">
-        <v>2009</v>
-      </c>
-      <c r="N39">
-        <v>2010</v>
-      </c>
-      <c r="O39">
-        <v>2011</v>
-      </c>
-      <c r="P39">
-        <v>2012</v>
-      </c>
-      <c r="Q39">
-        <v>2013</v>
-      </c>
-      <c r="R39">
-        <v>2014</v>
-      </c>
-      <c r="S39">
-        <v>2015</v>
-      </c>
-      <c r="T39">
-        <v>2016</v>
-      </c>
-      <c r="U39">
-        <v>2017</v>
-      </c>
-      <c r="V39">
-        <v>2018</v>
-      </c>
-      <c r="W39">
-        <v>2019</v>
-      </c>
-      <c r="X39">
-        <v>2020</v>
-      </c>
-      <c r="Y39">
-        <v>2021</v>
-      </c>
-      <c r="Z39">
-        <v>2022</v>
-      </c>
-      <c r="AA39">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>46</v>
-      </c>
-      <c r="B40" t="s">
-        <v>81</v>
-      </c>
-      <c r="C40" t="s">
-        <v>0</v>
-      </c>
-      <c r="D40">
-        <v>0</v>
-      </c>
-      <c r="E40">
-        <v>0</v>
-      </c>
-      <c r="F40">
-        <v>0</v>
-      </c>
-      <c r="G40">
-        <v>0</v>
-      </c>
-      <c r="H40">
-        <v>0</v>
-      </c>
-      <c r="I40">
-        <v>0</v>
-      </c>
-      <c r="J40">
-        <v>0</v>
-      </c>
-      <c r="K40">
-        <v>0</v>
-      </c>
-      <c r="L40">
-        <v>0.22831050228310504</v>
-      </c>
-      <c r="M40">
-        <v>0.11415525114155252</v>
-      </c>
-      <c r="N40">
-        <v>0.45662100456621008</v>
-      </c>
-      <c r="O40">
-        <v>0.68493150684931503</v>
-      </c>
-      <c r="P40">
-        <v>0.7990867579908677</v>
-      </c>
-      <c r="Q40">
-        <v>0.41856925418569257</v>
-      </c>
-      <c r="R40">
-        <v>0.57077625570776258</v>
-      </c>
-      <c r="S40">
-        <v>0.61643835616438358</v>
-      </c>
-      <c r="T40">
-        <v>0.66590563165905636</v>
-      </c>
-      <c r="U40">
-        <v>0.91324200913242015</v>
-      </c>
-      <c r="V40">
-        <v>2.5603392041748205</v>
-      </c>
-      <c r="W40">
-        <v>3.4627092846270933</v>
-      </c>
-      <c r="X40">
-        <v>3.8812785388127851</v>
-      </c>
-      <c r="Y40">
-        <v>5.9132420091324196</v>
-      </c>
-      <c r="Z40">
-        <v>5.1141552511415531</v>
-      </c>
-      <c r="AA40">
-        <v>4.9771689497716896</v>
-      </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>46</v>
-      </c>
-      <c r="B41" t="s">
-        <v>81</v>
-      </c>
-      <c r="C41" t="s">
-        <v>1</v>
-      </c>
-      <c r="D41">
-        <v>0.34409073920603195</v>
-      </c>
-      <c r="E41">
-        <v>0.39609028421001313</v>
-      </c>
-      <c r="F41">
-        <v>0.34896569655015519</v>
-      </c>
-      <c r="G41">
-        <v>0.3908090804205463</v>
-      </c>
-      <c r="H41">
-        <v>0.3922789539227895</v>
-      </c>
-      <c r="I41">
-        <v>0.38314653383146535</v>
-      </c>
-      <c r="J41">
-        <v>0.396222498962225</v>
-      </c>
-      <c r="K41">
-        <v>0.46430053964300544</v>
-      </c>
-      <c r="L41">
-        <v>0.48111249481112495</v>
-      </c>
-      <c r="M41">
-        <v>0.42782873873654675</v>
-      </c>
-      <c r="N41">
-        <v>0.45844586648499153</v>
-      </c>
-      <c r="O41">
-        <v>0.49726171897578175</v>
-      </c>
-      <c r="P41">
-        <v>0.41309028379862439</v>
-      </c>
-      <c r="Q41">
-        <v>0.36227010141320837</v>
-      </c>
-      <c r="R41">
-        <v>0.41231328844516674</v>
-      </c>
-      <c r="S41">
-        <v>0.50828415182197206</v>
-      </c>
-      <c r="T41">
-        <v>0.4369935206742831</v>
-      </c>
-      <c r="U41">
-        <v>0.46734400271649285</v>
-      </c>
-      <c r="V41">
-        <v>0.41685655309224456</v>
-      </c>
-      <c r="W41">
-        <v>0.38424076705180099</v>
-      </c>
-      <c r="X41">
-        <v>0.30180771877150181</v>
-      </c>
-      <c r="Y41">
-        <v>0.38178341330902782</v>
-      </c>
-      <c r="Z41">
-        <v>0.48677943686388042</v>
-      </c>
-      <c r="AA41">
-        <v>0.25824553878597789</v>
-      </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C42" t="s">
-        <v>2</v>
-      </c>
-      <c r="D42">
-        <v>0.19642930601834707</v>
-      </c>
-      <c r="E42">
-        <v>0.19642930601834707</v>
-      </c>
-      <c r="F42">
-        <v>0.1583775556378296</v>
-      </c>
-      <c r="G42">
-        <v>0.18100292072894811</v>
-      </c>
-      <c r="H42">
-        <v>0.15323542720802993</v>
-      </c>
-      <c r="I42">
-        <v>0.1779176436710683</v>
-      </c>
-      <c r="J42">
-        <v>0.22213994816734542</v>
-      </c>
-      <c r="K42">
-        <v>0.23228111971411552</v>
-      </c>
-      <c r="L42">
-        <v>0.23426642842962081</v>
-      </c>
-      <c r="M42">
-        <v>0.19456025411951558</v>
-      </c>
-      <c r="N42">
-        <v>0.19555290847726822</v>
-      </c>
-      <c r="O42">
-        <v>0.19786910197869106</v>
-      </c>
-      <c r="P42">
-        <v>0.22450532724505329</v>
-      </c>
-      <c r="Q42">
-        <v>0.2226027397260274</v>
-      </c>
-      <c r="R42">
-        <v>0.20357686453576868</v>
-      </c>
-      <c r="S42">
-        <v>0.17694063926940642</v>
-      </c>
-      <c r="T42">
-        <v>0.1950152207001522</v>
-      </c>
-      <c r="U42">
-        <v>0.18359969558599698</v>
-      </c>
-      <c r="V42">
-        <v>0.19216133942161343</v>
-      </c>
-      <c r="W42">
-        <v>0.20452815829528159</v>
-      </c>
-      <c r="X42">
-        <v>0.21784627092846273</v>
-      </c>
-      <c r="Y42">
-        <v>0.29014459665144599</v>
-      </c>
-      <c r="Z42">
-        <v>0.1950152207001522</v>
-      </c>
-      <c r="AA42">
-        <v>0.14840182648401828</v>
-      </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>46</v>
-      </c>
-      <c r="B43" t="s">
-        <v>81</v>
-      </c>
-      <c r="C43" t="s">
-        <v>12</v>
-      </c>
-      <c r="D43">
-        <v>0.29434148088459128</v>
-      </c>
-      <c r="E43">
-        <v>0.22423352902804958</v>
-      </c>
-      <c r="F43">
-        <v>0.22408253001860307</v>
-      </c>
-      <c r="G43">
-        <v>0.20686315206863154</v>
-      </c>
-      <c r="H43">
-        <v>0.18103408514367419</v>
-      </c>
-      <c r="I43">
-        <v>0.24791291914579586</v>
-      </c>
-      <c r="J43">
-        <v>0.2427240440939071</v>
-      </c>
-      <c r="K43">
-        <v>0.16072605011472321</v>
-      </c>
-      <c r="L43">
-        <v>0.1502326182476092</v>
-      </c>
-      <c r="M43">
-        <v>0.18296846327828276</v>
-      </c>
-      <c r="N43">
-        <v>0.26339491433119683</v>
-      </c>
-      <c r="O43">
-        <v>0.14626141552511415</v>
-      </c>
-      <c r="P43">
-        <v>0.15647142182333496</v>
-      </c>
-      <c r="Q43">
-        <v>0.19708855325293684</v>
-      </c>
-      <c r="R43">
-        <v>0.22250599798777185</v>
-      </c>
-      <c r="S43">
-        <v>0.27329541057193724</v>
-      </c>
-      <c r="T43">
-        <v>0.18767897221577279</v>
-      </c>
-      <c r="U43">
-        <v>0.12870890865760704</v>
-      </c>
-      <c r="V43">
-        <v>0.23422292564900221</v>
-      </c>
-      <c r="W43">
-        <v>0.13325692663137406</v>
-      </c>
-      <c r="X43">
-        <v>0.12825410686023031</v>
-      </c>
-      <c r="Y43">
-        <v>0.21921446633557101</v>
-      </c>
-      <c r="Z43">
-        <v>0.17145847997545438</v>
-      </c>
-      <c r="AA43">
-        <v>0.14032522966412186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" t="s">
-        <v>81</v>
-      </c>
-      <c r="C44" t="s">
-        <v>13</v>
-      </c>
-      <c r="D44">
-        <v>0.58791571267802401</v>
-      </c>
-      <c r="E44">
-        <v>0.632219592016247</v>
-      </c>
-      <c r="F44">
-        <v>0.84860999194198217</v>
-      </c>
-      <c r="G44">
-        <v>0.72522159548751008</v>
-      </c>
-      <c r="H44">
-        <v>0.70591592801504166</v>
-      </c>
-      <c r="I44">
-        <v>0.78271890948160072</v>
-      </c>
-      <c r="J44">
-        <v>0.81797273704002138</v>
-      </c>
-      <c r="K44">
-        <v>0.88425019931869253</v>
-      </c>
-      <c r="L44">
-        <v>0.95250175158850958</v>
-      </c>
-      <c r="M44">
-        <v>0.92169795366142393</v>
-      </c>
-      <c r="N44">
-        <v>0.92109395762363799</v>
-      </c>
-      <c r="O44">
-        <v>0.98511753762895304</v>
-      </c>
-      <c r="P44">
-        <v>0.94312558272968505</v>
-      </c>
-      <c r="Q44">
-        <v>0.81695954983626218</v>
-      </c>
-      <c r="R44">
-        <v>0.91497163414971638</v>
-      </c>
-      <c r="S44">
-        <v>0.88672109220054429</v>
-      </c>
-      <c r="T44">
-        <v>0.91440094569223274</v>
-      </c>
-      <c r="U44">
-        <v>0.90107317525438657</v>
-      </c>
-      <c r="V44">
-        <v>0.91608169199663791</v>
-      </c>
-      <c r="W44">
-        <v>0.94050296462891025</v>
-      </c>
-      <c r="X44">
-        <v>0.9444785206388151</v>
-      </c>
-      <c r="Y44">
-        <v>0.93652740861900541</v>
-      </c>
-      <c r="Z44">
-        <v>0.93482359890047495</v>
-      </c>
-      <c r="AA44">
-        <v>0.91778550171516859</v>
-      </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>81</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45">
-        <v>65535</v>
-      </c>
-      <c r="E45">
-        <v>65535</v>
-      </c>
-      <c r="F45">
-        <v>65535</v>
-      </c>
-      <c r="G45">
-        <v>65535</v>
-      </c>
-      <c r="H45">
-        <v>65535</v>
-      </c>
-      <c r="I45">
-        <v>65535</v>
-      </c>
-      <c r="J45">
-        <v>65535</v>
-      </c>
-      <c r="K45">
-        <v>65535</v>
-      </c>
-      <c r="L45">
-        <v>65535</v>
-      </c>
-      <c r="M45">
-        <v>65535</v>
-      </c>
-      <c r="N45">
-        <v>65535</v>
-      </c>
-      <c r="O45">
-        <v>65535</v>
-      </c>
-      <c r="P45">
-        <v>65535</v>
-      </c>
-      <c r="Q45">
-        <v>65535</v>
-      </c>
-      <c r="R45">
-        <v>65535</v>
-      </c>
-      <c r="S45">
-        <v>65535</v>
-      </c>
-      <c r="T45">
-        <v>65535</v>
-      </c>
-      <c r="U45">
-        <v>65535</v>
-      </c>
-      <c r="V45">
-        <v>65535</v>
-      </c>
-      <c r="W45">
-        <v>65535</v>
-      </c>
-      <c r="X45">
-        <v>65535</v>
-      </c>
-      <c r="Y45">
-        <v>65535</v>
-      </c>
-      <c r="Z45">
-        <v>65535</v>
-      </c>
-      <c r="AA45">
-        <v>65535</v>
-      </c>
-    </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" t="s">
-        <v>81</v>
-      </c>
-      <c r="C46" t="s">
-        <v>14</v>
-      </c>
-      <c r="N46">
-        <v>3.8051750380517509E-2</v>
-      </c>
-      <c r="O46">
-        <v>7.6103500761035017E-2</v>
-      </c>
-      <c r="P46">
-        <v>9.6783799880881469E-2</v>
-      </c>
-      <c r="Q46">
-        <v>0.1525728837372673</v>
-      </c>
-      <c r="R46">
-        <v>0.13964622955180209</v>
-      </c>
-      <c r="S46">
-        <v>0.15294587046149752</v>
-      </c>
-      <c r="T46">
-        <v>0.1540541738706388</v>
-      </c>
-      <c r="U46">
-        <v>0.15516247727978011</v>
-      </c>
-      <c r="V46">
-        <v>0.14851265682493239</v>
-      </c>
-      <c r="W46">
-        <v>0.15586582367404284</v>
-      </c>
-      <c r="X46">
-        <v>0.15255292652552924</v>
-      </c>
-      <c r="Y46">
-        <v>0.13213245604573401</v>
-      </c>
-      <c r="Z46">
-        <v>0.13711751430220961</v>
-      </c>
-      <c r="AA46">
-        <v>0.13667567483614451</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>81</v>
-      </c>
-      <c r="C47" t="s">
-        <v>15</v>
-      </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-      <c r="J47">
-        <v>7.6103500761035017E-2</v>
-      </c>
-      <c r="K47">
-        <v>0.19025875190258754</v>
-      </c>
-      <c r="L47">
-        <v>0.12453300124533001</v>
-      </c>
-      <c r="M47">
-        <v>8.3022000830220002E-2</v>
-      </c>
-      <c r="N47">
-        <v>0.15841953219644023</v>
-      </c>
-      <c r="O47">
-        <v>0.18180280737358362</v>
-      </c>
-      <c r="P47">
-        <v>0.20480795057749127</v>
-      </c>
-      <c r="Q47">
-        <v>0.22998925597636316</v>
-      </c>
-      <c r="R47">
-        <v>0.21689497716894979</v>
-      </c>
-      <c r="S47">
-        <v>0.23646444879321593</v>
-      </c>
-      <c r="T47">
-        <v>0.23157208088714937</v>
-      </c>
-      <c r="U47">
-        <v>0.24461839530332682</v>
-      </c>
-      <c r="V47">
-        <v>0.21526418786692761</v>
-      </c>
-      <c r="W47">
-        <v>0.21526418786692761</v>
-      </c>
-      <c r="X47">
-        <v>0.24135681669928247</v>
-      </c>
-      <c r="Y47">
-        <v>0.23320287018917157</v>
-      </c>
-      <c r="Z47">
-        <v>0.23483365949119375</v>
-      </c>
-      <c r="AA47">
-        <v>0.25277234181343772</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 06:46
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084AEEE7-24EF-4FB0-A3B3-88130D991CD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D0BD70-0281-439A-9917-0887ED86DD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="90">
   <si>
     <t>bioenergy</t>
   </si>
@@ -95,9 +95,6 @@
     <t>oil</t>
   </si>
   <si>
-    <t>iso_code</t>
-  </si>
-  <si>
     <t>model_fuel</t>
   </si>
   <si>
@@ -198,12 +195,6 @@
   </si>
   <si>
     <t>IRENA Utilization Factors</t>
-  </si>
-  <si>
-    <t>source</t>
-  </si>
-  <si>
-    <t>IRENA</t>
   </si>
   <si>
     <t>EMBER Utilization Factors</t>
@@ -859,36 +850,36 @@
     </row>
     <row r="3" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Q3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="R3">
         <v>2050</v>
       </c>
       <c r="S3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="T3">
         <v>2050</v>
       </c>
       <c r="V3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="O4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P4" t="s">
         <v>1</v>
@@ -905,20 +896,20 @@
     </row>
     <row r="5" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="e">
         <f>VLOOKUP(B5,historical_data!$B$2:$J$12,MATCH(Veda!$J5,historical_data!$B$1:$I$1,0),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="P5" t="s">
         <v>2</v>
@@ -938,50 +929,50 @@
     </row>
     <row r="6" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" t="e">
         <f>VLOOKUP(B6,historical_data!$B$2:$J$12,MATCH(Veda!$J6,historical_data!$B$1:$I$1,0),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U6" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="AD6" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" t="e">
         <f>VLOOKUP(B7,historical_data!$B$2:$J$12,MATCH(Veda!$J7,historical_data!$B$1:$I$1,0),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="U7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="V7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="W7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="X7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="Y7">
         <v>2022</v>
@@ -990,55 +981,55 @@
         <v>2050</v>
       </c>
       <c r="AA7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AB7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="AD7" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="AE7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="AF7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="AG7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="AH7">
         <v>2050</v>
       </c>
       <c r="AI7" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="AJ7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" t="e">
         <f>VLOOKUP(B8,historical_data!$B$2:$J$12,MATCH(Veda!$J8,historical_data!$B$1:$I$1,0),FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="J8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="U8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="V8" t="s">
         <v>1</v>
       </c>
       <c r="W8" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="X8">
         <v>1</v>
@@ -1055,7 +1046,7 @@
         <v>3</v>
       </c>
       <c r="AD8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="AE8" t="s">
         <v>1</v>
@@ -1076,13 +1067,13 @@
     </row>
     <row r="9" spans="2:36" x14ac:dyDescent="0.45">
       <c r="U9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="V9" t="s">
         <v>2</v>
       </c>
       <c r="W9" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="X9">
         <v>1</v>
@@ -1102,7 +1093,7 @@
         <v>3</v>
       </c>
       <c r="AD9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="AE9" t="s">
         <v>2</v>
@@ -1125,23 +1116,23 @@
     <row r="11" spans="2:36" ht="14.65" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="13" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15">
         <v>2100</v>
@@ -1151,63 +1142,63 @@
         <v>Bioenergy + CCUS,Bioenergy - Cofiring,Bioenergy - Large scale unit,Bioenergy - Medium-scale CHP,Concentrating solar power,Fuel cell (distributed electricity generation),Marine,Oxyfuel + CCS,Solar photovoltaics - Buildings,Solar photovoltaics - Large scale unit,Wind offshore,Wind onshore,CCGT - CHP</v>
       </c>
       <c r="L15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="2:36" x14ac:dyDescent="0.45">
       <c r="L16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E22">
         <f>G22*3.6</f>
@@ -1217,18 +1208,18 @@
         <v>94</v>
       </c>
       <c r="L22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C23" t="s">
         <v>2</v>
       </c>
       <c r="D23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E23">
         <f t="shared" ref="E23:E24" si="0">G23*3.6</f>
@@ -1238,18 +1229,18 @@
         <v>55</v>
       </c>
       <c r="L23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" t="s">
         <v>3</v>
       </c>
       <c r="D24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
@@ -1259,22 +1250,22 @@
         <v>70</v>
       </c>
       <c r="L24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.45">
       <c r="L27" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1275,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z81"/>
+  <dimension ref="A1:Z71"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="U26" sqref="U26"/>
@@ -1305,90 +1296,90 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D1" t="s">
         <v>59</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>71</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>72</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>73</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>74</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>75</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>76</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>77</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>78</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>79</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>80</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>81</v>
-      </c>
-      <c r="X1" t="s">
-        <v>82</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>83</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>2000</v>
@@ -1465,10 +1456,10 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C3">
         <v>5.6</v>
@@ -1545,10 +1536,10 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1625,12 +1616,12 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8">
         <v>2000</v>
@@ -1938,7 +1929,7 @@
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <v>0.29434148088459128</v>
@@ -2015,7 +2006,7 @@
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>0.58791571267802401</v>
@@ -2169,7 +2160,7 @@
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L15">
         <v>3.8051750380517509E-2</v>
@@ -2216,7 +2207,7 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G16">
         <v>0</v>
@@ -2278,12 +2269,12 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>2000</v>
@@ -2591,7 +2582,7 @@
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24">
         <v>1.02</v>
@@ -2668,7 +2659,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B25">
         <v>3.53</v>
@@ -2822,7 +2813,7 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -2899,7 +2890,7 @@
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -2976,12 +2967,12 @@
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32">
         <v>2000</v>
@@ -3289,7 +3280,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B36">
         <v>2.63</v>
@@ -3366,7 +3357,7 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37">
         <v>18.18</v>
@@ -3520,7 +3511,7 @@
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -3597,7 +3588,7 @@
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -3674,12 +3665,12 @@
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43">
         <v>2000</v>
@@ -3803,7 +3794,7 @@
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B45">
         <v>0.17918731176527739</v>
@@ -3877,7 +3868,7 @@
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46">
         <v>0.58751816400088952</v>
@@ -4025,7 +4016,7 @@
     </row>
     <row r="48" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I48">
         <v>0.22831050228310501</v>
@@ -4078,7 +4069,7 @@
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F49">
         <v>0.11415525114155251</v>
@@ -4140,12 +4131,12 @@
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B53">
         <v>2000</v>
@@ -4305,7 +4296,7 @@
     </row>
     <row r="55" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B55">
         <v>1.88</v>
@@ -4385,7 +4376,7 @@
     </row>
     <row r="56" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B56">
         <v>3.532</v>
@@ -4545,7 +4536,7 @@
     </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I58">
         <v>2.9999999999999997E-5</v>
@@ -4604,7 +4595,7 @@
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F59">
         <v>1E-3</v>
@@ -4672,12 +4663,12 @@
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B63">
         <v>2000</v>
@@ -4799,7 +4790,7 @@
         <v>2.2435940000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>1</v>
       </c>
@@ -4873,7 +4864,7 @@
         <v>21.785509999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -4947,9 +4938,9 @@
         <v>2.0534110000000001</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B67">
         <v>2.9509999999999996</v>
@@ -5021,9 +5012,9 @@
         <v>3.833256</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B68">
         <v>18.178000000000001</v>
@@ -5095,7 +5086,7 @@
         <v>16.462018</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -5169,9 +5160,9 @@
         <v>0.52855200000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I70">
         <v>5.9999999999999995E-5</v>
@@ -5222,9 +5213,9 @@
         <v>2.0938380000000003</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F71">
         <v>1E-3</v>
@@ -5282,514 +5273,6 @@
       </c>
       <c r="X71">
         <v>1.499125</v>
-      </c>
-    </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A75" t="s">
-        <v>39</v>
-      </c>
-      <c r="B75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" t="s">
-        <v>5</v>
-      </c>
-      <c r="D75">
-        <v>2000</v>
-      </c>
-      <c r="E75">
-        <v>2001</v>
-      </c>
-      <c r="F75">
-        <v>2002</v>
-      </c>
-      <c r="G75">
-        <v>2003</v>
-      </c>
-      <c r="H75">
-        <v>2004</v>
-      </c>
-      <c r="I75">
-        <v>2005</v>
-      </c>
-      <c r="J75">
-        <v>2006</v>
-      </c>
-      <c r="K75">
-        <v>2007</v>
-      </c>
-      <c r="L75">
-        <v>2008</v>
-      </c>
-      <c r="M75">
-        <v>2009</v>
-      </c>
-      <c r="N75">
-        <v>2010</v>
-      </c>
-      <c r="O75">
-        <v>2011</v>
-      </c>
-      <c r="P75">
-        <v>2012</v>
-      </c>
-      <c r="Q75">
-        <v>2013</v>
-      </c>
-      <c r="R75">
-        <v>2014</v>
-      </c>
-      <c r="S75">
-        <v>2015</v>
-      </c>
-      <c r="T75">
-        <v>2016</v>
-      </c>
-      <c r="U75">
-        <v>2017</v>
-      </c>
-      <c r="V75">
-        <v>2018</v>
-      </c>
-      <c r="W75">
-        <v>2019</v>
-      </c>
-      <c r="X75">
-        <v>2020</v>
-      </c>
-      <c r="Y75">
-        <v>2021</v>
-      </c>
-      <c r="Z75">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A76" t="s">
-        <v>40</v>
-      </c>
-      <c r="B76" t="s">
-        <v>86</v>
-      </c>
-      <c r="C76" t="s">
-        <v>0</v>
-      </c>
-      <c r="L76">
-        <v>0.30441400304414001</v>
-      </c>
-      <c r="M76">
-        <v>0.10147133434804669</v>
-      </c>
-      <c r="N76">
-        <v>0.40447488584474894</v>
-      </c>
-      <c r="O76">
-        <v>0.5811540058115402</v>
-      </c>
-      <c r="P76">
-        <v>0.53816046966731901</v>
-      </c>
-      <c r="Q76">
-        <v>0.37067553048616708</v>
-      </c>
-      <c r="R76">
-        <v>0.57077625570776258</v>
-      </c>
-      <c r="S76">
-        <v>0.57500422797226458</v>
-      </c>
-      <c r="T76">
-        <v>0.70696146759593048</v>
-      </c>
-      <c r="U76">
-        <v>0.86924428402751963</v>
-      </c>
-      <c r="V76">
-        <v>2.5863099724480505</v>
-      </c>
-      <c r="W76">
-        <v>3.6549813955986812</v>
-      </c>
-      <c r="X76">
-        <v>4.036889720525596</v>
-      </c>
-      <c r="Y76">
-        <v>6.2453375126974553</v>
-      </c>
-      <c r="Z76">
-        <v>3.2548137163984849</v>
-      </c>
-    </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A77" t="s">
-        <v>40</v>
-      </c>
-      <c r="B77" t="s">
-        <v>86</v>
-      </c>
-      <c r="C77" t="s">
-        <v>8</v>
-      </c>
-      <c r="D77">
-        <v>0.17918731176527739</v>
-      </c>
-      <c r="E77">
-        <v>0.14535545467936098</v>
-      </c>
-      <c r="F77">
-        <v>0.15845780240593327</v>
-      </c>
-      <c r="G77">
-        <v>0.1498316039834055</v>
-      </c>
-      <c r="H77">
-        <v>0.1347902156764661</v>
-      </c>
-      <c r="I77">
-        <v>0.18958653994151151</v>
-      </c>
-      <c r="J77">
-        <v>0.18353719344825822</v>
-      </c>
-      <c r="K77">
-        <v>0.12836507928947488</v>
-      </c>
-      <c r="L77">
-        <v>0.12535509016122517</v>
-      </c>
-      <c r="M77">
-        <v>0.15416139825537606</v>
-      </c>
-      <c r="N77">
-        <v>0.21319901365069094</v>
-      </c>
-      <c r="O77">
-        <v>0.13556538436675425</v>
-      </c>
-      <c r="P77">
-        <v>0.1426745416205524</v>
-      </c>
-      <c r="Q77">
-        <v>0.17089921406444017</v>
-      </c>
-      <c r="R77">
-        <v>0.18308207829936693</v>
-      </c>
-      <c r="S77">
-        <v>0.21797454043557021</v>
-      </c>
-      <c r="T77">
-        <v>0.16178813238750592</v>
-      </c>
-      <c r="U77">
-        <v>0.11826549026371555</v>
-      </c>
-      <c r="V77">
-        <v>0.18320015783762453</v>
-      </c>
-      <c r="W77">
-        <v>0.11430375923833559</v>
-      </c>
-      <c r="X77">
-        <v>0.11225524213694742</v>
-      </c>
-      <c r="Y77">
-        <v>0.1716829439171017</v>
-      </c>
-      <c r="Z77">
-        <v>0.13069358514235713</v>
-      </c>
-    </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A78" t="s">
-        <v>40</v>
-      </c>
-      <c r="B78" t="s">
-        <v>86</v>
-      </c>
-      <c r="C78" t="s">
-        <v>9</v>
-      </c>
-      <c r="D78">
-        <v>0.58751816400088952</v>
-      </c>
-      <c r="E78">
-        <v>0.63195855763612019</v>
-      </c>
-      <c r="F78">
-        <v>0.84807034848805107</v>
-      </c>
-      <c r="G78">
-        <v>0.72468873612271401</v>
-      </c>
-      <c r="H78">
-        <v>0.70518756353607848</v>
-      </c>
-      <c r="I78">
-        <v>0.78226961776024206</v>
-      </c>
-      <c r="J78">
-        <v>0.81749754243287398</v>
-      </c>
-      <c r="K78">
-        <v>0.88349648121868596</v>
-      </c>
-      <c r="L78">
-        <v>0.95119319991890894</v>
-      </c>
-      <c r="M78">
-        <v>0.92048229990249752</v>
-      </c>
-      <c r="N78">
-        <v>0.92005994960757642</v>
-      </c>
-      <c r="O78">
-        <v>0.98431753019201262</v>
-      </c>
-      <c r="P78">
-        <v>0.94540432280661413</v>
-      </c>
-      <c r="Q78">
-        <v>0.81619276686525755</v>
-      </c>
-      <c r="R78">
-        <v>0.91711461765215874</v>
-      </c>
-      <c r="S78">
-        <v>0.88913935610658323</v>
-      </c>
-      <c r="T78">
-        <v>0.91556341739152636</v>
-      </c>
-      <c r="U78">
-        <v>0.90218624426321981</v>
-      </c>
-      <c r="V78">
-        <v>0.91672584775055033</v>
-      </c>
-      <c r="W78">
-        <v>0.942110199083116</v>
-      </c>
-      <c r="X78">
-        <v>0.94612082701666678</v>
-      </c>
-      <c r="Y78">
-        <v>0.9382181082323805</v>
-      </c>
-      <c r="Z78">
-        <v>0.93680249206717758</v>
-      </c>
-    </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A79" t="s">
-        <v>40</v>
-      </c>
-      <c r="B79" t="s">
-        <v>86</v>
-      </c>
-      <c r="C79" t="s">
-        <v>3</v>
-      </c>
-      <c r="D79">
-        <v>1.3728687025740881E-2</v>
-      </c>
-      <c r="E79">
-        <v>8.9246408872480296E-3</v>
-      </c>
-      <c r="F79">
-        <v>1.4064542368890371E-2</v>
-      </c>
-      <c r="G79">
-        <v>1.3440969291696423E-2</v>
-      </c>
-      <c r="H79">
-        <v>1.4367639360976603E-2</v>
-      </c>
-      <c r="I79">
-        <v>1.06544901065449E-2</v>
-      </c>
-      <c r="J79">
-        <v>6.8721033906174785E-3</v>
-      </c>
-      <c r="K79">
-        <v>1.3383397499030053E-2</v>
-      </c>
-      <c r="L79">
-        <v>6.8134032678754683E-3</v>
-      </c>
-      <c r="M79">
-        <v>8.974387151398696E-3</v>
-      </c>
-      <c r="N79">
-        <v>1.0171012962918537E-2</v>
-      </c>
-      <c r="O79">
-        <v>4.0275281549390085E-3</v>
-      </c>
-      <c r="P79">
-        <v>5.4770281784942507E-3</v>
-      </c>
-      <c r="Q79">
-        <v>5.9193423561722108E-3</v>
-      </c>
-      <c r="R79">
-        <v>5.7979529360833674E-3</v>
-      </c>
-      <c r="S79">
-        <v>5.9440758150922698E-3</v>
-      </c>
-      <c r="T79">
-        <v>1.0672682178439969E-2</v>
-      </c>
-      <c r="U79">
-        <v>1.3166338195431674E-2</v>
-      </c>
-      <c r="V79">
-        <v>1.0273264456408587E-2</v>
-      </c>
-      <c r="W79">
-        <v>1.1459284473580975E-2</v>
-      </c>
-      <c r="X79">
-        <v>1.0273784895450284E-2</v>
-      </c>
-      <c r="Y79">
-        <v>1.1799059936493149E-2</v>
-      </c>
-      <c r="Z79">
-        <v>1.5180712412366853E-2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A80" t="s">
-        <v>40</v>
-      </c>
-      <c r="B80" t="s">
-        <v>86</v>
-      </c>
-      <c r="C80" t="s">
-        <v>10</v>
-      </c>
-      <c r="K80">
-        <v>0.22831050228310501</v>
-      </c>
-      <c r="L80">
-        <v>0.1906392694063927</v>
-      </c>
-      <c r="M80">
-        <v>0.18647260273972602</v>
-      </c>
-      <c r="N80">
-        <v>6.7876712328767116E-2</v>
-      </c>
-      <c r="O80">
-        <v>7.476575935480044E-2</v>
-      </c>
-      <c r="P80">
-        <v>9.6412405035707568E-2</v>
-      </c>
-      <c r="Q80">
-        <v>0.15293804193529958</v>
-      </c>
-      <c r="R80">
-        <v>0.13941040865139273</v>
-      </c>
-      <c r="S80">
-        <v>0.1534278778672068</v>
-      </c>
-      <c r="T80">
-        <v>0.15383140488540142</v>
-      </c>
-      <c r="U80">
-        <v>0.15538589047072227</v>
-      </c>
-      <c r="V80">
-        <v>0.14838111835914639</v>
-      </c>
-      <c r="W80">
-        <v>0.15491400651998427</v>
-      </c>
-      <c r="X80">
-        <v>0.15239085998651261</v>
-      </c>
-      <c r="Y80">
-        <v>0.13133926069138591</v>
-      </c>
-      <c r="Z80">
-        <v>0.13764325363624622</v>
-      </c>
-    </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A81" t="s">
-        <v>40</v>
-      </c>
-      <c r="B81" t="s">
-        <v>86</v>
-      </c>
-      <c r="C81" t="s">
-        <v>11</v>
-      </c>
-      <c r="H81">
-        <v>0.11415525114155251</v>
-      </c>
-      <c r="I81">
-        <v>6.5453767123287668E-2</v>
-      </c>
-      <c r="J81">
-        <v>8.4758159986470502E-2</v>
-      </c>
-      <c r="K81">
-        <v>0.17808980213089803</v>
-      </c>
-      <c r="L81">
-        <v>0.12192381639029079</v>
-      </c>
-      <c r="M81">
-        <v>8.1248714467892558E-2</v>
-      </c>
-      <c r="N81">
-        <v>0.15938903548169775</v>
-      </c>
-      <c r="O81">
-        <v>0.18169781142649755</v>
-      </c>
-      <c r="P81">
-        <v>0.2058669391554197</v>
-      </c>
-      <c r="Q81">
-        <v>0.22956604290766625</v>
-      </c>
-      <c r="R81">
-        <v>0.2172995015710637</v>
-      </c>
-      <c r="S81">
-        <v>0.23704950320418605</v>
-      </c>
-      <c r="T81">
-        <v>0.23271503321770831</v>
-      </c>
-      <c r="U81">
-        <v>0.24584659524473154</v>
-      </c>
-      <c r="V81">
-        <v>0.21529025081619735</v>
-      </c>
-      <c r="W81">
-        <v>0.21381996798613462</v>
-      </c>
-      <c r="X81">
-        <v>0.23992922634315969</v>
-      </c>
-      <c r="Y81">
-        <v>0.2323315222455867</v>
-      </c>
-      <c r="Z81">
-        <v>0.24297964087912982</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 07:12
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F14531B-1C43-4896-9029-F6F8C68D0C50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D07D71F-687F-451C-A851-B72DD70DCF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1275,7 +1275,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z72"/>
+  <dimension ref="A1:Z74"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="U26" sqref="U26"/>
@@ -2022,3256 +2022,3256 @@
         <v>0.25277234181343772</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14">
-        <v>2000</v>
-      </c>
-      <c r="C14">
-        <v>2001</v>
-      </c>
-      <c r="D14">
-        <v>2002</v>
-      </c>
-      <c r="E14">
-        <v>2003</v>
-      </c>
-      <c r="F14">
-        <v>2004</v>
-      </c>
-      <c r="G14">
-        <v>2005</v>
-      </c>
-      <c r="H14">
-        <v>2006</v>
-      </c>
-      <c r="I14">
-        <v>2007</v>
-      </c>
-      <c r="J14">
-        <v>2008</v>
-      </c>
-      <c r="K14">
-        <v>2009</v>
-      </c>
-      <c r="L14">
-        <v>2010</v>
-      </c>
-      <c r="M14">
-        <v>2011</v>
-      </c>
-      <c r="N14">
-        <v>2012</v>
-      </c>
-      <c r="O14">
-        <v>2013</v>
-      </c>
-      <c r="P14">
-        <v>2014</v>
-      </c>
-      <c r="Q14">
-        <v>2015</v>
-      </c>
-      <c r="R14">
-        <v>2016</v>
-      </c>
-      <c r="S14">
-        <v>2017</v>
-      </c>
-      <c r="T14">
-        <v>2018</v>
-      </c>
-      <c r="U14">
-        <v>2019</v>
-      </c>
-      <c r="V14">
-        <v>2020</v>
-      </c>
-      <c r="W14">
-        <v>2021</v>
-      </c>
-      <c r="X14">
-        <v>2022</v>
-      </c>
-    </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0.30441400304414001</v>
-      </c>
-      <c r="K15">
-        <v>0.10147133434804669</v>
-      </c>
-      <c r="L15">
-        <v>0.40447488584474894</v>
-      </c>
-      <c r="M15">
-        <v>0.5811540058115402</v>
-      </c>
-      <c r="N15">
-        <v>0.53816046966731901</v>
-      </c>
-      <c r="O15">
-        <v>0.37067553048616708</v>
-      </c>
-      <c r="P15">
-        <v>0.57077625570776258</v>
-      </c>
-      <c r="Q15">
-        <v>0.57500422797226458</v>
-      </c>
-      <c r="R15">
-        <v>0.70696146759593048</v>
-      </c>
-      <c r="S15">
-        <v>0.86924428402751963</v>
-      </c>
-      <c r="T15">
-        <v>2.5863099724480505</v>
-      </c>
-      <c r="U15">
-        <v>3.6549813955986812</v>
-      </c>
-      <c r="V15">
-        <v>4.036889720525596</v>
-      </c>
-      <c r="W15">
-        <v>6.2453375126974553</v>
-      </c>
-      <c r="X15">
-        <v>3.2548137163984849</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B16">
-        <v>0.17918731176527739</v>
+        <v>2000</v>
       </c>
       <c r="C16">
-        <v>0.14535545467936098</v>
+        <v>2001</v>
       </c>
       <c r="D16">
-        <v>0.15845780240593327</v>
+        <v>2002</v>
       </c>
       <c r="E16">
-        <v>0.1498316039834055</v>
+        <v>2003</v>
       </c>
       <c r="F16">
-        <v>0.1347902156764661</v>
+        <v>2004</v>
       </c>
       <c r="G16">
-        <v>0.18958653994151151</v>
+        <v>2005</v>
       </c>
       <c r="H16">
-        <v>0.18353719344825822</v>
+        <v>2006</v>
       </c>
       <c r="I16">
-        <v>0.12836507928947488</v>
+        <v>2007</v>
       </c>
       <c r="J16">
-        <v>0.12535509016122517</v>
+        <v>2008</v>
       </c>
       <c r="K16">
-        <v>0.15416139825537606</v>
+        <v>2009</v>
       </c>
       <c r="L16">
-        <v>0.21319901365069094</v>
+        <v>2010</v>
       </c>
       <c r="M16">
-        <v>0.13556538436675425</v>
+        <v>2011</v>
       </c>
       <c r="N16">
-        <v>0.1426745416205524</v>
+        <v>2012</v>
       </c>
       <c r="O16">
-        <v>0.17089921406444017</v>
+        <v>2013</v>
       </c>
       <c r="P16">
-        <v>0.18308207829936693</v>
+        <v>2014</v>
       </c>
       <c r="Q16">
-        <v>0.21797454043557021</v>
+        <v>2015</v>
       </c>
       <c r="R16">
-        <v>0.16178813238750592</v>
+        <v>2016</v>
       </c>
       <c r="S16">
-        <v>0.11826549026371555</v>
+        <v>2017</v>
       </c>
       <c r="T16">
-        <v>0.18320015783762453</v>
+        <v>2018</v>
       </c>
       <c r="U16">
-        <v>0.11430375923833559</v>
+        <v>2019</v>
       </c>
       <c r="V16">
-        <v>0.11225524213694742</v>
+        <v>2020</v>
       </c>
       <c r="W16">
-        <v>0.1716829439171017</v>
+        <v>2021</v>
       </c>
       <c r="X16">
-        <v>0.13069358514235713</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17">
-        <v>0.58751816400088952</v>
-      </c>
-      <c r="C17">
-        <v>0.63195855763612019</v>
-      </c>
-      <c r="D17">
-        <v>0.84807034848805107</v>
-      </c>
-      <c r="E17">
-        <v>0.72468873612271401</v>
-      </c>
-      <c r="F17">
-        <v>0.70518756353607848</v>
-      </c>
-      <c r="G17">
-        <v>0.78226961776024206</v>
-      </c>
-      <c r="H17">
-        <v>0.81749754243287398</v>
-      </c>
-      <c r="I17">
-        <v>0.88349648121868596</v>
+        <v>0</v>
       </c>
       <c r="J17">
-        <v>0.95119319991890894</v>
+        <v>0.30441400304414001</v>
       </c>
       <c r="K17">
-        <v>0.92048229990249752</v>
+        <v>0.10147133434804669</v>
       </c>
       <c r="L17">
-        <v>0.92005994960757642</v>
+        <v>0.40447488584474894</v>
       </c>
       <c r="M17">
-        <v>0.98431753019201262</v>
+        <v>0.5811540058115402</v>
       </c>
       <c r="N17">
-        <v>0.94540432280661413</v>
+        <v>0.53816046966731901</v>
       </c>
       <c r="O17">
-        <v>0.81619276686525755</v>
+        <v>0.37067553048616708</v>
       </c>
       <c r="P17">
-        <v>0.91711461765215874</v>
+        <v>0.57077625570776258</v>
       </c>
       <c r="Q17">
-        <v>0.88913935610658323</v>
+        <v>0.57500422797226458</v>
       </c>
       <c r="R17">
-        <v>0.91556341739152636</v>
+        <v>0.70696146759593048</v>
       </c>
       <c r="S17">
-        <v>0.90218624426321981</v>
+        <v>0.86924428402751963</v>
       </c>
       <c r="T17">
-        <v>0.91672584775055033</v>
+        <v>2.5863099724480505</v>
       </c>
       <c r="U17">
-        <v>0.942110199083116</v>
+        <v>3.6549813955986812</v>
       </c>
       <c r="V17">
-        <v>0.94612082701666678</v>
+        <v>4.036889720525596</v>
       </c>
       <c r="W17">
-        <v>0.9382181082323805</v>
+        <v>6.2453375126974553</v>
       </c>
       <c r="X17">
-        <v>0.93680249206717758</v>
+        <v>3.2548137163984849</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B18">
-        <v>1.3728687025740881E-2</v>
+        <v>0.17918731176527739</v>
       </c>
       <c r="C18">
-        <v>8.9246408872480296E-3</v>
+        <v>0.14535545467936098</v>
       </c>
       <c r="D18">
-        <v>1.4064542368890371E-2</v>
+        <v>0.15845780240593327</v>
       </c>
       <c r="E18">
-        <v>1.3440969291696423E-2</v>
+        <v>0.1498316039834055</v>
       </c>
       <c r="F18">
-        <v>1.4367639360976603E-2</v>
+        <v>0.1347902156764661</v>
       </c>
       <c r="G18">
-        <v>1.06544901065449E-2</v>
+        <v>0.18958653994151151</v>
       </c>
       <c r="H18">
-        <v>6.8721033906174785E-3</v>
+        <v>0.18353719344825822</v>
       </c>
       <c r="I18">
-        <v>1.3383397499030053E-2</v>
+        <v>0.12836507928947488</v>
       </c>
       <c r="J18">
-        <v>6.8134032678754683E-3</v>
+        <v>0.12535509016122517</v>
       </c>
       <c r="K18">
-        <v>8.974387151398696E-3</v>
+        <v>0.15416139825537606</v>
       </c>
       <c r="L18">
-        <v>1.0171012962918537E-2</v>
+        <v>0.21319901365069094</v>
       </c>
       <c r="M18">
-        <v>4.0275281549390085E-3</v>
+        <v>0.13556538436675425</v>
       </c>
       <c r="N18">
-        <v>5.4770281784942507E-3</v>
+        <v>0.1426745416205524</v>
       </c>
       <c r="O18">
-        <v>5.9193423561722108E-3</v>
+        <v>0.17089921406444017</v>
       </c>
       <c r="P18">
-        <v>5.7979529360833674E-3</v>
+        <v>0.18308207829936693</v>
       </c>
       <c r="Q18">
-        <v>5.9440758150922698E-3</v>
+        <v>0.21797454043557021</v>
       </c>
       <c r="R18">
-        <v>1.0672682178439969E-2</v>
+        <v>0.16178813238750592</v>
       </c>
       <c r="S18">
-        <v>1.3166338195431674E-2</v>
+        <v>0.11826549026371555</v>
       </c>
       <c r="T18">
-        <v>1.0273264456408587E-2</v>
+        <v>0.18320015783762453</v>
       </c>
       <c r="U18">
-        <v>1.1459284473580975E-2</v>
+        <v>0.11430375923833559</v>
       </c>
       <c r="V18">
-        <v>1.0273784895450284E-2</v>
+        <v>0.11225524213694742</v>
       </c>
       <c r="W18">
-        <v>1.1799059936493149E-2</v>
+        <v>0.1716829439171017</v>
       </c>
       <c r="X18">
-        <v>1.5180712412366853E-2</v>
+        <v>0.13069358514235713</v>
       </c>
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B19">
+        <v>0.58751816400088952</v>
+      </c>
+      <c r="C19">
+        <v>0.63195855763612019</v>
+      </c>
+      <c r="D19">
+        <v>0.84807034848805107</v>
+      </c>
+      <c r="E19">
+        <v>0.72468873612271401</v>
+      </c>
+      <c r="F19">
+        <v>0.70518756353607848</v>
+      </c>
+      <c r="G19">
+        <v>0.78226961776024206</v>
+      </c>
+      <c r="H19">
+        <v>0.81749754243287398</v>
       </c>
       <c r="I19">
-        <v>0.22831050228310501</v>
+        <v>0.88349648121868596</v>
       </c>
       <c r="J19">
-        <v>0.1906392694063927</v>
+        <v>0.95119319991890894</v>
       </c>
       <c r="K19">
-        <v>0.18647260273972602</v>
+        <v>0.92048229990249752</v>
       </c>
       <c r="L19">
-        <v>6.7876712328767116E-2</v>
+        <v>0.92005994960757642</v>
       </c>
       <c r="M19">
-        <v>7.476575935480044E-2</v>
+        <v>0.98431753019201262</v>
       </c>
       <c r="N19">
-        <v>9.6412405035707568E-2</v>
+        <v>0.94540432280661413</v>
       </c>
       <c r="O19">
-        <v>0.15293804193529958</v>
+        <v>0.81619276686525755</v>
       </c>
       <c r="P19">
-        <v>0.13941040865139273</v>
+        <v>0.91711461765215874</v>
       </c>
       <c r="Q19">
-        <v>0.1534278778672068</v>
+        <v>0.88913935610658323</v>
       </c>
       <c r="R19">
-        <v>0.15383140488540142</v>
+        <v>0.91556341739152636</v>
       </c>
       <c r="S19">
-        <v>0.15538589047072227</v>
+        <v>0.90218624426321981</v>
       </c>
       <c r="T19">
-        <v>0.14838111835914639</v>
+        <v>0.91672584775055033</v>
       </c>
       <c r="U19">
-        <v>0.15491400651998427</v>
+        <v>0.942110199083116</v>
       </c>
       <c r="V19">
-        <v>0.15239085998651261</v>
+        <v>0.94612082701666678</v>
       </c>
       <c r="W19">
-        <v>0.13133926069138591</v>
+        <v>0.9382181082323805</v>
       </c>
       <c r="X19">
-        <v>0.13764325363624622</v>
+        <v>0.93680249206717758</v>
       </c>
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>1.3728687025740881E-2</v>
+      </c>
+      <c r="C20">
+        <v>8.9246408872480296E-3</v>
+      </c>
+      <c r="D20">
+        <v>1.4064542368890371E-2</v>
+      </c>
+      <c r="E20">
+        <v>1.3440969291696423E-2</v>
+      </c>
+      <c r="F20">
+        <v>1.4367639360976603E-2</v>
+      </c>
+      <c r="G20">
+        <v>1.06544901065449E-2</v>
+      </c>
+      <c r="H20">
+        <v>6.8721033906174785E-3</v>
+      </c>
+      <c r="I20">
+        <v>1.3383397499030053E-2</v>
+      </c>
+      <c r="J20">
+        <v>6.8134032678754683E-3</v>
+      </c>
+      <c r="K20">
+        <v>8.974387151398696E-3</v>
+      </c>
+      <c r="L20">
+        <v>1.0171012962918537E-2</v>
+      </c>
+      <c r="M20">
+        <v>4.0275281549390085E-3</v>
+      </c>
+      <c r="N20">
+        <v>5.4770281784942507E-3</v>
+      </c>
+      <c r="O20">
+        <v>5.9193423561722108E-3</v>
+      </c>
+      <c r="P20">
+        <v>5.7979529360833674E-3</v>
+      </c>
+      <c r="Q20">
+        <v>5.9440758150922698E-3</v>
+      </c>
+      <c r="R20">
+        <v>1.0672682178439969E-2</v>
+      </c>
+      <c r="S20">
+        <v>1.3166338195431674E-2</v>
+      </c>
+      <c r="T20">
+        <v>1.0273264456408587E-2</v>
+      </c>
+      <c r="U20">
+        <v>1.1459284473580975E-2</v>
+      </c>
+      <c r="V20">
+        <v>1.0273784895450284E-2</v>
+      </c>
+      <c r="W20">
+        <v>1.1799059936493149E-2</v>
+      </c>
+      <c r="X20">
+        <v>1.5180712412366853E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="I21">
+        <v>0.22831050228310501</v>
+      </c>
+      <c r="J21">
+        <v>0.1906392694063927</v>
+      </c>
+      <c r="K21">
+        <v>0.18647260273972602</v>
+      </c>
+      <c r="L21">
+        <v>6.7876712328767116E-2</v>
+      </c>
+      <c r="M21">
+        <v>7.476575935480044E-2</v>
+      </c>
+      <c r="N21">
+        <v>9.6412405035707568E-2</v>
+      </c>
+      <c r="O21">
+        <v>0.15293804193529958</v>
+      </c>
+      <c r="P21">
+        <v>0.13941040865139273</v>
+      </c>
+      <c r="Q21">
+        <v>0.1534278778672068</v>
+      </c>
+      <c r="R21">
+        <v>0.15383140488540142</v>
+      </c>
+      <c r="S21">
+        <v>0.15538589047072227</v>
+      </c>
+      <c r="T21">
+        <v>0.14838111835914639</v>
+      </c>
+      <c r="U21">
+        <v>0.15491400651998427</v>
+      </c>
+      <c r="V21">
+        <v>0.15239085998651261</v>
+      </c>
+      <c r="W21">
+        <v>0.13133926069138591</v>
+      </c>
+      <c r="X21">
+        <v>0.13764325363624622</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>10</v>
       </c>
-      <c r="F20">
+      <c r="F22">
         <v>0.11415525114155251</v>
       </c>
-      <c r="G20">
+      <c r="G22">
         <v>6.5453767123287668E-2</v>
       </c>
-      <c r="H20">
+      <c r="H22">
         <v>8.4758159986470502E-2</v>
       </c>
-      <c r="I20">
+      <c r="I22">
         <v>0.17808980213089803</v>
       </c>
-      <c r="J20">
+      <c r="J22">
         <v>0.12192381639029079</v>
       </c>
-      <c r="K20">
+      <c r="K22">
         <v>8.1248714467892558E-2</v>
       </c>
-      <c r="L20">
+      <c r="L22">
         <v>0.15938903548169775</v>
       </c>
-      <c r="M20">
+      <c r="M22">
         <v>0.18169781142649755</v>
       </c>
-      <c r="N20">
+      <c r="N22">
         <v>0.2058669391554197</v>
       </c>
-      <c r="O20">
+      <c r="O22">
         <v>0.22956604290766625</v>
       </c>
-      <c r="P20">
+      <c r="P22">
         <v>0.2172995015710637</v>
       </c>
-      <c r="Q20">
+      <c r="Q22">
         <v>0.23704950320418605</v>
       </c>
-      <c r="R20">
+      <c r="R22">
         <v>0.23271503321770831</v>
       </c>
-      <c r="S20">
+      <c r="S22">
         <v>0.24584659524473154</v>
       </c>
-      <c r="T20">
+      <c r="T22">
         <v>0.21529025081619735</v>
       </c>
-      <c r="U20">
+      <c r="U22">
         <v>0.21381996798613462</v>
       </c>
-      <c r="V20">
+      <c r="V22">
         <v>0.23992922634315969</v>
       </c>
-      <c r="W20">
+      <c r="W22">
         <v>0.2323315222455867</v>
       </c>
-      <c r="X20">
+      <c r="X22">
         <v>0.24297964087912982</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>4</v>
-      </c>
-      <c r="B24">
-        <v>2000</v>
-      </c>
-      <c r="C24">
-        <v>2001</v>
-      </c>
-      <c r="D24">
-        <v>2002</v>
-      </c>
-      <c r="E24">
-        <v>2003</v>
-      </c>
-      <c r="F24">
-        <v>2004</v>
-      </c>
-      <c r="G24">
-        <v>2005</v>
-      </c>
-      <c r="H24">
-        <v>2006</v>
-      </c>
-      <c r="I24">
-        <v>2007</v>
-      </c>
-      <c r="J24">
-        <v>2008</v>
-      </c>
-      <c r="K24">
-        <v>2009</v>
-      </c>
-      <c r="L24">
-        <v>2010</v>
-      </c>
-      <c r="M24">
-        <v>2011</v>
-      </c>
-      <c r="N24">
-        <v>2012</v>
-      </c>
-      <c r="O24">
-        <v>2013</v>
-      </c>
-      <c r="P24">
-        <v>2014</v>
-      </c>
-      <c r="Q24">
-        <v>2015</v>
-      </c>
-      <c r="R24">
-        <v>2016</v>
-      </c>
-      <c r="S24">
-        <v>2017</v>
-      </c>
-      <c r="T24">
-        <v>2018</v>
-      </c>
-      <c r="U24">
-        <v>2019</v>
-      </c>
-      <c r="V24">
-        <v>2020</v>
-      </c>
-      <c r="W24">
-        <v>2021</v>
-      </c>
-      <c r="X24">
-        <v>2022</v>
-      </c>
-      <c r="Y24">
-        <v>2023</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>0.05</v>
-      </c>
-      <c r="C25">
-        <v>0.05</v>
-      </c>
-      <c r="D25">
-        <v>0.05</v>
-      </c>
-      <c r="E25">
-        <v>0.01</v>
-      </c>
-      <c r="F25">
-        <v>0.01</v>
-      </c>
-      <c r="G25">
-        <v>0.01</v>
-      </c>
-      <c r="H25">
-        <v>0.01</v>
-      </c>
-      <c r="I25">
-        <v>0.01</v>
-      </c>
-      <c r="J25">
-        <v>0.01</v>
-      </c>
-      <c r="K25">
-        <v>0.01</v>
-      </c>
-      <c r="L25">
-        <v>0.01</v>
-      </c>
-      <c r="M25">
-        <v>0.01</v>
-      </c>
-      <c r="N25">
-        <v>0.01</v>
-      </c>
-      <c r="O25">
-        <v>0.03</v>
-      </c>
-      <c r="P25">
-        <v>0.04</v>
-      </c>
-      <c r="Q25">
-        <v>0.05</v>
-      </c>
-      <c r="R25">
-        <v>0.06</v>
-      </c>
-      <c r="S25">
-        <v>0.05</v>
-      </c>
-      <c r="T25">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="U25">
-        <v>0.06</v>
-      </c>
-      <c r="V25">
-        <v>0.05</v>
-      </c>
-      <c r="W25">
-        <v>0.05</v>
-      </c>
-      <c r="X25">
-        <v>0.05</v>
-      </c>
-      <c r="Y25">
-        <v>0.05</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B26">
-        <v>5.62</v>
+        <v>2000</v>
       </c>
       <c r="C26">
-        <v>5.62</v>
+        <v>2001</v>
       </c>
       <c r="D26">
-        <v>5.62</v>
+        <v>2002</v>
       </c>
       <c r="E26">
-        <v>5.62</v>
+        <v>2003</v>
       </c>
       <c r="F26">
-        <v>5.5</v>
+        <v>2004</v>
       </c>
       <c r="G26">
-        <v>5.5</v>
+        <v>2005</v>
       </c>
       <c r="H26">
-        <v>5.5</v>
+        <v>2006</v>
       </c>
       <c r="I26">
-        <v>5.5</v>
+        <v>2007</v>
       </c>
       <c r="J26">
-        <v>5.5</v>
+        <v>2008</v>
       </c>
       <c r="K26">
-        <v>5.63</v>
+        <v>2009</v>
       </c>
       <c r="L26">
-        <v>5.63</v>
+        <v>2010</v>
       </c>
       <c r="M26">
-        <v>6.32</v>
+        <v>2011</v>
       </c>
       <c r="N26">
-        <v>6.32</v>
+        <v>2012</v>
       </c>
       <c r="O26">
-        <v>6.11</v>
+        <v>2013</v>
       </c>
       <c r="P26">
-        <v>5.9</v>
+        <v>2014</v>
       </c>
       <c r="Q26">
-        <v>5.0599999999999996</v>
+        <v>2015</v>
       </c>
       <c r="R26">
-        <v>5.0599999999999996</v>
+        <v>2016</v>
       </c>
       <c r="S26">
-        <v>5.1100000000000003</v>
+        <v>2017</v>
       </c>
       <c r="T26">
-        <v>5.1100000000000003</v>
+        <v>2018</v>
       </c>
       <c r="U26">
-        <v>5.1100000000000003</v>
+        <v>2019</v>
       </c>
       <c r="V26">
-        <v>5.1100000000000003</v>
+        <v>2020</v>
       </c>
       <c r="W26">
-        <v>5.1100000000000003</v>
+        <v>2021</v>
       </c>
       <c r="X26">
-        <v>5.1100000000000003</v>
+        <v>2022</v>
       </c>
       <c r="Y26">
-        <v>5.1100000000000003</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B27">
-        <v>1.1100000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="C27">
-        <v>1.1100000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="D27">
-        <v>1.1100000000000001</v>
+        <v>0.05</v>
       </c>
       <c r="E27">
-        <v>1.1100000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="F27">
-        <v>1.1100000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="G27">
-        <v>1.1100000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="H27">
-        <v>1.1100000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="I27">
-        <v>1.1499999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="J27">
-        <v>1.1499999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="K27">
-        <v>1.1499999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="L27">
-        <v>1.1499999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="M27">
-        <v>1.2</v>
+        <v>0.01</v>
       </c>
       <c r="N27">
-        <v>1.2</v>
+        <v>0.01</v>
       </c>
       <c r="O27">
-        <v>1.2</v>
+        <v>0.03</v>
       </c>
       <c r="P27">
-        <v>1.2</v>
+        <v>0.04</v>
       </c>
       <c r="Q27">
-        <v>1.2</v>
+        <v>0.05</v>
       </c>
       <c r="R27">
-        <v>1.2</v>
+        <v>0.06</v>
       </c>
       <c r="S27">
-        <v>1.2</v>
+        <v>0.05</v>
       </c>
       <c r="T27">
-        <v>1.2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="U27">
-        <v>1.2</v>
+        <v>0.06</v>
       </c>
       <c r="V27">
-        <v>1.2</v>
+        <v>0.05</v>
       </c>
       <c r="W27">
-        <v>1.2</v>
+        <v>0.05</v>
       </c>
       <c r="X27">
-        <v>1.2</v>
+        <v>0.05</v>
       </c>
       <c r="Y27">
-        <v>1.2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B28">
-        <v>1.02</v>
+        <v>5.62</v>
       </c>
       <c r="C28">
-        <v>0.84</v>
+        <v>5.62</v>
       </c>
       <c r="D28">
-        <v>1.08</v>
+        <v>5.62</v>
       </c>
       <c r="E28">
-        <v>1.65</v>
+        <v>5.62</v>
       </c>
       <c r="F28">
-        <v>1.98</v>
+        <v>5.5</v>
       </c>
       <c r="G28">
-        <v>1.98</v>
+        <v>5.5</v>
       </c>
       <c r="H28">
-        <v>1.98</v>
+        <v>5.5</v>
       </c>
       <c r="I28">
-        <v>2.0099999999999998</v>
+        <v>5.5</v>
       </c>
       <c r="J28">
-        <v>2.12</v>
+        <v>5.5</v>
       </c>
       <c r="K28">
-        <v>2.14</v>
+        <v>5.63</v>
       </c>
       <c r="L28">
-        <v>2.1800000000000002</v>
+        <v>5.63</v>
       </c>
       <c r="M28">
-        <v>2.2400000000000002</v>
+        <v>6.32</v>
       </c>
       <c r="N28">
-        <v>2.3199999999999998</v>
+        <v>6.32</v>
       </c>
       <c r="O28">
-        <v>2.34</v>
+        <v>6.11</v>
       </c>
       <c r="P28">
-        <v>2.36</v>
+        <v>5.9</v>
       </c>
       <c r="Q28">
-        <v>2.36</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="R28">
-        <v>2.36</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="S28">
-        <v>2.5099999999999998</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="T28">
-        <v>2.5099999999999998</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="U28">
-        <v>2.5099999999999998</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="V28">
-        <v>2.5099999999999998</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="W28">
-        <v>2.5099999999999998</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="X28">
-        <v>2.5299999999999998</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="Y28">
-        <v>2.5299999999999998</v>
+        <v>5.1100000000000003</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B29">
-        <v>3.53</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="C29">
-        <v>3.53</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="D29">
-        <v>2.72</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="E29">
-        <v>2.72</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="F29">
-        <v>2.72</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="G29">
-        <v>2.72</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="H29">
-        <v>2.72</v>
+        <v>1.1100000000000001</v>
       </c>
       <c r="I29">
-        <v>1.89</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="J29">
-        <v>1.89</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="K29">
-        <v>1.89</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="L29">
-        <v>1.89</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="M29">
-        <v>1.89</v>
+        <v>1.2</v>
       </c>
       <c r="N29">
-        <v>1.91</v>
+        <v>1.2</v>
       </c>
       <c r="O29">
-        <v>1.98</v>
+        <v>1.2</v>
       </c>
       <c r="P29">
-        <v>1.98</v>
+        <v>1.2</v>
       </c>
       <c r="Q29">
-        <v>1.98</v>
+        <v>1.2</v>
       </c>
       <c r="R29">
-        <v>1.97</v>
+        <v>1.2</v>
       </c>
       <c r="S29">
-        <v>1.97</v>
+        <v>1.2</v>
       </c>
       <c r="T29">
-        <v>2.0099999999999998</v>
+        <v>1.2</v>
       </c>
       <c r="U29">
-        <v>2.0099999999999998</v>
+        <v>1.2</v>
       </c>
       <c r="V29">
-        <v>2.0099999999999998</v>
+        <v>1.2</v>
       </c>
       <c r="W29">
-        <v>2.0099999999999998</v>
+        <v>1.2</v>
       </c>
       <c r="X29">
-        <v>2.0099999999999998</v>
+        <v>1.2</v>
       </c>
       <c r="Y29">
-        <v>2.0099999999999998</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>1.02</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.84</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1.08</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>1.65</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>1.98</v>
       </c>
       <c r="G30">
-        <v>0</v>
+        <v>1.98</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>1.98</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>2.12</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>2.14</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>2.1800000000000002</v>
       </c>
       <c r="M30">
-        <v>0</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="N30">
-        <v>0</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="O30">
-        <v>0</v>
+        <v>2.34</v>
       </c>
       <c r="P30">
-        <v>0</v>
+        <v>2.36</v>
       </c>
       <c r="Q30">
-        <v>0</v>
+        <v>2.36</v>
       </c>
       <c r="R30">
-        <v>0</v>
+        <v>2.36</v>
       </c>
       <c r="S30">
-        <v>0</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="T30">
-        <v>0</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="U30">
-        <v>0</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="V30">
-        <v>0</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="W30">
-        <v>0</v>
+        <v>2.5099999999999998</v>
       </c>
       <c r="X30">
-        <v>0</v>
+        <v>2.5299999999999998</v>
       </c>
       <c r="Y30">
-        <v>0</v>
+        <v>2.5299999999999998</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>3.53</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>3.53</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>2.72</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>2.72</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>2.72</v>
       </c>
       <c r="G31">
-        <v>0</v>
+        <v>2.72</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>2.72</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1.89</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1.89</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>1.89</v>
       </c>
       <c r="L31">
-        <v>0.03</v>
+        <v>1.89</v>
       </c>
       <c r="M31">
-        <v>0.15</v>
+        <v>1.89</v>
       </c>
       <c r="N31">
-        <v>0.92</v>
+        <v>1.91</v>
       </c>
       <c r="O31">
-        <v>1.04</v>
+        <v>1.98</v>
       </c>
       <c r="P31">
-        <v>1.03</v>
+        <v>1.98</v>
       </c>
       <c r="Q31">
-        <v>1.03</v>
+        <v>1.98</v>
       </c>
       <c r="R31">
-        <v>1.03</v>
+        <v>1.97</v>
       </c>
       <c r="S31">
-        <v>1.03</v>
+        <v>1.97</v>
       </c>
       <c r="T31">
-        <v>1.03</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="U31">
-        <v>1.04</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="V31">
-        <v>1.1000000000000001</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="W31">
-        <v>1.27</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="X31">
-        <v>1.74</v>
+        <v>2.0099999999999998</v>
       </c>
       <c r="Y31">
-        <v>2.94</v>
+        <v>2.0099999999999998</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+      <c r="J32">
+        <v>0</v>
+      </c>
+      <c r="K32">
+        <v>0</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
+      </c>
+      <c r="M32">
+        <v>0</v>
+      </c>
+      <c r="N32">
+        <v>0</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>0</v>
+      </c>
+      <c r="U32">
+        <v>0</v>
+      </c>
+      <c r="V32">
+        <v>0</v>
+      </c>
+      <c r="W32">
+        <v>0</v>
+      </c>
+      <c r="X32">
+        <v>0</v>
+      </c>
+      <c r="Y32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>0</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>0</v>
+      </c>
+      <c r="L33">
+        <v>0.03</v>
+      </c>
+      <c r="M33">
+        <v>0.15</v>
+      </c>
+      <c r="N33">
+        <v>0.92</v>
+      </c>
+      <c r="O33">
+        <v>1.04</v>
+      </c>
+      <c r="P33">
+        <v>1.03</v>
+      </c>
+      <c r="Q33">
+        <v>1.03</v>
+      </c>
+      <c r="R33">
+        <v>1.03</v>
+      </c>
+      <c r="S33">
+        <v>1.03</v>
+      </c>
+      <c r="T33">
+        <v>1.03</v>
+      </c>
+      <c r="U33">
+        <v>1.04</v>
+      </c>
+      <c r="V33">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W33">
+        <v>1.27</v>
+      </c>
+      <c r="X33">
+        <v>1.74</v>
+      </c>
+      <c r="Y33">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
         <v>10</v>
       </c>
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-      <c r="D32">
-        <v>0</v>
-      </c>
-      <c r="E32">
-        <v>0</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-      <c r="G32">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>0</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
         <v>0.01</v>
       </c>
-      <c r="H32">
+      <c r="H34">
         <v>0.03</v>
       </c>
-      <c r="I32">
+      <c r="I34">
         <v>0.03</v>
       </c>
-      <c r="J32">
+      <c r="J34">
         <v>0.11</v>
       </c>
-      <c r="K32">
+      <c r="K34">
         <v>0.33</v>
       </c>
-      <c r="L32">
+      <c r="L34">
         <v>0.49</v>
       </c>
-      <c r="M32">
+      <c r="M34">
         <v>0.54</v>
       </c>
-      <c r="N32">
+      <c r="N34">
         <v>0.68</v>
       </c>
-      <c r="O32">
+      <c r="O34">
         <v>0.68</v>
       </c>
-      <c r="P32">
+      <c r="P34">
         <v>0.7</v>
       </c>
-      <c r="Q32">
+      <c r="Q34">
         <v>0.7</v>
       </c>
-      <c r="R32">
+      <c r="R34">
         <v>0.7</v>
       </c>
-      <c r="S32">
+      <c r="S34">
         <v>0.7</v>
       </c>
-      <c r="T32">
+      <c r="T34">
         <v>0.7</v>
       </c>
-      <c r="U32">
+      <c r="U34">
         <v>0.7</v>
       </c>
-      <c r="V32">
+      <c r="V34">
         <v>0.7</v>
       </c>
-      <c r="W32">
+      <c r="W34">
         <v>0.7</v>
       </c>
-      <c r="X32">
+      <c r="X34">
         <v>0.7</v>
       </c>
-      <c r="Y32">
+      <c r="Y34">
         <v>0.7</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B36">
+      <c r="B38">
         <v>2000</v>
       </c>
-      <c r="C36">
+      <c r="C38">
         <v>2001</v>
       </c>
-      <c r="D36">
+      <c r="D38">
         <v>2002</v>
       </c>
-      <c r="E36">
+      <c r="E38">
         <v>2003</v>
       </c>
-      <c r="F36">
+      <c r="F38">
         <v>2004</v>
       </c>
-      <c r="G36">
+      <c r="G38">
         <v>2005</v>
       </c>
-      <c r="H36">
+      <c r="H38">
         <v>2006</v>
       </c>
-      <c r="I36">
+      <c r="I38">
         <v>2007</v>
       </c>
-      <c r="J36">
+      <c r="J38">
         <v>2008</v>
       </c>
-      <c r="K36">
+      <c r="K38">
         <v>2009</v>
       </c>
-      <c r="L36">
+      <c r="L38">
         <v>2010</v>
       </c>
-      <c r="M36">
+      <c r="M38">
         <v>2011</v>
       </c>
-      <c r="N36">
+      <c r="N38">
         <v>2012</v>
       </c>
-      <c r="O36">
+      <c r="O38">
         <v>2013</v>
       </c>
-      <c r="P36">
+      <c r="P38">
         <v>2014</v>
       </c>
-      <c r="Q36">
+      <c r="Q38">
         <v>2015</v>
       </c>
-      <c r="R36">
+      <c r="R38">
         <v>2016</v>
       </c>
-      <c r="S36">
+      <c r="S38">
         <v>2017</v>
       </c>
-      <c r="T36">
+      <c r="T38">
         <v>2018</v>
       </c>
-      <c r="U36">
+      <c r="U38">
         <v>2019</v>
       </c>
-      <c r="V36">
+      <c r="V38">
         <v>2020</v>
       </c>
-      <c r="W36">
+      <c r="W38">
         <v>2021</v>
       </c>
-      <c r="X36">
+      <c r="X38">
         <v>2022</v>
       </c>
-      <c r="Y36">
+      <c r="Y38">
         <v>2023</v>
       </c>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37">
-        <v>0</v>
-      </c>
-      <c r="C37">
-        <v>0</v>
-      </c>
-      <c r="D37">
-        <v>0</v>
-      </c>
-      <c r="E37">
-        <v>0</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
-      <c r="H37">
-        <v>0</v>
-      </c>
-      <c r="I37">
-        <v>0</v>
-      </c>
-      <c r="J37">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39">
+        <v>0</v>
+      </c>
+      <c r="J39">
         <v>0.02</v>
       </c>
-      <c r="K37">
+      <c r="K39">
         <v>0.01</v>
       </c>
-      <c r="L37">
+      <c r="L39">
         <v>0.04</v>
       </c>
-      <c r="M37">
+      <c r="M39">
         <v>0.06</v>
       </c>
-      <c r="N37">
+      <c r="N39">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O37">
+      <c r="O39">
         <v>0.11</v>
       </c>
-      <c r="P37">
+      <c r="P39">
         <v>0.2</v>
       </c>
-      <c r="Q37">
+      <c r="Q39">
         <v>0.27</v>
       </c>
-      <c r="R37">
+      <c r="R39">
         <v>0.35</v>
       </c>
-      <c r="S37">
+      <c r="S39">
         <v>0.4</v>
       </c>
-      <c r="T37">
+      <c r="T39">
         <v>1.57</v>
       </c>
-      <c r="U37">
+      <c r="U39">
         <v>1.82</v>
       </c>
-      <c r="V37">
+      <c r="V39">
         <v>1.7</v>
       </c>
-      <c r="W37">
+      <c r="W39">
         <v>2.59</v>
       </c>
-      <c r="X37">
+      <c r="X39">
         <v>2.2400000000000002</v>
       </c>
-      <c r="Y37">
+      <c r="Y39">
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>1</v>
       </c>
-      <c r="B38">
+      <c r="B40">
         <v>16.940000000000001</v>
       </c>
-      <c r="C38">
+      <c r="C40">
         <v>19.5</v>
       </c>
-      <c r="D38">
+      <c r="D40">
         <v>17.18</v>
       </c>
-      <c r="E38">
+      <c r="E40">
         <v>19.239999999999998</v>
       </c>
-      <c r="F38">
+      <c r="F40">
         <v>18.899999999999999</v>
       </c>
-      <c r="G38">
+      <c r="G40">
         <v>18.46</v>
       </c>
-      <c r="H38">
+      <c r="H40">
         <v>19.09</v>
       </c>
-      <c r="I38">
+      <c r="I40">
         <v>22.37</v>
       </c>
-      <c r="J38">
+      <c r="J40">
         <v>23.18</v>
       </c>
-      <c r="K38">
+      <c r="K40">
         <v>21.1</v>
       </c>
-      <c r="L38">
+      <c r="L40">
         <v>22.61</v>
       </c>
-      <c r="M38">
+      <c r="M40">
         <v>27.53</v>
       </c>
-      <c r="N38">
+      <c r="N40">
         <v>22.87</v>
       </c>
-      <c r="O38">
+      <c r="O40">
         <v>19.39</v>
       </c>
-      <c r="P38">
+      <c r="P40">
         <v>21.31</v>
       </c>
-      <c r="Q38">
+      <c r="Q40">
         <v>22.53</v>
       </c>
-      <c r="R38">
+      <c r="R40">
         <v>19.37</v>
       </c>
-      <c r="S38">
+      <c r="S40">
         <v>20.92</v>
       </c>
-      <c r="T38">
+      <c r="T40">
         <v>18.66</v>
       </c>
-      <c r="U38">
+      <c r="U40">
         <v>17.2</v>
       </c>
-      <c r="V38">
+      <c r="V40">
         <v>13.51</v>
       </c>
-      <c r="W38">
+      <c r="W40">
         <v>17.09</v>
       </c>
-      <c r="X38">
+      <c r="X40">
         <v>21.79</v>
       </c>
-      <c r="Y38">
+      <c r="Y40">
         <v>11.56</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>2</v>
       </c>
-      <c r="B39">
+      <c r="B41">
         <v>1.91</v>
       </c>
-      <c r="C39">
+      <c r="C41">
         <v>1.91</v>
       </c>
-      <c r="D39">
+      <c r="D41">
         <v>1.54</v>
       </c>
-      <c r="E39">
+      <c r="E41">
         <v>1.76</v>
       </c>
-      <c r="F39">
+      <c r="F41">
         <v>1.49</v>
       </c>
-      <c r="G39">
+      <c r="G41">
         <v>1.73</v>
       </c>
-      <c r="H39">
+      <c r="H41">
         <v>2.16</v>
       </c>
-      <c r="I39">
+      <c r="I41">
         <v>2.34</v>
       </c>
-      <c r="J39">
+      <c r="J41">
         <v>2.36</v>
       </c>
-      <c r="K39">
+      <c r="K41">
         <v>1.96</v>
       </c>
-      <c r="L39">
+      <c r="L41">
         <v>1.97</v>
       </c>
-      <c r="M39">
+      <c r="M41">
         <v>2.08</v>
       </c>
-      <c r="N39">
+      <c r="N41">
         <v>2.36</v>
       </c>
-      <c r="O39">
+      <c r="O41">
         <v>2.34</v>
       </c>
-      <c r="P39">
+      <c r="P41">
         <v>2.14</v>
       </c>
-      <c r="Q39">
+      <c r="Q41">
         <v>1.86</v>
       </c>
-      <c r="R39">
+      <c r="R41">
         <v>2.0499999999999998</v>
       </c>
-      <c r="S39">
+      <c r="S41">
         <v>1.93</v>
       </c>
-      <c r="T39">
+      <c r="T41">
         <v>2.02</v>
       </c>
-      <c r="U39">
+      <c r="U41">
         <v>2.15</v>
       </c>
-      <c r="V39">
+      <c r="V41">
         <v>2.29</v>
       </c>
-      <c r="W39">
+      <c r="W41">
         <v>3.05</v>
       </c>
-      <c r="X39">
+      <c r="X41">
         <v>2.0499999999999998</v>
       </c>
-      <c r="Y39">
+      <c r="Y41">
         <v>1.56</v>
       </c>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>7</v>
       </c>
-      <c r="B40">
+      <c r="B42">
         <v>2.63</v>
       </c>
-      <c r="C40">
+      <c r="C42">
         <v>1.65</v>
       </c>
-      <c r="D40">
+      <c r="D42">
         <v>2.12</v>
       </c>
-      <c r="E40">
+      <c r="E42">
         <v>2.99</v>
       </c>
-      <c r="F40">
+      <c r="F42">
         <v>3.14</v>
       </c>
-      <c r="G40">
+      <c r="G42">
         <v>4.3</v>
       </c>
-      <c r="H40">
+      <c r="H42">
         <v>4.21</v>
       </c>
-      <c r="I40">
+      <c r="I42">
         <v>2.83</v>
       </c>
-      <c r="J40">
+      <c r="J42">
         <v>2.79</v>
       </c>
-      <c r="K40">
+      <c r="K42">
         <v>3.43</v>
       </c>
-      <c r="L40">
+      <c r="L42">
         <v>5.03</v>
       </c>
-      <c r="M40">
+      <c r="M42">
         <v>2.87</v>
       </c>
-      <c r="N40">
+      <c r="N42">
         <v>3.18</v>
       </c>
-      <c r="O40">
+      <c r="O42">
         <v>4.04</v>
       </c>
-      <c r="P40">
+      <c r="P42">
         <v>4.5999999999999996</v>
       </c>
-      <c r="Q40">
+      <c r="Q42">
         <v>5.65</v>
       </c>
-      <c r="R40">
+      <c r="R42">
         <v>3.88</v>
       </c>
-      <c r="S40">
+      <c r="S42">
         <v>2.83</v>
       </c>
-      <c r="T40">
+      <c r="T42">
         <v>5.15</v>
       </c>
-      <c r="U40">
+      <c r="U42">
         <v>2.93</v>
       </c>
-      <c r="V40">
+      <c r="V42">
         <v>2.82</v>
       </c>
-      <c r="W40">
+      <c r="W42">
         <v>4.82</v>
       </c>
-      <c r="X40">
+      <c r="X42">
         <v>3.8</v>
       </c>
-      <c r="Y40">
+      <c r="Y42">
         <v>3.11</v>
       </c>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>8</v>
       </c>
-      <c r="B41">
+      <c r="B43">
         <v>18.18</v>
       </c>
-      <c r="C41">
+      <c r="C43">
         <v>19.55</v>
       </c>
-      <c r="D41">
+      <c r="D43">
         <v>20.22</v>
       </c>
-      <c r="E41">
+      <c r="E43">
         <v>17.28</v>
       </c>
-      <c r="F41">
+      <c r="F43">
         <v>16.82</v>
       </c>
-      <c r="G41">
+      <c r="G43">
         <v>18.649999999999999</v>
       </c>
-      <c r="H41">
+      <c r="H43">
         <v>19.489999999999998</v>
       </c>
-      <c r="I41">
+      <c r="I43">
         <v>14.64</v>
       </c>
-      <c r="J41">
+      <c r="J43">
         <v>15.77</v>
       </c>
-      <c r="K41">
+      <c r="K43">
         <v>15.26</v>
       </c>
-      <c r="L41">
+      <c r="L43">
         <v>15.25</v>
       </c>
-      <c r="M41">
+      <c r="M43">
         <v>16.309999999999999</v>
       </c>
-      <c r="N41">
+      <c r="N43">
         <v>15.78</v>
       </c>
-      <c r="O41">
+      <c r="O43">
         <v>14.17</v>
       </c>
-      <c r="P41">
+      <c r="P43">
         <v>15.87</v>
       </c>
-      <c r="Q41">
+      <c r="Q43">
         <v>15.38</v>
       </c>
-      <c r="R41">
+      <c r="R43">
         <v>15.78</v>
       </c>
-      <c r="S41">
+      <c r="S43">
         <v>15.55</v>
       </c>
-      <c r="T41">
+      <c r="T43">
         <v>16.13</v>
       </c>
-      <c r="U41">
+      <c r="U43">
         <v>16.559999999999999</v>
       </c>
-      <c r="V41">
+      <c r="V43">
         <v>16.63</v>
       </c>
-      <c r="W41">
+      <c r="W43">
         <v>16.489999999999998</v>
       </c>
-      <c r="X41">
+      <c r="X43">
         <v>16.46</v>
       </c>
-      <c r="Y41">
+      <c r="Y43">
         <v>16.16</v>
       </c>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>3</v>
       </c>
-      <c r="B42">
+      <c r="B44">
         <v>0.93</v>
       </c>
-      <c r="C42">
+      <c r="C44">
         <v>0.83</v>
       </c>
-      <c r="D42">
+      <c r="D44">
         <v>1.02</v>
       </c>
-      <c r="E42">
+      <c r="E44">
         <v>1.01</v>
       </c>
-      <c r="F42">
+      <c r="F44">
         <v>1.01</v>
       </c>
-      <c r="G42">
+      <c r="G44">
         <v>0.75</v>
       </c>
-      <c r="H42">
+      <c r="H44">
         <v>0.47</v>
       </c>
-      <c r="I42">
+      <c r="I44">
         <v>0.59</v>
       </c>
-      <c r="J42">
+      <c r="J44">
         <v>0.25</v>
       </c>
-      <c r="K42">
+      <c r="K44">
         <v>0.31</v>
       </c>
-      <c r="L42">
+      <c r="L44">
         <v>0.34</v>
       </c>
-      <c r="M42">
+      <c r="M44">
         <v>0.15</v>
       </c>
-      <c r="N42">
+      <c r="N44">
         <v>0.2</v>
       </c>
-      <c r="O42">
+      <c r="O44">
         <v>0.21</v>
       </c>
-      <c r="P42">
+      <c r="P44">
         <v>0.21</v>
       </c>
-      <c r="Q42">
+      <c r="Q44">
         <v>0.19</v>
       </c>
-      <c r="R42">
+      <c r="R44">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S42">
+      <c r="S44">
         <v>0.31</v>
       </c>
-      <c r="T42">
+      <c r="T44">
         <v>0.32</v>
       </c>
-      <c r="U42">
+      <c r="U44">
         <v>0.32</v>
       </c>
-      <c r="V42">
+      <c r="V44">
         <v>0.24</v>
       </c>
-      <c r="W42">
+      <c r="W44">
         <v>0.28000000000000003</v>
       </c>
-      <c r="X42">
+      <c r="X44">
         <v>0.35</v>
       </c>
-      <c r="Y42">
+      <c r="Y44">
         <v>0.35</v>
       </c>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
         <v>9</v>
       </c>
-      <c r="B43">
-        <v>0</v>
-      </c>
-      <c r="C43">
-        <v>0</v>
-      </c>
-      <c r="D43">
-        <v>0</v>
-      </c>
-      <c r="E43">
-        <v>0</v>
-      </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <v>0</v>
-      </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
-        <v>0</v>
-      </c>
-      <c r="K43">
-        <v>0</v>
-      </c>
-      <c r="L43">
+      <c r="B45">
+        <v>0</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
         <v>0.01</v>
       </c>
-      <c r="M43">
+      <c r="M45">
         <v>0.1</v>
       </c>
-      <c r="N43">
+      <c r="N45">
         <v>0.78</v>
       </c>
-      <c r="O43">
+      <c r="O45">
         <v>1.39</v>
       </c>
-      <c r="P43">
+      <c r="P45">
         <v>1.26</v>
       </c>
-      <c r="Q43">
+      <c r="Q45">
         <v>1.38</v>
       </c>
-      <c r="R43">
+      <c r="R45">
         <v>1.39</v>
       </c>
-      <c r="S43">
+      <c r="S45">
         <v>1.4</v>
       </c>
-      <c r="T43">
+      <c r="T45">
         <v>1.34</v>
       </c>
-      <c r="U43">
+      <c r="U45">
         <v>1.42</v>
       </c>
-      <c r="V43">
+      <c r="V45">
         <v>1.47</v>
       </c>
-      <c r="W43">
+      <c r="W45">
         <v>1.47</v>
       </c>
-      <c r="X43">
+      <c r="X45">
         <v>2.09</v>
       </c>
-      <c r="Y43">
+      <c r="Y45">
         <v>3.52</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>10</v>
       </c>
-      <c r="B44">
-        <v>0</v>
-      </c>
-      <c r="C44">
-        <v>0</v>
-      </c>
-      <c r="D44">
-        <v>0</v>
-      </c>
-      <c r="E44">
-        <v>0</v>
-      </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
+      <c r="B46">
+        <v>0</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
         <v>0.02</v>
       </c>
-      <c r="I44">
+      <c r="I46">
         <v>0.05</v>
       </c>
-      <c r="J44">
+      <c r="J46">
         <v>0.12</v>
       </c>
-      <c r="K44">
+      <c r="K46">
         <v>0.24</v>
       </c>
-      <c r="L44">
+      <c r="L46">
         <v>0.68</v>
       </c>
-      <c r="M44">
+      <c r="M46">
         <v>0.86</v>
       </c>
-      <c r="N44">
+      <c r="N46">
         <v>1.22</v>
       </c>
-      <c r="O44">
+      <c r="O46">
         <v>1.37</v>
       </c>
-      <c r="P44">
+      <c r="P46">
         <v>1.33</v>
       </c>
-      <c r="Q44">
+      <c r="Q46">
         <v>1.45</v>
       </c>
-      <c r="R44">
+      <c r="R46">
         <v>1.42</v>
       </c>
-      <c r="S44">
+      <c r="S46">
         <v>1.5</v>
       </c>
-      <c r="T44">
+      <c r="T46">
         <v>1.32</v>
       </c>
-      <c r="U44">
+      <c r="U46">
         <v>1.32</v>
       </c>
-      <c r="V44">
+      <c r="V46">
         <v>1.48</v>
       </c>
-      <c r="W44">
+      <c r="W46">
         <v>1.43</v>
       </c>
-      <c r="X44">
+      <c r="X46">
         <v>1.44</v>
       </c>
-      <c r="Y44">
+      <c r="Y46">
         <v>1.55</v>
-      </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>4</v>
-      </c>
-      <c r="B48">
-        <v>2000</v>
-      </c>
-      <c r="C48">
-        <v>2001</v>
-      </c>
-      <c r="D48">
-        <v>2002</v>
-      </c>
-      <c r="E48">
-        <v>2003</v>
-      </c>
-      <c r="F48">
-        <v>2004</v>
-      </c>
-      <c r="G48">
-        <v>2005</v>
-      </c>
-      <c r="H48">
-        <v>2006</v>
-      </c>
-      <c r="I48">
-        <v>2007</v>
-      </c>
-      <c r="J48">
-        <v>2008</v>
-      </c>
-      <c r="K48">
-        <v>2009</v>
-      </c>
-      <c r="L48">
-        <v>2010</v>
-      </c>
-      <c r="M48">
-        <v>2011</v>
-      </c>
-      <c r="N48">
-        <v>2012</v>
-      </c>
-      <c r="O48">
-        <v>2013</v>
-      </c>
-      <c r="P48">
-        <v>2014</v>
-      </c>
-      <c r="Q48">
-        <v>2015</v>
-      </c>
-      <c r="R48">
-        <v>2016</v>
-      </c>
-      <c r="S48">
-        <v>2017</v>
-      </c>
-      <c r="T48">
-        <v>2018</v>
-      </c>
-      <c r="U48">
-        <v>2019</v>
-      </c>
-      <c r="V48">
-        <v>2020</v>
-      </c>
-      <c r="W48">
-        <v>2021</v>
-      </c>
-      <c r="X48">
-        <v>2022</v>
-      </c>
-      <c r="Y48">
-        <v>2023</v>
-      </c>
-      <c r="Z48">
-        <v>2024</v>
       </c>
     </row>
     <row r="49" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B49">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="C49">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="D49">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="E49">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="F49">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="G49">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="H49">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="I49">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="J49">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="K49">
-        <v>9.0000000000000011E-3</v>
-      </c>
-      <c r="L49">
-        <v>0.01</v>
-      </c>
-      <c r="M49">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="N49">
-        <v>1.4E-2</v>
-      </c>
-      <c r="O49">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="P49">
-        <v>0.04</v>
-      </c>
-      <c r="Q49">
-        <v>5.4000000000000006E-2</v>
-      </c>
-      <c r="R49">
-        <v>5.6999999999999995E-2</v>
-      </c>
-      <c r="S49">
-        <v>5.2003000000000001E-2</v>
-      </c>
-      <c r="T49">
-        <v>6.942799999999999E-2</v>
-      </c>
-      <c r="U49">
-        <v>5.6869000000000003E-2</v>
-      </c>
-      <c r="V49">
-        <v>4.8054000000000006E-2</v>
-      </c>
-      <c r="W49">
-        <v>4.7321000000000002E-2</v>
-      </c>
-      <c r="X49">
-        <v>7.8688999999999995E-2</v>
-      </c>
-      <c r="Y49">
-        <v>7.8688999999999995E-2</v>
-      </c>
-      <c r="Z49">
-        <v>7.8688999999999995E-2</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B50">
-        <v>1.88</v>
+        <v>2000</v>
       </c>
       <c r="C50">
-        <v>1.7050000000000001</v>
+        <v>2001</v>
       </c>
       <c r="D50">
-        <v>1.948</v>
+        <v>2002</v>
       </c>
       <c r="E50">
-        <v>2.5150000000000001</v>
+        <v>2003</v>
       </c>
       <c r="F50">
-        <v>2.8479999999999999</v>
+        <v>2004</v>
       </c>
       <c r="G50">
-        <v>2.8479999999999999</v>
+        <v>2005</v>
       </c>
       <c r="H50">
-        <v>2.8479999999999999</v>
+        <v>2006</v>
       </c>
       <c r="I50">
-        <v>2.8759999999999999</v>
+        <v>2007</v>
       </c>
       <c r="J50">
-        <v>2.984</v>
+        <v>2008</v>
       </c>
       <c r="K50">
-        <v>3.0009999999999999</v>
+        <v>2009</v>
       </c>
       <c r="L50">
-        <v>3.048</v>
+        <v>2010</v>
       </c>
       <c r="M50">
-        <v>3.1080000000000001</v>
+        <v>2011</v>
       </c>
       <c r="N50">
-        <v>3.181</v>
+        <v>2012</v>
       </c>
       <c r="O50">
-        <v>3.2029999999999998</v>
+        <v>2013</v>
       </c>
       <c r="P50">
-        <v>3.2189999999999999</v>
+        <v>2014</v>
       </c>
       <c r="Q50">
-        <v>3.2189999999999999</v>
+        <v>2015</v>
       </c>
       <c r="R50">
-        <v>3.2229999999999999</v>
+        <v>2016</v>
       </c>
       <c r="S50">
-        <v>3.37155</v>
+        <v>2017</v>
       </c>
       <c r="T50">
-        <v>3.379</v>
+        <v>2018</v>
       </c>
       <c r="U50">
-        <v>3.3783499999999997</v>
+        <v>2019</v>
       </c>
       <c r="V50">
-        <v>3.3764560000000001</v>
+        <v>2020</v>
       </c>
       <c r="W50">
-        <v>3.3692329999999999</v>
+        <v>2021</v>
       </c>
       <c r="X50">
-        <v>3.348185</v>
+        <v>2022</v>
       </c>
       <c r="Y50">
-        <v>3.3502800000000001</v>
+        <v>2023</v>
       </c>
       <c r="Z50">
-        <v>3.3502800000000001</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B51">
-        <v>3.532</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="C51">
-        <v>3.532</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="D51">
-        <v>2.722</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="E51">
-        <v>2.722</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F51">
-        <v>2.722</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G51">
-        <v>2.722</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H51">
-        <v>2.722</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I51">
-        <v>1.8919999999999999</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="J51">
-        <v>1.8919999999999999</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="K51">
-        <v>1.8919999999999999</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="L51">
-        <v>1.8919999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="M51">
-        <v>1.8919999999999999</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N51">
-        <v>1.9059999999999999</v>
+        <v>1.4E-2</v>
       </c>
       <c r="O51">
-        <v>1.982</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="P51">
-        <v>1.9750000000000001</v>
+        <v>0.04</v>
       </c>
       <c r="Q51">
-        <v>1.9750000000000001</v>
+        <v>5.4000000000000006E-2</v>
       </c>
       <c r="R51">
-        <v>1.9670000000000001</v>
+        <v>5.6999999999999995E-2</v>
       </c>
       <c r="S51">
-        <v>1.9670000000000001</v>
+        <v>5.2003000000000001E-2</v>
       </c>
       <c r="T51">
-        <v>2.008</v>
+        <v>6.942799999999999E-2</v>
       </c>
       <c r="U51">
-        <v>2.0059999999999998</v>
+        <v>5.6869000000000003E-2</v>
       </c>
       <c r="V51">
-        <v>2.0059999999999998</v>
+        <v>4.8054000000000006E-2</v>
       </c>
       <c r="W51">
-        <v>2.0059999999999998</v>
+        <v>4.7321000000000002E-2</v>
       </c>
       <c r="X51">
-        <v>2.0059999999999998</v>
+        <v>7.8688999999999995E-2</v>
       </c>
       <c r="Y51">
-        <v>2.0059999999999998</v>
+        <v>7.8688999999999995E-2</v>
       </c>
       <c r="Z51">
-        <v>2.0059999999999998</v>
+        <v>7.8688999999999995E-2</v>
       </c>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B52">
-        <v>5.6210000000000004</v>
+        <v>1.88</v>
       </c>
       <c r="C52">
-        <v>7.4059999999999997</v>
+        <v>1.7050000000000001</v>
       </c>
       <c r="D52">
-        <v>6.8259999999999996</v>
+        <v>1.948</v>
       </c>
       <c r="E52">
-        <v>6.7519999999999998</v>
+        <v>2.5150000000000001</v>
       </c>
       <c r="F52">
-        <v>6.6820000000000004</v>
+        <v>2.8479999999999999</v>
       </c>
       <c r="G52">
-        <v>6.6749999999999998</v>
+        <v>2.8479999999999999</v>
       </c>
       <c r="H52">
-        <v>6.4119999999999999</v>
+        <v>2.8479999999999999</v>
       </c>
       <c r="I52">
-        <v>4.8959999999999999</v>
+        <v>2.8759999999999999</v>
       </c>
       <c r="J52">
-        <v>4.641</v>
+        <v>2.984</v>
       </c>
       <c r="K52">
-        <v>4.3630000000000004</v>
+        <v>3.0009999999999999</v>
       </c>
       <c r="L52">
-        <v>4.5679999999999996</v>
+        <v>3.048</v>
       </c>
       <c r="M52">
-        <v>4.5350000000000001</v>
+        <v>3.1080000000000001</v>
       </c>
       <c r="N52">
-        <v>4.8979999999999997</v>
+        <v>3.181</v>
       </c>
       <c r="O52">
-        <v>4.6669999999999998</v>
+        <v>3.2029999999999998</v>
       </c>
       <c r="P52">
-        <v>4.43</v>
+        <v>3.2189999999999999</v>
       </c>
       <c r="Q52">
-        <v>3.9369999999999998</v>
+        <v>3.2189999999999999</v>
       </c>
       <c r="R52">
-        <v>3.7650000000000001</v>
+        <v>3.2229999999999999</v>
       </c>
       <c r="S52">
-        <v>3.7333600000000002</v>
+        <v>3.37155</v>
       </c>
       <c r="T52">
-        <v>4.1509750000000007</v>
+        <v>3.379</v>
       </c>
       <c r="U52">
-        <v>4.040362</v>
+        <v>3.3783499999999997</v>
       </c>
       <c r="V52">
-        <v>3.7584020000000002</v>
+        <v>3.3764560000000001</v>
       </c>
       <c r="W52">
-        <v>3.8066649999999997</v>
+        <v>3.3692329999999999</v>
       </c>
       <c r="X52">
-        <v>3.9745819999999998</v>
+        <v>3.348185</v>
       </c>
       <c r="Y52">
-        <v>3.9745819999999998</v>
+        <v>3.3502800000000001</v>
       </c>
       <c r="Z52">
-        <v>3.9745819999999998</v>
+        <v>3.3502800000000001</v>
       </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B53">
+        <v>3.532</v>
+      </c>
+      <c r="C53">
+        <v>3.532</v>
+      </c>
+      <c r="D53">
+        <v>2.722</v>
+      </c>
+      <c r="E53">
+        <v>2.722</v>
+      </c>
+      <c r="F53">
+        <v>2.722</v>
+      </c>
+      <c r="G53">
+        <v>2.722</v>
+      </c>
+      <c r="H53">
+        <v>2.722</v>
       </c>
       <c r="I53">
-        <v>2.9999999999999997E-5</v>
+        <v>1.8919999999999999</v>
       </c>
       <c r="J53">
-        <v>1E-4</v>
+        <v>1.8919999999999999</v>
       </c>
       <c r="K53">
-        <v>2E-3</v>
+        <v>1.8919999999999999</v>
       </c>
       <c r="L53">
-        <v>2.5000000000000001E-2</v>
+        <v>1.8919999999999999</v>
       </c>
       <c r="M53">
-        <v>0.154</v>
+        <v>1.8919999999999999</v>
       </c>
       <c r="N53">
-        <v>0.92200000000000004</v>
+        <v>1.9059999999999999</v>
       </c>
       <c r="O53">
-        <v>1.0389999999999999</v>
+        <v>1.982</v>
       </c>
       <c r="P53">
-        <v>1.0289999999999999</v>
+        <v>1.9750000000000001</v>
       </c>
       <c r="Q53">
-        <v>1.028</v>
+        <v>1.9750000000000001</v>
       </c>
       <c r="R53">
-        <v>1.03</v>
+        <v>1.9670000000000001</v>
       </c>
       <c r="S53">
-        <v>1.0307010000000001</v>
+        <v>1.9670000000000001</v>
       </c>
       <c r="T53">
-        <v>1.033058</v>
+        <v>2.008</v>
       </c>
       <c r="U53">
-        <v>1.0443900000000002</v>
+        <v>2.0059999999999998</v>
       </c>
       <c r="V53">
-        <v>1.1002110000000001</v>
+        <v>2.0059999999999998</v>
       </c>
       <c r="W53">
-        <v>1.274713</v>
+        <v>2.0059999999999998</v>
       </c>
       <c r="X53">
-        <v>1.736537</v>
+        <v>2.0059999999999998</v>
       </c>
       <c r="Y53">
-        <v>2.9081269999999999</v>
+        <v>2.0059999999999998</v>
       </c>
       <c r="Z53">
-        <v>3.9081269999999999</v>
+        <v>2.0059999999999998</v>
       </c>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54">
+        <v>5.6210000000000004</v>
+      </c>
+      <c r="C54">
+        <v>7.4059999999999997</v>
+      </c>
+      <c r="D54">
+        <v>6.8259999999999996</v>
+      </c>
+      <c r="E54">
+        <v>6.7519999999999998</v>
+      </c>
+      <c r="F54">
+        <v>6.6820000000000004</v>
+      </c>
+      <c r="G54">
+        <v>6.6749999999999998</v>
+      </c>
+      <c r="H54">
+        <v>6.4119999999999999</v>
+      </c>
+      <c r="I54">
+        <v>4.8959999999999999</v>
+      </c>
+      <c r="J54">
+        <v>4.641</v>
+      </c>
+      <c r="K54">
+        <v>4.3630000000000004</v>
+      </c>
+      <c r="L54">
+        <v>4.5679999999999996</v>
+      </c>
+      <c r="M54">
+        <v>4.5350000000000001</v>
+      </c>
+      <c r="N54">
+        <v>4.8979999999999997</v>
+      </c>
+      <c r="O54">
+        <v>4.6669999999999998</v>
+      </c>
+      <c r="P54">
+        <v>4.43</v>
+      </c>
+      <c r="Q54">
+        <v>3.9369999999999998</v>
+      </c>
+      <c r="R54">
+        <v>3.7650000000000001</v>
+      </c>
+      <c r="S54">
+        <v>3.7333600000000002</v>
+      </c>
+      <c r="T54">
+        <v>4.1509750000000007</v>
+      </c>
+      <c r="U54">
+        <v>4.040362</v>
+      </c>
+      <c r="V54">
+        <v>3.7584020000000002</v>
+      </c>
+      <c r="W54">
+        <v>3.8066649999999997</v>
+      </c>
+      <c r="X54">
+        <v>3.9745819999999998</v>
+      </c>
+      <c r="Y54">
+        <v>3.9745819999999998</v>
+      </c>
+      <c r="Z54">
+        <v>3.9745819999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
+        <v>9</v>
+      </c>
+      <c r="I55">
+        <v>2.9999999999999997E-5</v>
+      </c>
+      <c r="J55">
+        <v>1E-4</v>
+      </c>
+      <c r="K55">
+        <v>2E-3</v>
+      </c>
+      <c r="L55">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="M55">
+        <v>0.154</v>
+      </c>
+      <c r="N55">
+        <v>0.92200000000000004</v>
+      </c>
+      <c r="O55">
+        <v>1.0389999999999999</v>
+      </c>
+      <c r="P55">
+        <v>1.0289999999999999</v>
+      </c>
+      <c r="Q55">
+        <v>1.028</v>
+      </c>
+      <c r="R55">
+        <v>1.03</v>
+      </c>
+      <c r="S55">
+        <v>1.0307010000000001</v>
+      </c>
+      <c r="T55">
+        <v>1.033058</v>
+      </c>
+      <c r="U55">
+        <v>1.0443900000000002</v>
+      </c>
+      <c r="V55">
+        <v>1.1002110000000001</v>
+      </c>
+      <c r="W55">
+        <v>1.274713</v>
+      </c>
+      <c r="X55">
+        <v>1.736537</v>
+      </c>
+      <c r="Y55">
+        <v>2.9081269999999999</v>
+      </c>
+      <c r="Z55">
+        <v>3.9081269999999999</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
         <v>10</v>
       </c>
-      <c r="F54">
+      <c r="F56">
         <v>1E-3</v>
       </c>
-      <c r="G54">
+      <c r="G56">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H54">
+      <c r="H56">
         <v>2.7E-2</v>
       </c>
-      <c r="I54">
+      <c r="I56">
         <v>0.03</v>
       </c>
-      <c r="J54">
+      <c r="J56">
         <v>0.114</v>
       </c>
-      <c r="K54">
+      <c r="K56">
         <v>0.33300000000000002</v>
       </c>
-      <c r="L54">
+      <c r="L56">
         <v>0.48799999999999999</v>
       </c>
-      <c r="M54">
+      <c r="M56">
         <v>0.54100000000000004</v>
       </c>
-      <c r="N54">
+      <c r="N56">
         <v>0.67700000000000005</v>
       </c>
-      <c r="O54">
+      <c r="O56">
         <v>0.68300000000000005</v>
       </c>
-      <c r="P54">
+      <c r="P56">
         <v>0.69899999999999995</v>
       </c>
-      <c r="Q54">
+      <c r="Q56">
         <v>0.69899999999999995</v>
       </c>
-      <c r="R54">
+      <c r="R56">
         <v>0.69899999999999995</v>
       </c>
-      <c r="S54">
+      <c r="S56">
         <v>0.69838999999999996</v>
       </c>
-      <c r="T54">
+      <c r="T56">
         <v>0.69891999999999999</v>
       </c>
-      <c r="U54">
+      <c r="U56">
         <v>0.70311999999999997</v>
       </c>
-      <c r="V54">
+      <c r="V56">
         <v>0.70279999999999998</v>
       </c>
-      <c r="W54">
+      <c r="W56">
         <v>0.70437499999999997</v>
       </c>
-      <c r="X54">
+      <c r="X56">
         <v>0.70430999999999999</v>
       </c>
-      <c r="Y54">
+      <c r="Y56">
         <v>0.70430999999999999</v>
       </c>
-      <c r="Z54">
+      <c r="Z56">
         <v>0.70430999999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>4</v>
-      </c>
-      <c r="B58">
-        <v>2000</v>
-      </c>
-      <c r="C58">
-        <v>2001</v>
-      </c>
-      <c r="D58">
-        <v>2002</v>
-      </c>
-      <c r="E58">
-        <v>2003</v>
-      </c>
-      <c r="F58">
-        <v>2004</v>
-      </c>
-      <c r="G58">
-        <v>2005</v>
-      </c>
-      <c r="H58">
-        <v>2006</v>
-      </c>
-      <c r="I58">
-        <v>2007</v>
-      </c>
-      <c r="J58">
-        <v>2008</v>
-      </c>
-      <c r="K58">
-        <v>2009</v>
-      </c>
-      <c r="L58">
-        <v>2010</v>
-      </c>
-      <c r="M58">
-        <v>2011</v>
-      </c>
-      <c r="N58">
-        <v>2012</v>
-      </c>
-      <c r="O58">
-        <v>2013</v>
-      </c>
-      <c r="P58">
-        <v>2014</v>
-      </c>
-      <c r="Q58">
-        <v>2015</v>
-      </c>
-      <c r="R58">
-        <v>2016</v>
-      </c>
-      <c r="S58">
-        <v>2017</v>
-      </c>
-      <c r="T58">
-        <v>2018</v>
-      </c>
-      <c r="U58">
-        <v>2019</v>
-      </c>
-      <c r="V58">
-        <v>2020</v>
-      </c>
-      <c r="W58">
-        <v>2021</v>
-      </c>
-      <c r="X58">
-        <v>2022</v>
       </c>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
-        <v>0</v>
-      </c>
-      <c r="J59">
-        <v>1.6E-2</v>
-      </c>
-      <c r="K59">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="L59">
-        <v>3.5431999999999998E-2</v>
-      </c>
-      <c r="M59">
-        <v>5.5999999999999994E-2</v>
-      </c>
-      <c r="N59">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="O59">
-        <v>0.110402</v>
-      </c>
-      <c r="P59">
-        <v>0.2</v>
-      </c>
-      <c r="Q59">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="R59">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="S59">
-        <v>0.39598100000000003</v>
-      </c>
-      <c r="T59">
-        <v>1.5729660000000001</v>
-      </c>
-      <c r="U59">
-        <v>1.820811</v>
-      </c>
-      <c r="V59">
-        <v>1.699341</v>
-      </c>
-      <c r="W59">
-        <v>2.5888920000000004</v>
-      </c>
-      <c r="X59">
-        <v>2.2435940000000003</v>
+        <v>84</v>
       </c>
     </row>
     <row r="60" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B60">
-        <v>17.207000000000001</v>
+        <v>2000</v>
       </c>
       <c r="C60">
-        <v>19.757000000000001</v>
+        <v>2001</v>
       </c>
       <c r="D60">
-        <v>17.373000000000001</v>
+        <v>2002</v>
       </c>
       <c r="E60">
-        <v>19.462</v>
+        <v>2003</v>
       </c>
       <c r="F60">
-        <v>19.106999999999999</v>
+        <v>2004</v>
       </c>
       <c r="G60">
-        <v>18.625</v>
+        <v>2005</v>
       </c>
       <c r="H60">
-        <v>19.206</v>
+        <v>2006</v>
       </c>
       <c r="I60">
-        <v>22.463000000000001</v>
+        <v>2007</v>
       </c>
       <c r="J60">
-        <v>23.22</v>
+        <v>2008</v>
       </c>
       <c r="K60">
-        <v>21.103000000000002</v>
+        <v>2009</v>
       </c>
       <c r="L60">
-        <v>22.606000000000002</v>
+        <v>2010</v>
       </c>
       <c r="M60">
-        <v>27.536999999999999</v>
+        <v>2011</v>
       </c>
       <c r="N60">
-        <v>22.876000000000001</v>
+        <v>2012</v>
       </c>
       <c r="O60">
-        <v>19.391598000000002</v>
+        <v>2013</v>
       </c>
       <c r="P60">
-        <v>21.305</v>
+        <v>2014</v>
       </c>
       <c r="Q60">
-        <v>22.521999999999998</v>
+        <v>2015</v>
       </c>
       <c r="R60">
-        <v>19.364000000000001</v>
+        <v>2016</v>
       </c>
       <c r="S60">
-        <v>20.914090999999999</v>
+        <v>2017</v>
       </c>
       <c r="T60">
-        <v>18.659473000000002</v>
+        <v>2018</v>
       </c>
       <c r="U60">
-        <v>17.224985</v>
+        <v>2019</v>
       </c>
       <c r="V60">
-        <v>13.53266</v>
+        <v>2020</v>
       </c>
       <c r="W60">
-        <v>17.085889999999999</v>
+        <v>2021</v>
       </c>
       <c r="X60">
-        <v>21.785509999999999</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>2</v>
-      </c>
-      <c r="B61">
-        <v>1.9119999999999999</v>
-      </c>
-      <c r="C61">
-        <v>1.9079999999999999</v>
-      </c>
-      <c r="D61">
-        <v>1.5389999999999999</v>
-      </c>
-      <c r="E61">
-        <v>1.762</v>
-      </c>
-      <c r="F61">
-        <v>1.494</v>
-      </c>
-      <c r="G61">
-        <v>1.7290000000000001</v>
-      </c>
-      <c r="H61">
-        <v>2.1589999999999998</v>
-      </c>
-      <c r="I61">
-        <v>2.3359999999999999</v>
+        <v>0</v>
       </c>
       <c r="J61">
-        <v>2.36</v>
+        <v>1.6E-2</v>
       </c>
       <c r="K61">
-        <v>1.9610000000000001</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="L61">
-        <v>1.9665680000000001</v>
+        <v>3.5431999999999998E-2</v>
       </c>
       <c r="M61">
-        <v>2.077</v>
+        <v>5.5999999999999994E-2</v>
       </c>
       <c r="N61">
-        <v>2.3559999999999999</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="O61">
-        <v>2.339</v>
+        <v>0.110402</v>
       </c>
       <c r="P61">
-        <v>2.1419999999999999</v>
+        <v>0.2</v>
       </c>
       <c r="Q61">
-        <v>1.8640000000000001</v>
+        <v>0.27200000000000002</v>
       </c>
       <c r="R61">
-        <v>2.0529999999999999</v>
+        <v>0.35299999999999998</v>
       </c>
       <c r="S61">
-        <v>1.9266459999999999</v>
+        <v>0.39598100000000003</v>
       </c>
       <c r="T61">
-        <v>2.0227580000000001</v>
+        <v>1.5729660000000001</v>
       </c>
       <c r="U61">
-        <v>2.1529029999999998</v>
+        <v>1.820811</v>
       </c>
       <c r="V61">
-        <v>2.292316</v>
+        <v>1.699341</v>
       </c>
       <c r="W61">
-        <v>3.0456720000000002</v>
+        <v>2.5888920000000004</v>
       </c>
       <c r="X61">
-        <v>2.0534110000000001</v>
+        <v>2.2435940000000003</v>
       </c>
     </row>
     <row r="62" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B62">
-        <v>2.9509999999999996</v>
+        <v>17.207000000000001</v>
       </c>
       <c r="C62">
-        <v>2.1710000000000003</v>
+        <v>19.757000000000001</v>
       </c>
       <c r="D62">
-        <v>2.7040000000000002</v>
+        <v>17.373000000000001</v>
       </c>
       <c r="E62">
-        <v>3.3010000000000002</v>
+        <v>19.462</v>
       </c>
       <c r="F62">
-        <v>3.3628110000000002</v>
+        <v>19.106999999999999</v>
       </c>
       <c r="G62">
-        <v>4.7298960000000001</v>
+        <v>18.625</v>
       </c>
       <c r="H62">
-        <v>4.5789740000000005</v>
+        <v>19.206</v>
       </c>
       <c r="I62">
-        <v>3.2339989999999998</v>
+        <v>22.463000000000001</v>
       </c>
       <c r="J62">
-        <v>3.2767620000000002</v>
+        <v>23.22</v>
       </c>
       <c r="K62">
-        <v>4.0527119999999996</v>
+        <v>21.103000000000002</v>
       </c>
       <c r="L62">
-        <v>5.6925160000000004</v>
+        <v>22.606000000000002</v>
       </c>
       <c r="M62">
-        <v>3.6909139999999998</v>
+        <v>27.536999999999999</v>
       </c>
       <c r="N62">
-        <v>3.9757060000000002</v>
+        <v>22.876000000000001</v>
       </c>
       <c r="O62">
-        <v>4.7951379999999997</v>
+        <v>19.391598000000002</v>
       </c>
       <c r="P62">
-        <v>5.1626289999999999</v>
+        <v>21.305</v>
       </c>
       <c r="Q62">
-        <v>6.1465419999999993</v>
+        <v>22.521999999999998</v>
       </c>
       <c r="R62">
-        <v>4.5678419999999997</v>
+        <v>19.364000000000001</v>
       </c>
       <c r="S62">
-        <v>3.4929449999999997</v>
+        <v>20.914090999999999</v>
       </c>
       <c r="T62">
-        <v>5.4227320000000008</v>
+        <v>18.659473000000002</v>
       </c>
       <c r="U62">
-        <v>3.3827449999999999</v>
+        <v>17.224985</v>
       </c>
       <c r="V62">
-        <v>3.3202579999999999</v>
+        <v>13.53266</v>
       </c>
       <c r="W62">
-        <v>5.0671330000000001</v>
+        <v>17.085889999999999</v>
       </c>
       <c r="X62">
-        <v>3.833256</v>
+        <v>21.785509999999999</v>
       </c>
     </row>
     <row r="63" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="B63">
-        <v>18.178000000000001</v>
+        <v>1.9119999999999999</v>
       </c>
       <c r="C63">
-        <v>19.553000000000001</v>
+        <v>1.9079999999999999</v>
       </c>
       <c r="D63">
-        <v>20.222000000000001</v>
+        <v>1.5389999999999999</v>
       </c>
       <c r="E63">
-        <v>17.28</v>
+        <v>1.762</v>
       </c>
       <c r="F63">
-        <v>16.815000000000001</v>
+        <v>1.494</v>
       </c>
       <c r="G63">
-        <v>18.652999999999999</v>
+        <v>1.7290000000000001</v>
       </c>
       <c r="H63">
-        <v>19.492999999999999</v>
+        <v>2.1589999999999998</v>
       </c>
       <c r="I63">
-        <v>14.643000000000001</v>
+        <v>2.3359999999999999</v>
       </c>
       <c r="J63">
-        <v>15.765000000000001</v>
+        <v>2.36</v>
       </c>
       <c r="K63">
-        <v>15.256</v>
+        <v>1.9610000000000001</v>
       </c>
       <c r="L63">
-        <v>15.249000000000001</v>
+        <v>1.9665680000000001</v>
       </c>
       <c r="M63">
-        <v>16.314</v>
+        <v>2.077</v>
       </c>
       <c r="N63">
-        <v>15.785</v>
+        <v>2.3559999999999999</v>
       </c>
       <c r="O63">
-        <v>14.170999999999999</v>
+        <v>2.339</v>
       </c>
       <c r="P63">
-        <v>15.867000000000001</v>
+        <v>2.1419999999999999</v>
       </c>
       <c r="Q63">
-        <v>15.382999999999999</v>
+        <v>1.8640000000000001</v>
       </c>
       <c r="R63">
-        <v>15.776</v>
+        <v>2.0529999999999999</v>
       </c>
       <c r="S63">
-        <v>15.545499</v>
+        <v>1.9266459999999999</v>
       </c>
       <c r="T63">
-        <v>16.125281000000001</v>
+        <v>2.0227580000000001</v>
       </c>
       <c r="U63">
-        <v>16.555288000000001</v>
+        <v>2.1529029999999998</v>
       </c>
       <c r="V63">
-        <v>16.625764999999998</v>
+        <v>2.292316</v>
       </c>
       <c r="W63">
-        <v>16.486893999999999</v>
+        <v>3.0456720000000002</v>
       </c>
       <c r="X63">
-        <v>16.462018</v>
+        <v>2.0534110000000001</v>
       </c>
     </row>
     <row r="64" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B64">
-        <v>0.67600000000000005</v>
+        <v>2.9509999999999996</v>
       </c>
       <c r="C64">
-        <v>0.57899999999999996</v>
+        <v>2.1710000000000003</v>
       </c>
       <c r="D64">
-        <v>0.84099999999999997</v>
+        <v>2.7040000000000002</v>
       </c>
       <c r="E64">
-        <v>0.79500000000000004</v>
+        <v>3.3010000000000002</v>
       </c>
       <c r="F64">
-        <v>0.84099999999999997</v>
+        <v>3.3628110000000002</v>
       </c>
       <c r="G64">
-        <v>0.623</v>
+        <v>4.7298960000000001</v>
       </c>
       <c r="H64">
-        <v>0.38600000000000001</v>
+        <v>4.5789740000000005</v>
       </c>
       <c r="I64">
-        <v>0.57399999999999995</v>
+        <v>3.2339989999999998</v>
       </c>
       <c r="J64">
-        <v>0.27700000000000002</v>
+        <v>3.2767620000000002</v>
       </c>
       <c r="K64">
-        <v>0.34300000000000003</v>
+        <v>4.0527119999999996</v>
       </c>
       <c r="L64">
-        <v>0.40700000000000003</v>
+        <v>5.6925160000000004</v>
       </c>
       <c r="M64">
-        <v>0.16</v>
+        <v>3.6909139999999998</v>
       </c>
       <c r="N64">
-        <v>0.23499999999999999</v>
+        <v>3.9757060000000002</v>
       </c>
       <c r="O64">
-        <v>0.24199999999999999</v>
+        <v>4.7951379999999997</v>
       </c>
       <c r="P64">
-        <v>0.22500000000000001</v>
+        <v>5.1626289999999999</v>
       </c>
       <c r="Q64">
-        <v>0.20499999999999999</v>
+        <v>6.1465419999999993</v>
       </c>
       <c r="R64">
-        <v>0.35199999999999998</v>
+        <v>4.5678419999999997</v>
       </c>
       <c r="S64">
-        <v>0.43059500000000001</v>
+        <v>3.4929449999999997</v>
       </c>
       <c r="T64">
-        <v>0.37356200000000001</v>
+        <v>5.4227320000000008</v>
       </c>
       <c r="U64">
-        <v>0.40558499999999997</v>
+        <v>3.3827449999999999</v>
       </c>
       <c r="V64">
-        <v>0.33825000000000005</v>
+        <v>3.3202579999999999</v>
       </c>
       <c r="W64">
-        <v>0.39345599999999997</v>
+        <v>5.0671330000000001</v>
       </c>
       <c r="X64">
-        <v>0.52855200000000002</v>
+        <v>3.833256</v>
       </c>
     </row>
     <row r="65" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="B65">
+        <v>18.178000000000001</v>
+      </c>
+      <c r="C65">
+        <v>19.553000000000001</v>
+      </c>
+      <c r="D65">
+        <v>20.222000000000001</v>
+      </c>
+      <c r="E65">
+        <v>17.28</v>
+      </c>
+      <c r="F65">
+        <v>16.815000000000001</v>
+      </c>
+      <c r="G65">
+        <v>18.652999999999999</v>
+      </c>
+      <c r="H65">
+        <v>19.492999999999999</v>
       </c>
       <c r="I65">
-        <v>5.9999999999999995E-5</v>
+        <v>14.643000000000001</v>
       </c>
       <c r="J65">
-        <v>1.6700000000000002E-4</v>
+        <v>15.765000000000001</v>
       </c>
       <c r="K65">
-        <v>3.2669999999999999E-3</v>
+        <v>15.256</v>
       </c>
       <c r="L65">
-        <v>1.4865E-2</v>
+        <v>15.249000000000001</v>
       </c>
       <c r="M65">
-        <v>0.10086199999999999</v>
+        <v>16.314</v>
       </c>
       <c r="N65">
-        <v>0.77869600000000005</v>
+        <v>15.785</v>
       </c>
       <c r="O65">
-        <v>1.3919870000000001</v>
+        <v>14.170999999999999</v>
       </c>
       <c r="P65">
-        <v>1.256651</v>
+        <v>15.867000000000001</v>
       </c>
       <c r="Q65">
-        <v>1.381661</v>
+        <v>15.382999999999999</v>
       </c>
       <c r="R65">
-        <v>1.3879900000000001</v>
+        <v>15.776</v>
       </c>
       <c r="S65">
-        <v>1.4029700000000001</v>
+        <v>15.545499</v>
       </c>
       <c r="T65">
-        <v>1.3427880000000001</v>
+        <v>16.125281000000001</v>
       </c>
       <c r="U65">
-        <v>1.417286</v>
+        <v>16.555288000000001</v>
       </c>
       <c r="V65">
-        <v>1.46872</v>
+        <v>16.625764999999998</v>
       </c>
       <c r="W65">
-        <v>1.4665979999999998</v>
+        <v>16.486893999999999</v>
       </c>
       <c r="X65">
-        <v>2.0938380000000003</v>
+        <v>16.462018</v>
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="C66">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="D66">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="E66">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F66">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="G66">
+        <v>0.623</v>
+      </c>
+      <c r="H66">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="I66">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="J66">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="K66">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="L66">
+        <v>0.40700000000000003</v>
+      </c>
+      <c r="M66">
+        <v>0.16</v>
+      </c>
+      <c r="N66">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="O66">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P66">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="Q66">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="R66">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="S66">
+        <v>0.43059500000000001</v>
+      </c>
+      <c r="T66">
+        <v>0.37356200000000001</v>
+      </c>
+      <c r="U66">
+        <v>0.40558499999999997</v>
+      </c>
+      <c r="V66">
+        <v>0.33825000000000005</v>
+      </c>
+      <c r="W66">
+        <v>0.39345599999999997</v>
+      </c>
+      <c r="X66">
+        <v>0.52855200000000002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A67" t="s">
+        <v>9</v>
+      </c>
+      <c r="I67">
+        <v>5.9999999999999995E-5</v>
+      </c>
+      <c r="J67">
+        <v>1.6700000000000002E-4</v>
+      </c>
+      <c r="K67">
+        <v>3.2669999999999999E-3</v>
+      </c>
+      <c r="L67">
+        <v>1.4865E-2</v>
+      </c>
+      <c r="M67">
+        <v>0.10086199999999999</v>
+      </c>
+      <c r="N67">
+        <v>0.77869600000000005</v>
+      </c>
+      <c r="O67">
+        <v>1.3919870000000001</v>
+      </c>
+      <c r="P67">
+        <v>1.256651</v>
+      </c>
+      <c r="Q67">
+        <v>1.381661</v>
+      </c>
+      <c r="R67">
+        <v>1.3879900000000001</v>
+      </c>
+      <c r="S67">
+        <v>1.4029700000000001</v>
+      </c>
+      <c r="T67">
+        <v>1.3427880000000001</v>
+      </c>
+      <c r="U67">
+        <v>1.417286</v>
+      </c>
+      <c r="V67">
+        <v>1.46872</v>
+      </c>
+      <c r="W67">
+        <v>1.4665979999999998</v>
+      </c>
+      <c r="X67">
+        <v>2.0938380000000003</v>
+      </c>
+    </row>
+    <row r="68" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
         <v>10</v>
       </c>
-      <c r="F66">
+      <c r="F68">
         <v>1E-3</v>
       </c>
-      <c r="G66">
+      <c r="G68">
         <v>4.5869999999999999E-3</v>
       </c>
-      <c r="H66">
+      <c r="H68">
         <v>2.0047000000000002E-2</v>
       </c>
-      <c r="I66">
+      <c r="I68">
         <v>4.6801999999999996E-2</v>
       </c>
-      <c r="J66">
+      <c r="J68">
         <v>0.12175799999999999</v>
       </c>
-      <c r="K66">
+      <c r="K68">
         <v>0.237009</v>
       </c>
-      <c r="L66">
+      <c r="L68">
         <v>0.681369</v>
       </c>
-      <c r="M66">
+      <c r="M68">
         <v>0.86109500000000005</v>
       </c>
-      <c r="N66">
+      <c r="N68">
         <v>1.2208979999999998</v>
       </c>
-      <c r="O66">
+      <c r="O68">
         <v>1.3735119999999998</v>
       </c>
-      <c r="P66">
+      <c r="P68">
         <v>1.3305769999999999</v>
       </c>
-      <c r="Q66">
+      <c r="Q68">
         <v>1.451511</v>
       </c>
-      <c r="R66">
+      <c r="R68">
         <v>1.4249700000000001</v>
       </c>
-      <c r="S66">
+      <c r="S68">
         <v>1.5040640000000001</v>
       </c>
-      <c r="T66">
+      <c r="T68">
         <v>1.3181230000000002</v>
       </c>
-      <c r="U66">
+      <c r="U68">
         <v>1.316988</v>
       </c>
-      <c r="V66">
+      <c r="V68">
         <v>1.4771310000000002</v>
       </c>
-      <c r="W66">
+      <c r="W68">
         <v>1.4335609999999999</v>
       </c>
-      <c r="X66">
+      <c r="X68">
         <v>1.499125</v>
-      </c>
-    </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A70" t="s">
-        <v>86</v>
-      </c>
-      <c r="B70" t="s">
-        <v>17</v>
-      </c>
-      <c r="C70">
-        <v>2000</v>
-      </c>
-      <c r="D70">
-        <v>2001</v>
-      </c>
-      <c r="E70">
-        <v>2002</v>
-      </c>
-      <c r="F70">
-        <v>2003</v>
-      </c>
-      <c r="G70">
-        <v>2004</v>
-      </c>
-      <c r="H70">
-        <v>2005</v>
-      </c>
-      <c r="I70">
-        <v>2006</v>
-      </c>
-      <c r="J70">
-        <v>2007</v>
-      </c>
-      <c r="K70">
-        <v>2008</v>
-      </c>
-      <c r="L70">
-        <v>2009</v>
-      </c>
-      <c r="M70">
-        <v>2010</v>
-      </c>
-      <c r="N70">
-        <v>2011</v>
-      </c>
-      <c r="O70">
-        <v>2012</v>
-      </c>
-      <c r="P70">
-        <v>2013</v>
-      </c>
-      <c r="Q70">
-        <v>2014</v>
-      </c>
-      <c r="R70">
-        <v>2015</v>
-      </c>
-      <c r="S70">
-        <v>2016</v>
-      </c>
-      <c r="T70">
-        <v>2017</v>
-      </c>
-      <c r="U70">
-        <v>2018</v>
-      </c>
-      <c r="V70">
-        <v>2019</v>
-      </c>
-      <c r="W70">
-        <v>2020</v>
-      </c>
-      <c r="X70">
-        <v>2021</v>
-      </c>
-      <c r="Y70">
-        <v>2022</v>
-      </c>
-      <c r="Z70">
-        <v>2023</v>
       </c>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>87</v>
-      </c>
-      <c r="B71" t="s">
-        <v>88</v>
-      </c>
-      <c r="C71">
-        <v>5.6</v>
-      </c>
-      <c r="D71">
-        <v>8</v>
-      </c>
-      <c r="E71">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="F71">
-        <v>6.8</v>
-      </c>
-      <c r="G71">
-        <v>6.6</v>
-      </c>
-      <c r="H71">
-        <v>8.4</v>
-      </c>
-      <c r="I71">
-        <v>8.9</v>
-      </c>
-      <c r="J71">
-        <v>7.5</v>
-      </c>
-      <c r="K71">
-        <v>8.4</v>
-      </c>
-      <c r="L71">
-        <v>7.7</v>
-      </c>
-      <c r="M71">
-        <v>9.6</v>
-      </c>
-      <c r="N71">
-        <v>12.1</v>
-      </c>
-      <c r="O71">
-        <v>10.7</v>
-      </c>
-      <c r="P71">
-        <v>9.5</v>
-      </c>
-      <c r="Q71">
-        <v>13.8</v>
-      </c>
-      <c r="R71">
-        <v>14.8</v>
-      </c>
-      <c r="S71">
-        <v>10.9</v>
-      </c>
-      <c r="T71">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="U71">
-        <v>10</v>
-      </c>
-      <c r="V71">
-        <v>8.9</v>
-      </c>
-      <c r="W71">
-        <v>7.1</v>
-      </c>
-      <c r="X71">
-        <v>10.6</v>
-      </c>
-      <c r="Y71">
-        <v>13.7</v>
-      </c>
-      <c r="Z71">
-        <v>7.7</v>
+        <v>85</v>
       </c>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
+        <v>86</v>
+      </c>
+      <c r="B72" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72">
+        <v>2000</v>
+      </c>
+      <c r="D72">
+        <v>2001</v>
+      </c>
+      <c r="E72">
+        <v>2002</v>
+      </c>
+      <c r="F72">
+        <v>2003</v>
+      </c>
+      <c r="G72">
+        <v>2004</v>
+      </c>
+      <c r="H72">
+        <v>2005</v>
+      </c>
+      <c r="I72">
+        <v>2006</v>
+      </c>
+      <c r="J72">
+        <v>2007</v>
+      </c>
+      <c r="K72">
+        <v>2008</v>
+      </c>
+      <c r="L72">
+        <v>2009</v>
+      </c>
+      <c r="M72">
+        <v>2010</v>
+      </c>
+      <c r="N72">
+        <v>2011</v>
+      </c>
+      <c r="O72">
+        <v>2012</v>
+      </c>
+      <c r="P72">
+        <v>2013</v>
+      </c>
+      <c r="Q72">
+        <v>2014</v>
+      </c>
+      <c r="R72">
+        <v>2015</v>
+      </c>
+      <c r="S72">
+        <v>2016</v>
+      </c>
+      <c r="T72">
+        <v>2017</v>
+      </c>
+      <c r="U72">
+        <v>2018</v>
+      </c>
+      <c r="V72">
+        <v>2019</v>
+      </c>
+      <c r="W72">
+        <v>2020</v>
+      </c>
+      <c r="X72">
+        <v>2021</v>
+      </c>
+      <c r="Y72">
+        <v>2022</v>
+      </c>
+      <c r="Z72">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="73" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A73" t="s">
         <v>87</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73">
+        <v>5.6</v>
+      </c>
+      <c r="D73">
+        <v>8</v>
+      </c>
+      <c r="E73">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F73">
+        <v>6.8</v>
+      </c>
+      <c r="G73">
+        <v>6.6</v>
+      </c>
+      <c r="H73">
+        <v>8.4</v>
+      </c>
+      <c r="I73">
+        <v>8.9</v>
+      </c>
+      <c r="J73">
+        <v>7.5</v>
+      </c>
+      <c r="K73">
+        <v>8.4</v>
+      </c>
+      <c r="L73">
+        <v>7.7</v>
+      </c>
+      <c r="M73">
+        <v>9.6</v>
+      </c>
+      <c r="N73">
+        <v>12.1</v>
+      </c>
+      <c r="O73">
+        <v>10.7</v>
+      </c>
+      <c r="P73">
+        <v>9.5</v>
+      </c>
+      <c r="Q73">
+        <v>13.8</v>
+      </c>
+      <c r="R73">
+        <v>14.8</v>
+      </c>
+      <c r="S73">
+        <v>10.9</v>
+      </c>
+      <c r="T73">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="U73">
+        <v>10</v>
+      </c>
+      <c r="V73">
+        <v>8.9</v>
+      </c>
+      <c r="W73">
+        <v>7.1</v>
+      </c>
+      <c r="X73">
+        <v>10.6</v>
+      </c>
+      <c r="Y73">
+        <v>13.7</v>
+      </c>
+      <c r="Z73">
+        <v>7.7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>87</v>
+      </c>
+      <c r="B74" t="s">
         <v>89</v>
       </c>
-      <c r="C72">
+      <c r="C74">
         <v>1</v>
       </c>
-      <c r="D72">
+      <c r="D74">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E72">
+      <c r="E74">
         <v>2</v>
       </c>
-      <c r="F72">
+      <c r="F74">
         <v>1.3</v>
       </c>
-      <c r="G72">
+      <c r="G74">
         <v>0.7</v>
       </c>
-      <c r="H72">
+      <c r="H74">
         <v>0.8</v>
       </c>
-      <c r="I72">
+      <c r="I74">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J72">
+      <c r="J74">
         <v>3.1</v>
       </c>
-      <c r="K72">
+      <c r="K74">
         <v>3.1</v>
       </c>
-      <c r="L72">
+      <c r="L74">
         <v>2.7</v>
       </c>
-      <c r="M72">
+      <c r="M74">
         <v>1.2</v>
       </c>
-      <c r="N72">
+      <c r="N74">
         <v>1.4</v>
       </c>
-      <c r="O72">
+      <c r="O74">
         <v>2.4</v>
       </c>
-      <c r="P72">
+      <c r="P74">
         <v>3.4</v>
       </c>
-      <c r="Q72">
+      <c r="Q74">
         <v>4.3</v>
       </c>
-      <c r="R72">
+      <c r="R74">
         <v>4.3</v>
       </c>
-      <c r="S72">
+      <c r="S74">
         <v>4.5999999999999996</v>
       </c>
-      <c r="T72">
+      <c r="T74">
         <v>3.7</v>
       </c>
-      <c r="U72">
+      <c r="U74">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V72">
+      <c r="V74">
         <v>3</v>
       </c>
-      <c r="W72">
+      <c r="W74">
         <v>3.7</v>
       </c>
-      <c r="X72">
+      <c r="X74">
         <v>1.9</v>
       </c>
-      <c r="Y72">
+      <c r="Y74">
         <v>1.5</v>
       </c>
-      <c r="Z72">
+      <c r="Z74">
         <v>4.4000000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 08:56
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FC846F-7D93-41F9-AAED-C74593A8E069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BA5DC2C-C4B6-415B-87D6-6CE521CDCA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -326,16 +326,16 @@
     <t>Unnamed: 25</t>
   </si>
   <si>
+    <t>EMBER Generation (TWh)</t>
+  </si>
+  <si>
     <t>EMBER Capacity (GW)</t>
   </si>
   <si>
-    <t>EMBER Generation (TWh)</t>
+    <t>IRENA Generation (TWh)</t>
   </si>
   <si>
     <t>IRENA Capacity (GW)</t>
-  </si>
-  <si>
-    <t>IRENA Generation (TWh)</t>
   </si>
   <si>
     <t>Electricity Trade Data (TWh) - Source: UNSD</t>
@@ -1275,7 +1275,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z74"/>
+  <dimension ref="A1:Z79"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="U26" sqref="U26"/>
@@ -2488,476 +2488,91 @@
         <v>0.24297964087912982</v>
       </c>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26">
-        <v>2000</v>
-      </c>
-      <c r="C26">
-        <v>2001</v>
-      </c>
-      <c r="D26">
-        <v>2002</v>
-      </c>
-      <c r="E26">
-        <v>2003</v>
-      </c>
-      <c r="F26">
-        <v>2004</v>
-      </c>
-      <c r="G26">
-        <v>2005</v>
-      </c>
-      <c r="H26">
-        <v>2006</v>
-      </c>
-      <c r="I26">
-        <v>2007</v>
-      </c>
-      <c r="J26">
-        <v>2008</v>
-      </c>
-      <c r="K26">
-        <v>2009</v>
-      </c>
-      <c r="L26">
-        <v>2010</v>
-      </c>
-      <c r="M26">
-        <v>2011</v>
-      </c>
-      <c r="N26">
-        <v>2012</v>
-      </c>
-      <c r="O26">
-        <v>2013</v>
-      </c>
-      <c r="P26">
-        <v>2014</v>
-      </c>
-      <c r="Q26">
-        <v>2015</v>
-      </c>
-      <c r="R26">
-        <v>2016</v>
-      </c>
-      <c r="S26">
-        <v>2017</v>
-      </c>
-      <c r="T26">
-        <v>2018</v>
-      </c>
-      <c r="U26">
-        <v>2019</v>
-      </c>
-      <c r="V26">
-        <v>2020</v>
-      </c>
-      <c r="W26">
-        <v>2021</v>
-      </c>
-      <c r="X26">
-        <v>2022</v>
-      </c>
-      <c r="Y26">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <v>0.05</v>
-      </c>
-      <c r="C27">
-        <v>0.05</v>
-      </c>
-      <c r="D27">
-        <v>0.05</v>
-      </c>
-      <c r="E27">
-        <v>0.01</v>
-      </c>
-      <c r="F27">
-        <v>0.01</v>
-      </c>
-      <c r="G27">
-        <v>0.01</v>
-      </c>
-      <c r="H27">
-        <v>0.01</v>
-      </c>
-      <c r="I27">
-        <v>0.01</v>
-      </c>
-      <c r="J27">
-        <v>0.01</v>
-      </c>
-      <c r="K27">
-        <v>0.01</v>
-      </c>
-      <c r="L27">
-        <v>0.01</v>
-      </c>
-      <c r="M27">
-        <v>0.01</v>
-      </c>
-      <c r="N27">
-        <v>0.01</v>
-      </c>
-      <c r="O27">
-        <v>0.03</v>
-      </c>
-      <c r="P27">
-        <v>0.04</v>
-      </c>
-      <c r="Q27">
-        <v>0.05</v>
-      </c>
-      <c r="R27">
-        <v>0.06</v>
-      </c>
-      <c r="S27">
-        <v>0.05</v>
-      </c>
-      <c r="T27">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="U27">
-        <v>0.06</v>
-      </c>
-      <c r="V27">
-        <v>0.05</v>
-      </c>
-      <c r="W27">
-        <v>0.05</v>
-      </c>
-      <c r="X27">
-        <v>0.05</v>
-      </c>
-      <c r="Y27">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28">
-        <v>5.62</v>
-      </c>
-      <c r="C28">
-        <v>5.62</v>
-      </c>
-      <c r="D28">
-        <v>5.62</v>
-      </c>
-      <c r="E28">
-        <v>5.62</v>
-      </c>
-      <c r="F28">
-        <v>5.5</v>
-      </c>
-      <c r="G28">
-        <v>5.5</v>
-      </c>
-      <c r="H28">
-        <v>5.5</v>
-      </c>
-      <c r="I28">
-        <v>5.5</v>
-      </c>
-      <c r="J28">
-        <v>5.5</v>
-      </c>
-      <c r="K28">
-        <v>5.63</v>
-      </c>
-      <c r="L28">
-        <v>5.63</v>
-      </c>
-      <c r="M28">
-        <v>6.32</v>
-      </c>
-      <c r="N28">
-        <v>6.32</v>
-      </c>
-      <c r="O28">
-        <v>6.11</v>
-      </c>
-      <c r="P28">
-        <v>5.9</v>
-      </c>
-      <c r="Q28">
-        <v>5.0599999999999996</v>
-      </c>
-      <c r="R28">
-        <v>5.0599999999999996</v>
-      </c>
-      <c r="S28">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="T28">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="U28">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="V28">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="W28">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="X28">
-        <v>5.1100000000000003</v>
-      </c>
-      <c r="Y28">
-        <v>5.1100000000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>2</v>
-      </c>
-      <c r="B29">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="C29">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="D29">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="E29">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="F29">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="G29">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="H29">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="I29">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="J29">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="K29">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="L29">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="M29">
-        <v>1.2</v>
-      </c>
-      <c r="N29">
-        <v>1.2</v>
-      </c>
-      <c r="O29">
-        <v>1.2</v>
-      </c>
-      <c r="P29">
-        <v>1.2</v>
-      </c>
-      <c r="Q29">
-        <v>1.2</v>
-      </c>
-      <c r="R29">
-        <v>1.2</v>
-      </c>
-      <c r="S29">
-        <v>1.2</v>
-      </c>
-      <c r="T29">
-        <v>1.2</v>
-      </c>
-      <c r="U29">
-        <v>1.2</v>
-      </c>
-      <c r="V29">
-        <v>1.2</v>
-      </c>
-      <c r="W29">
-        <v>1.2</v>
-      </c>
-      <c r="X29">
-        <v>1.2</v>
-      </c>
-      <c r="Y29">
-        <v>1.2</v>
-      </c>
-    </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30">
-        <v>1.02</v>
-      </c>
-      <c r="C30">
-        <v>0.84</v>
-      </c>
-      <c r="D30">
-        <v>1.08</v>
-      </c>
-      <c r="E30">
-        <v>1.65</v>
-      </c>
-      <c r="F30">
-        <v>1.98</v>
-      </c>
-      <c r="G30">
-        <v>1.98</v>
-      </c>
-      <c r="H30">
-        <v>1.98</v>
-      </c>
-      <c r="I30">
-        <v>2.0099999999999998</v>
-      </c>
-      <c r="J30">
-        <v>2.12</v>
-      </c>
-      <c r="K30">
-        <v>2.14</v>
-      </c>
-      <c r="L30">
-        <v>2.1800000000000002</v>
-      </c>
-      <c r="M30">
-        <v>2.2400000000000002</v>
-      </c>
-      <c r="N30">
-        <v>2.3199999999999998</v>
-      </c>
-      <c r="O30">
-        <v>2.34</v>
-      </c>
-      <c r="P30">
-        <v>2.36</v>
-      </c>
-      <c r="Q30">
-        <v>2.36</v>
-      </c>
-      <c r="R30">
-        <v>2.36</v>
-      </c>
-      <c r="S30">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="T30">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="U30">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="V30">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="W30">
-        <v>2.5099999999999998</v>
-      </c>
-      <c r="X30">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="Y30">
-        <v>2.5299999999999998</v>
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B31">
-        <v>3.53</v>
+        <v>2000</v>
       </c>
       <c r="C31">
-        <v>3.53</v>
+        <v>2001</v>
       </c>
       <c r="D31">
-        <v>2.72</v>
+        <v>2002</v>
       </c>
       <c r="E31">
-        <v>2.72</v>
+        <v>2003</v>
       </c>
       <c r="F31">
-        <v>2.72</v>
+        <v>2004</v>
       </c>
       <c r="G31">
-        <v>2.72</v>
+        <v>2005</v>
       </c>
       <c r="H31">
-        <v>2.72</v>
+        <v>2006</v>
       </c>
       <c r="I31">
-        <v>1.89</v>
+        <v>2007</v>
       </c>
       <c r="J31">
-        <v>1.89</v>
+        <v>2008</v>
       </c>
       <c r="K31">
-        <v>1.89</v>
+        <v>2009</v>
       </c>
       <c r="L31">
-        <v>1.89</v>
+        <v>2010</v>
       </c>
       <c r="M31">
-        <v>1.89</v>
+        <v>2011</v>
       </c>
       <c r="N31">
-        <v>1.91</v>
+        <v>2012</v>
       </c>
       <c r="O31">
-        <v>1.98</v>
+        <v>2013</v>
       </c>
       <c r="P31">
-        <v>1.98</v>
+        <v>2014</v>
       </c>
       <c r="Q31">
-        <v>1.98</v>
+        <v>2015</v>
       </c>
       <c r="R31">
-        <v>1.97</v>
+        <v>2016</v>
       </c>
       <c r="S31">
-        <v>1.97</v>
+        <v>2017</v>
       </c>
       <c r="T31">
-        <v>2.0099999999999998</v>
+        <v>2018</v>
       </c>
       <c r="U31">
-        <v>2.0099999999999998</v>
+        <v>2019</v>
       </c>
       <c r="V31">
-        <v>2.0099999999999998</v>
+        <v>2020</v>
       </c>
       <c r="W31">
-        <v>2.0099999999999998</v>
+        <v>2021</v>
       </c>
       <c r="X31">
-        <v>2.0099999999999998</v>
+        <v>2022</v>
       </c>
       <c r="Y31">
-        <v>2.0099999999999998</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -2984,293 +2599,519 @@
         <v>0</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="K32">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L32">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="M32">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="N32">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="O32">
-        <v>0</v>
+        <v>0.11</v>
       </c>
       <c r="P32">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="Q32">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="R32">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="S32">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="T32">
-        <v>0</v>
+        <v>1.57</v>
       </c>
       <c r="U32">
-        <v>0</v>
+        <v>1.82</v>
       </c>
       <c r="V32">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="W32">
-        <v>0</v>
+        <v>2.59</v>
       </c>
       <c r="X32">
-        <v>0</v>
+        <v>2.2400000000000002</v>
       </c>
       <c r="Y32">
-        <v>0</v>
+        <v>2.1800000000000002</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>16.940000000000001</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>19.5</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>17.18</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>19.239999999999998</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="G33">
-        <v>0</v>
+        <v>18.46</v>
       </c>
       <c r="H33">
-        <v>0</v>
+        <v>19.09</v>
       </c>
       <c r="I33">
-        <v>0</v>
+        <v>22.37</v>
       </c>
       <c r="J33">
-        <v>0</v>
+        <v>23.18</v>
       </c>
       <c r="K33">
-        <v>0</v>
+        <v>21.1</v>
       </c>
       <c r="L33">
-        <v>0.03</v>
+        <v>22.61</v>
       </c>
       <c r="M33">
-        <v>0.15</v>
+        <v>27.53</v>
       </c>
       <c r="N33">
-        <v>0.92</v>
+        <v>22.87</v>
       </c>
       <c r="O33">
-        <v>1.04</v>
+        <v>19.39</v>
       </c>
       <c r="P33">
-        <v>1.03</v>
+        <v>21.31</v>
       </c>
       <c r="Q33">
-        <v>1.03</v>
+        <v>22.53</v>
       </c>
       <c r="R33">
-        <v>1.03</v>
+        <v>19.37</v>
       </c>
       <c r="S33">
-        <v>1.03</v>
+        <v>20.92</v>
       </c>
       <c r="T33">
-        <v>1.03</v>
+        <v>18.66</v>
       </c>
       <c r="U33">
-        <v>1.04</v>
+        <v>17.2</v>
       </c>
       <c r="V33">
-        <v>1.1000000000000001</v>
+        <v>13.51</v>
       </c>
       <c r="W33">
-        <v>1.27</v>
+        <v>17.09</v>
       </c>
       <c r="X33">
-        <v>1.74</v>
+        <v>21.79</v>
       </c>
       <c r="Y33">
-        <v>2.94</v>
+        <v>11.56</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>1.91</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>1.91</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1.54</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1.76</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>1.49</v>
       </c>
       <c r="G34">
-        <v>0.01</v>
+        <v>1.73</v>
       </c>
       <c r="H34">
-        <v>0.03</v>
+        <v>2.16</v>
       </c>
       <c r="I34">
-        <v>0.03</v>
+        <v>2.34</v>
       </c>
       <c r="J34">
-        <v>0.11</v>
+        <v>2.36</v>
       </c>
       <c r="K34">
-        <v>0.33</v>
+        <v>1.96</v>
       </c>
       <c r="L34">
-        <v>0.49</v>
+        <v>1.97</v>
       </c>
       <c r="M34">
-        <v>0.54</v>
+        <v>2.08</v>
       </c>
       <c r="N34">
-        <v>0.68</v>
+        <v>2.36</v>
       </c>
       <c r="O34">
-        <v>0.68</v>
+        <v>2.34</v>
       </c>
       <c r="P34">
-        <v>0.7</v>
+        <v>2.14</v>
       </c>
       <c r="Q34">
-        <v>0.7</v>
+        <v>1.86</v>
       </c>
       <c r="R34">
-        <v>0.7</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="S34">
-        <v>0.7</v>
+        <v>1.93</v>
       </c>
       <c r="T34">
-        <v>0.7</v>
+        <v>2.02</v>
       </c>
       <c r="U34">
-        <v>0.7</v>
+        <v>2.15</v>
       </c>
       <c r="V34">
-        <v>0.7</v>
+        <v>2.29</v>
       </c>
       <c r="W34">
-        <v>0.7</v>
+        <v>3.05</v>
       </c>
       <c r="X34">
-        <v>0.7</v>
+        <v>2.0499999999999998</v>
       </c>
       <c r="Y34">
-        <v>0.7</v>
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35">
+        <v>2.63</v>
+      </c>
+      <c r="C35">
+        <v>1.65</v>
+      </c>
+      <c r="D35">
+        <v>2.12</v>
+      </c>
+      <c r="E35">
+        <v>2.99</v>
+      </c>
+      <c r="F35">
+        <v>3.14</v>
+      </c>
+      <c r="G35">
+        <v>4.3</v>
+      </c>
+      <c r="H35">
+        <v>4.21</v>
+      </c>
+      <c r="I35">
+        <v>2.83</v>
+      </c>
+      <c r="J35">
+        <v>2.79</v>
+      </c>
+      <c r="K35">
+        <v>3.43</v>
+      </c>
+      <c r="L35">
+        <v>5.03</v>
+      </c>
+      <c r="M35">
+        <v>2.87</v>
+      </c>
+      <c r="N35">
+        <v>3.18</v>
+      </c>
+      <c r="O35">
+        <v>4.04</v>
+      </c>
+      <c r="P35">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Q35">
+        <v>5.65</v>
+      </c>
+      <c r="R35">
+        <v>3.88</v>
+      </c>
+      <c r="S35">
+        <v>2.83</v>
+      </c>
+      <c r="T35">
+        <v>5.15</v>
+      </c>
+      <c r="U35">
+        <v>2.93</v>
+      </c>
+      <c r="V35">
+        <v>2.82</v>
+      </c>
+      <c r="W35">
+        <v>4.82</v>
+      </c>
+      <c r="X35">
+        <v>3.8</v>
+      </c>
+      <c r="Y35">
+        <v>3.11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36">
+        <v>18.18</v>
+      </c>
+      <c r="C36">
+        <v>19.55</v>
+      </c>
+      <c r="D36">
+        <v>20.22</v>
+      </c>
+      <c r="E36">
+        <v>17.28</v>
+      </c>
+      <c r="F36">
+        <v>16.82</v>
+      </c>
+      <c r="G36">
+        <v>18.649999999999999</v>
+      </c>
+      <c r="H36">
+        <v>19.489999999999998</v>
+      </c>
+      <c r="I36">
+        <v>14.64</v>
+      </c>
+      <c r="J36">
+        <v>15.77</v>
+      </c>
+      <c r="K36">
+        <v>15.26</v>
+      </c>
+      <c r="L36">
+        <v>15.25</v>
+      </c>
+      <c r="M36">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="N36">
+        <v>15.78</v>
+      </c>
+      <c r="O36">
+        <v>14.17</v>
+      </c>
+      <c r="P36">
+        <v>15.87</v>
+      </c>
+      <c r="Q36">
+        <v>15.38</v>
+      </c>
+      <c r="R36">
+        <v>15.78</v>
+      </c>
+      <c r="S36">
+        <v>15.55</v>
+      </c>
+      <c r="T36">
+        <v>16.13</v>
+      </c>
+      <c r="U36">
+        <v>16.559999999999999</v>
+      </c>
+      <c r="V36">
+        <v>16.63</v>
+      </c>
+      <c r="W36">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="X36">
+        <v>16.46</v>
+      </c>
+      <c r="Y36">
+        <v>16.16</v>
       </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>3</v>
+      </c>
+      <c r="B37">
+        <v>0.93</v>
+      </c>
+      <c r="C37">
+        <v>0.83</v>
+      </c>
+      <c r="D37">
+        <v>1.02</v>
+      </c>
+      <c r="E37">
+        <v>1.01</v>
+      </c>
+      <c r="F37">
+        <v>1.01</v>
+      </c>
+      <c r="G37">
+        <v>0.75</v>
+      </c>
+      <c r="H37">
+        <v>0.47</v>
+      </c>
+      <c r="I37">
+        <v>0.59</v>
+      </c>
+      <c r="J37">
+        <v>0.25</v>
+      </c>
+      <c r="K37">
+        <v>0.31</v>
+      </c>
+      <c r="L37">
+        <v>0.34</v>
+      </c>
+      <c r="M37">
+        <v>0.15</v>
+      </c>
+      <c r="N37">
+        <v>0.2</v>
+      </c>
+      <c r="O37">
+        <v>0.21</v>
+      </c>
+      <c r="P37">
+        <v>0.21</v>
+      </c>
+      <c r="Q37">
+        <v>0.19</v>
+      </c>
+      <c r="R37">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="S37">
+        <v>0.31</v>
+      </c>
+      <c r="T37">
+        <v>0.32</v>
+      </c>
+      <c r="U37">
+        <v>0.32</v>
+      </c>
+      <c r="V37">
+        <v>0.24</v>
+      </c>
+      <c r="W37">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="X37">
+        <v>0.35</v>
+      </c>
+      <c r="Y37">
+        <v>0.35</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B38">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="C38">
-        <v>2001</v>
+        <v>0</v>
       </c>
       <c r="D38">
-        <v>2002</v>
+        <v>0</v>
       </c>
       <c r="E38">
-        <v>2003</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>2004</v>
+        <v>0</v>
       </c>
       <c r="G38">
-        <v>2005</v>
+        <v>0</v>
       </c>
       <c r="H38">
-        <v>2006</v>
+        <v>0</v>
       </c>
       <c r="I38">
-        <v>2007</v>
+        <v>0</v>
       </c>
       <c r="J38">
-        <v>2008</v>
+        <v>0</v>
       </c>
       <c r="K38">
-        <v>2009</v>
+        <v>0</v>
       </c>
       <c r="L38">
-        <v>2010</v>
+        <v>0.01</v>
       </c>
       <c r="M38">
-        <v>2011</v>
+        <v>0.1</v>
       </c>
       <c r="N38">
-        <v>2012</v>
+        <v>0.78</v>
       </c>
       <c r="O38">
-        <v>2013</v>
+        <v>1.39</v>
       </c>
       <c r="P38">
-        <v>2014</v>
+        <v>1.26</v>
       </c>
       <c r="Q38">
-        <v>2015</v>
+        <v>1.38</v>
       </c>
       <c r="R38">
-        <v>2016</v>
+        <v>1.39</v>
       </c>
       <c r="S38">
-        <v>2017</v>
+        <v>1.4</v>
       </c>
       <c r="T38">
-        <v>2018</v>
+        <v>1.34</v>
       </c>
       <c r="U38">
-        <v>2019</v>
+        <v>1.42</v>
       </c>
       <c r="V38">
-        <v>2020</v>
+        <v>1.47</v>
       </c>
       <c r="W38">
-        <v>2021</v>
+        <v>1.47</v>
       </c>
       <c r="X38">
-        <v>2022</v>
+        <v>2.09</v>
       </c>
       <c r="Y38">
-        <v>2023</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -3291,1987 +3132,2146 @@
         <v>0</v>
       </c>
       <c r="H39">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="I39">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="J39">
-        <v>0.02</v>
+        <v>0.12</v>
       </c>
       <c r="K39">
-        <v>0.01</v>
+        <v>0.24</v>
       </c>
       <c r="L39">
-        <v>0.04</v>
+        <v>0.68</v>
       </c>
       <c r="M39">
-        <v>0.06</v>
+        <v>0.86</v>
       </c>
       <c r="N39">
-        <v>7.0000000000000007E-2</v>
+        <v>1.22</v>
       </c>
       <c r="O39">
-        <v>0.11</v>
+        <v>1.37</v>
       </c>
       <c r="P39">
-        <v>0.2</v>
+        <v>1.33</v>
       </c>
       <c r="Q39">
-        <v>0.27</v>
+        <v>1.45</v>
       </c>
       <c r="R39">
-        <v>0.35</v>
+        <v>1.42</v>
       </c>
       <c r="S39">
-        <v>0.4</v>
+        <v>1.5</v>
       </c>
       <c r="T39">
-        <v>1.57</v>
+        <v>1.32</v>
       </c>
       <c r="U39">
-        <v>1.82</v>
+        <v>1.32</v>
       </c>
       <c r="V39">
-        <v>1.7</v>
+        <v>1.48</v>
       </c>
       <c r="W39">
-        <v>2.59</v>
+        <v>1.43</v>
       </c>
       <c r="X39">
-        <v>2.2400000000000002</v>
+        <v>1.44</v>
       </c>
       <c r="Y39">
-        <v>2.1800000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>1</v>
-      </c>
-      <c r="B40">
-        <v>16.940000000000001</v>
-      </c>
-      <c r="C40">
-        <v>19.5</v>
-      </c>
-      <c r="D40">
-        <v>17.18</v>
-      </c>
-      <c r="E40">
-        <v>19.239999999999998</v>
-      </c>
-      <c r="F40">
-        <v>18.899999999999999</v>
-      </c>
-      <c r="G40">
-        <v>18.46</v>
-      </c>
-      <c r="H40">
-        <v>19.09</v>
-      </c>
-      <c r="I40">
-        <v>22.37</v>
-      </c>
-      <c r="J40">
-        <v>23.18</v>
-      </c>
-      <c r="K40">
-        <v>21.1</v>
-      </c>
-      <c r="L40">
-        <v>22.61</v>
-      </c>
-      <c r="M40">
-        <v>27.53</v>
-      </c>
-      <c r="N40">
-        <v>22.87</v>
-      </c>
-      <c r="O40">
-        <v>19.39</v>
-      </c>
-      <c r="P40">
-        <v>21.31</v>
-      </c>
-      <c r="Q40">
-        <v>22.53</v>
-      </c>
-      <c r="R40">
-        <v>19.37</v>
-      </c>
-      <c r="S40">
-        <v>20.92</v>
-      </c>
-      <c r="T40">
-        <v>18.66</v>
-      </c>
-      <c r="U40">
-        <v>17.2</v>
-      </c>
-      <c r="V40">
-        <v>13.51</v>
-      </c>
-      <c r="W40">
-        <v>17.09</v>
-      </c>
-      <c r="X40">
-        <v>21.79</v>
-      </c>
-      <c r="Y40">
-        <v>11.56</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>2</v>
-      </c>
-      <c r="B41">
-        <v>1.91</v>
-      </c>
-      <c r="C41">
-        <v>1.91</v>
-      </c>
-      <c r="D41">
-        <v>1.54</v>
-      </c>
-      <c r="E41">
-        <v>1.76</v>
-      </c>
-      <c r="F41">
-        <v>1.49</v>
-      </c>
-      <c r="G41">
-        <v>1.73</v>
-      </c>
-      <c r="H41">
-        <v>2.16</v>
-      </c>
-      <c r="I41">
-        <v>2.34</v>
-      </c>
-      <c r="J41">
-        <v>2.36</v>
-      </c>
-      <c r="K41">
-        <v>1.96</v>
-      </c>
-      <c r="L41">
-        <v>1.97</v>
-      </c>
-      <c r="M41">
-        <v>2.08</v>
-      </c>
-      <c r="N41">
-        <v>2.36</v>
-      </c>
-      <c r="O41">
-        <v>2.34</v>
-      </c>
-      <c r="P41">
-        <v>2.14</v>
-      </c>
-      <c r="Q41">
-        <v>1.86</v>
-      </c>
-      <c r="R41">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="S41">
-        <v>1.93</v>
-      </c>
-      <c r="T41">
-        <v>2.02</v>
-      </c>
-      <c r="U41">
-        <v>2.15</v>
-      </c>
-      <c r="V41">
-        <v>2.29</v>
-      </c>
-      <c r="W41">
-        <v>3.05</v>
-      </c>
-      <c r="X41">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="Y41">
-        <v>1.56</v>
+        <v>1.55</v>
       </c>
     </row>
     <row r="42" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42">
-        <v>2.63</v>
-      </c>
-      <c r="C42">
-        <v>1.65</v>
-      </c>
-      <c r="D42">
-        <v>2.12</v>
-      </c>
-      <c r="E42">
-        <v>2.99</v>
-      </c>
-      <c r="F42">
-        <v>3.14</v>
-      </c>
-      <c r="G42">
-        <v>4.3</v>
-      </c>
-      <c r="H42">
-        <v>4.21</v>
-      </c>
-      <c r="I42">
-        <v>2.83</v>
-      </c>
-      <c r="J42">
-        <v>2.79</v>
-      </c>
-      <c r="K42">
-        <v>3.43</v>
-      </c>
-      <c r="L42">
-        <v>5.03</v>
-      </c>
-      <c r="M42">
-        <v>2.87</v>
-      </c>
-      <c r="N42">
-        <v>3.18</v>
-      </c>
-      <c r="O42">
-        <v>4.04</v>
-      </c>
-      <c r="P42">
-        <v>4.5999999999999996</v>
-      </c>
-      <c r="Q42">
-        <v>5.65</v>
-      </c>
-      <c r="R42">
-        <v>3.88</v>
-      </c>
-      <c r="S42">
-        <v>2.83</v>
-      </c>
-      <c r="T42">
-        <v>5.15</v>
-      </c>
-      <c r="U42">
-        <v>2.93</v>
-      </c>
-      <c r="V42">
-        <v>2.82</v>
-      </c>
-      <c r="W42">
-        <v>4.82</v>
-      </c>
-      <c r="X42">
-        <v>3.8</v>
-      </c>
-      <c r="Y42">
-        <v>3.11</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B43">
-        <v>18.18</v>
+        <v>2000</v>
       </c>
       <c r="C43">
-        <v>19.55</v>
+        <v>2001</v>
       </c>
       <c r="D43">
-        <v>20.22</v>
+        <v>2002</v>
       </c>
       <c r="E43">
-        <v>17.28</v>
+        <v>2003</v>
       </c>
       <c r="F43">
-        <v>16.82</v>
+        <v>2004</v>
       </c>
       <c r="G43">
-        <v>18.649999999999999</v>
+        <v>2005</v>
       </c>
       <c r="H43">
-        <v>19.489999999999998</v>
+        <v>2006</v>
       </c>
       <c r="I43">
-        <v>14.64</v>
+        <v>2007</v>
       </c>
       <c r="J43">
-        <v>15.77</v>
+        <v>2008</v>
       </c>
       <c r="K43">
-        <v>15.26</v>
+        <v>2009</v>
       </c>
       <c r="L43">
-        <v>15.25</v>
+        <v>2010</v>
       </c>
       <c r="M43">
-        <v>16.309999999999999</v>
+        <v>2011</v>
       </c>
       <c r="N43">
-        <v>15.78</v>
+        <v>2012</v>
       </c>
       <c r="O43">
-        <v>14.17</v>
+        <v>2013</v>
       </c>
       <c r="P43">
-        <v>15.87</v>
+        <v>2014</v>
       </c>
       <c r="Q43">
-        <v>15.38</v>
+        <v>2015</v>
       </c>
       <c r="R43">
-        <v>15.78</v>
+        <v>2016</v>
       </c>
       <c r="S43">
-        <v>15.55</v>
+        <v>2017</v>
       </c>
       <c r="T43">
-        <v>16.13</v>
+        <v>2018</v>
       </c>
       <c r="U43">
-        <v>16.559999999999999</v>
+        <v>2019</v>
       </c>
       <c r="V43">
-        <v>16.63</v>
+        <v>2020</v>
       </c>
       <c r="W43">
-        <v>16.489999999999998</v>
+        <v>2021</v>
       </c>
       <c r="X43">
-        <v>16.46</v>
+        <v>2022</v>
       </c>
       <c r="Y43">
-        <v>16.16</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="44" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B44">
-        <v>0.93</v>
+        <v>0.05</v>
       </c>
       <c r="C44">
-        <v>0.83</v>
+        <v>0.05</v>
       </c>
       <c r="D44">
-        <v>1.02</v>
+        <v>0.05</v>
       </c>
       <c r="E44">
-        <v>1.01</v>
+        <v>0.01</v>
       </c>
       <c r="F44">
-        <v>1.01</v>
+        <v>0.01</v>
       </c>
       <c r="G44">
-        <v>0.75</v>
+        <v>0.01</v>
       </c>
       <c r="H44">
-        <v>0.47</v>
+        <v>0.01</v>
       </c>
       <c r="I44">
-        <v>0.59</v>
+        <v>0.01</v>
       </c>
       <c r="J44">
-        <v>0.25</v>
+        <v>0.01</v>
       </c>
       <c r="K44">
-        <v>0.31</v>
+        <v>0.01</v>
       </c>
       <c r="L44">
-        <v>0.34</v>
+        <v>0.01</v>
       </c>
       <c r="M44">
-        <v>0.15</v>
+        <v>0.01</v>
       </c>
       <c r="N44">
-        <v>0.2</v>
+        <v>0.01</v>
       </c>
       <c r="O44">
-        <v>0.21</v>
+        <v>0.03</v>
       </c>
       <c r="P44">
-        <v>0.21</v>
+        <v>0.04</v>
       </c>
       <c r="Q44">
-        <v>0.19</v>
+        <v>0.05</v>
       </c>
       <c r="R44">
-        <v>0.28999999999999998</v>
+        <v>0.06</v>
       </c>
       <c r="S44">
-        <v>0.31</v>
+        <v>0.05</v>
       </c>
       <c r="T44">
-        <v>0.32</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="U44">
-        <v>0.32</v>
+        <v>0.06</v>
       </c>
       <c r="V44">
-        <v>0.24</v>
+        <v>0.05</v>
       </c>
       <c r="W44">
-        <v>0.28000000000000003</v>
+        <v>0.05</v>
       </c>
       <c r="X44">
-        <v>0.35</v>
+        <v>0.05</v>
       </c>
       <c r="Y44">
-        <v>0.35</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>5.62</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>5.62</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>5.62</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>5.62</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="G45">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="I45">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>5.5</v>
       </c>
       <c r="K45">
-        <v>0</v>
+        <v>5.63</v>
       </c>
       <c r="L45">
-        <v>0.01</v>
+        <v>5.63</v>
       </c>
       <c r="M45">
-        <v>0.1</v>
+        <v>6.32</v>
       </c>
       <c r="N45">
-        <v>0.78</v>
+        <v>6.32</v>
       </c>
       <c r="O45">
-        <v>1.39</v>
+        <v>6.11</v>
       </c>
       <c r="P45">
-        <v>1.26</v>
+        <v>5.9</v>
       </c>
       <c r="Q45">
-        <v>1.38</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="R45">
-        <v>1.39</v>
+        <v>5.0599999999999996</v>
       </c>
       <c r="S45">
-        <v>1.4</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="T45">
-        <v>1.34</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="U45">
-        <v>1.42</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="V45">
-        <v>1.47</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="W45">
-        <v>1.47</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="X45">
-        <v>2.09</v>
+        <v>5.1100000000000003</v>
       </c>
       <c r="Y45">
-        <v>3.52</v>
+        <v>5.1100000000000003</v>
       </c>
     </row>
     <row r="46" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C46">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="D46">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="E46">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="F46">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G46">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="H46">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="I46">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="J46">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="K46">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="L46">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="M46">
+        <v>1.2</v>
+      </c>
+      <c r="N46">
+        <v>1.2</v>
+      </c>
+      <c r="O46">
+        <v>1.2</v>
+      </c>
+      <c r="P46">
+        <v>1.2</v>
+      </c>
+      <c r="Q46">
+        <v>1.2</v>
+      </c>
+      <c r="R46">
+        <v>1.2</v>
+      </c>
+      <c r="S46">
+        <v>1.2</v>
+      </c>
+      <c r="T46">
+        <v>1.2</v>
+      </c>
+      <c r="U46">
+        <v>1.2</v>
+      </c>
+      <c r="V46">
+        <v>1.2</v>
+      </c>
+      <c r="W46">
+        <v>1.2</v>
+      </c>
+      <c r="X46">
+        <v>1.2</v>
+      </c>
+      <c r="Y46">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47">
+        <v>1.02</v>
+      </c>
+      <c r="C47">
+        <v>0.84</v>
+      </c>
+      <c r="D47">
+        <v>1.08</v>
+      </c>
+      <c r="E47">
+        <v>1.65</v>
+      </c>
+      <c r="F47">
+        <v>1.98</v>
+      </c>
+      <c r="G47">
+        <v>1.98</v>
+      </c>
+      <c r="H47">
+        <v>1.98</v>
+      </c>
+      <c r="I47">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="J47">
+        <v>2.12</v>
+      </c>
+      <c r="K47">
+        <v>2.14</v>
+      </c>
+      <c r="L47">
+        <v>2.1800000000000002</v>
+      </c>
+      <c r="M47">
+        <v>2.2400000000000002</v>
+      </c>
+      <c r="N47">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="O47">
+        <v>2.34</v>
+      </c>
+      <c r="P47">
+        <v>2.36</v>
+      </c>
+      <c r="Q47">
+        <v>2.36</v>
+      </c>
+      <c r="R47">
+        <v>2.36</v>
+      </c>
+      <c r="S47">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="T47">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="U47">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="V47">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="W47">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="X47">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="Y47">
+        <v>2.5299999999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>3.53</v>
+      </c>
+      <c r="C48">
+        <v>3.53</v>
+      </c>
+      <c r="D48">
+        <v>2.72</v>
+      </c>
+      <c r="E48">
+        <v>2.72</v>
+      </c>
+      <c r="F48">
+        <v>2.72</v>
+      </c>
+      <c r="G48">
+        <v>2.72</v>
+      </c>
+      <c r="H48">
+        <v>2.72</v>
+      </c>
+      <c r="I48">
+        <v>1.89</v>
+      </c>
+      <c r="J48">
+        <v>1.89</v>
+      </c>
+      <c r="K48">
+        <v>1.89</v>
+      </c>
+      <c r="L48">
+        <v>1.89</v>
+      </c>
+      <c r="M48">
+        <v>1.89</v>
+      </c>
+      <c r="N48">
+        <v>1.91</v>
+      </c>
+      <c r="O48">
+        <v>1.98</v>
+      </c>
+      <c r="P48">
+        <v>1.98</v>
+      </c>
+      <c r="Q48">
+        <v>1.98</v>
+      </c>
+      <c r="R48">
+        <v>1.97</v>
+      </c>
+      <c r="S48">
+        <v>1.97</v>
+      </c>
+      <c r="T48">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="U48">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="V48">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="W48">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="X48">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="Y48">
+        <v>2.0099999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49">
+        <v>0</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A50" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50">
+        <v>0</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0.03</v>
+      </c>
+      <c r="M50">
+        <v>0.15</v>
+      </c>
+      <c r="N50">
+        <v>0.92</v>
+      </c>
+      <c r="O50">
+        <v>1.04</v>
+      </c>
+      <c r="P50">
+        <v>1.03</v>
+      </c>
+      <c r="Q50">
+        <v>1.03</v>
+      </c>
+      <c r="R50">
+        <v>1.03</v>
+      </c>
+      <c r="S50">
+        <v>1.03</v>
+      </c>
+      <c r="T50">
+        <v>1.03</v>
+      </c>
+      <c r="U50">
+        <v>1.04</v>
+      </c>
+      <c r="V50">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W50">
+        <v>1.27</v>
+      </c>
+      <c r="X50">
+        <v>1.74</v>
+      </c>
+      <c r="Y50">
+        <v>2.94</v>
+      </c>
+    </row>
+    <row r="51" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
         <v>10</v>
       </c>
-      <c r="B46">
-        <v>0</v>
-      </c>
-      <c r="C46">
-        <v>0</v>
-      </c>
-      <c r="D46">
-        <v>0</v>
-      </c>
-      <c r="E46">
-        <v>0</v>
-      </c>
-      <c r="F46">
-        <v>0</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <v>0.02</v>
-      </c>
-      <c r="I46">
-        <v>0.05</v>
-      </c>
-      <c r="J46">
-        <v>0.12</v>
-      </c>
-      <c r="K46">
-        <v>0.24</v>
-      </c>
-      <c r="L46">
+      <c r="B51">
+        <v>0</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0.01</v>
+      </c>
+      <c r="H51">
+        <v>0.03</v>
+      </c>
+      <c r="I51">
+        <v>0.03</v>
+      </c>
+      <c r="J51">
+        <v>0.11</v>
+      </c>
+      <c r="K51">
+        <v>0.33</v>
+      </c>
+      <c r="L51">
+        <v>0.49</v>
+      </c>
+      <c r="M51">
+        <v>0.54</v>
+      </c>
+      <c r="N51">
         <v>0.68</v>
       </c>
-      <c r="M46">
-        <v>0.86</v>
-      </c>
-      <c r="N46">
-        <v>1.22</v>
-      </c>
-      <c r="O46">
-        <v>1.37</v>
-      </c>
-      <c r="P46">
-        <v>1.33</v>
-      </c>
-      <c r="Q46">
-        <v>1.45</v>
-      </c>
-      <c r="R46">
-        <v>1.42</v>
-      </c>
-      <c r="S46">
-        <v>1.5</v>
-      </c>
-      <c r="T46">
-        <v>1.32</v>
-      </c>
-      <c r="U46">
-        <v>1.32</v>
-      </c>
-      <c r="V46">
-        <v>1.48</v>
-      </c>
-      <c r="W46">
-        <v>1.43</v>
-      </c>
-      <c r="X46">
-        <v>1.44</v>
-      </c>
-      <c r="Y46">
-        <v>1.55</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
+      <c r="O51">
+        <v>0.68</v>
+      </c>
+      <c r="P51">
+        <v>0.7</v>
+      </c>
+      <c r="Q51">
+        <v>0.7</v>
+      </c>
+      <c r="R51">
+        <v>0.7</v>
+      </c>
+      <c r="S51">
+        <v>0.7</v>
+      </c>
+      <c r="T51">
+        <v>0.7</v>
+      </c>
+      <c r="U51">
+        <v>0.7</v>
+      </c>
+      <c r="V51">
+        <v>0.7</v>
+      </c>
+      <c r="W51">
+        <v>0.7</v>
+      </c>
+      <c r="X51">
+        <v>0.7</v>
+      </c>
+      <c r="Y51">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A54" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
+    <row r="55" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A55" t="s">
         <v>4</v>
       </c>
-      <c r="B50">
+      <c r="B55">
         <v>2000</v>
       </c>
-      <c r="C50">
+      <c r="C55">
         <v>2001</v>
       </c>
-      <c r="D50">
+      <c r="D55">
         <v>2002</v>
       </c>
-      <c r="E50">
+      <c r="E55">
         <v>2003</v>
       </c>
-      <c r="F50">
+      <c r="F55">
         <v>2004</v>
       </c>
-      <c r="G50">
+      <c r="G55">
         <v>2005</v>
       </c>
-      <c r="H50">
+      <c r="H55">
         <v>2006</v>
       </c>
-      <c r="I50">
+      <c r="I55">
         <v>2007</v>
       </c>
-      <c r="J50">
+      <c r="J55">
         <v>2008</v>
       </c>
-      <c r="K50">
+      <c r="K55">
         <v>2009</v>
       </c>
-      <c r="L50">
+      <c r="L55">
         <v>2010</v>
       </c>
-      <c r="M50">
+      <c r="M55">
         <v>2011</v>
       </c>
-      <c r="N50">
+      <c r="N55">
         <v>2012</v>
       </c>
-      <c r="O50">
+      <c r="O55">
         <v>2013</v>
       </c>
-      <c r="P50">
+      <c r="P55">
         <v>2014</v>
       </c>
-      <c r="Q50">
+      <c r="Q55">
         <v>2015</v>
       </c>
-      <c r="R50">
+      <c r="R55">
         <v>2016</v>
       </c>
-      <c r="S50">
+      <c r="S55">
         <v>2017</v>
       </c>
-      <c r="T50">
+      <c r="T55">
         <v>2018</v>
       </c>
-      <c r="U50">
+      <c r="U55">
         <v>2019</v>
       </c>
-      <c r="V50">
+      <c r="V55">
         <v>2020</v>
       </c>
-      <c r="W50">
+      <c r="W55">
         <v>2021</v>
       </c>
-      <c r="X50">
+      <c r="X55">
         <v>2022</v>
       </c>
-      <c r="Y50">
-        <v>2023</v>
-      </c>
-      <c r="Z50">
-        <v>2024</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B51">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="C51">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="D51">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="E51">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="F51">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="G51">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="H51">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="I51">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="J51">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="K51">
-        <v>9.0000000000000011E-3</v>
-      </c>
-      <c r="L51">
-        <v>0.01</v>
-      </c>
-      <c r="M51">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="N51">
-        <v>1.4E-2</v>
-      </c>
-      <c r="O51">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="P51">
-        <v>0.04</v>
-      </c>
-      <c r="Q51">
-        <v>5.4000000000000006E-2</v>
-      </c>
-      <c r="R51">
-        <v>5.6999999999999995E-2</v>
-      </c>
-      <c r="S51">
-        <v>5.2003000000000001E-2</v>
-      </c>
-      <c r="T51">
-        <v>6.942799999999999E-2</v>
-      </c>
-      <c r="U51">
-        <v>5.6869000000000003E-2</v>
-      </c>
-      <c r="V51">
-        <v>4.8054000000000006E-2</v>
-      </c>
-      <c r="W51">
-        <v>4.7321000000000002E-2</v>
-      </c>
-      <c r="X51">
-        <v>7.8688999999999995E-2</v>
-      </c>
-      <c r="Y51">
-        <v>7.8688999999999995E-2</v>
-      </c>
-      <c r="Z51">
-        <v>7.8688999999999995E-2</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A52" t="s">
+    </row>
+    <row r="56" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A56" t="s">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K56">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L56">
+        <v>3.5431999999999998E-2</v>
+      </c>
+      <c r="M56">
+        <v>5.5999999999999994E-2</v>
+      </c>
+      <c r="N56">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="O56">
+        <v>0.110402</v>
+      </c>
+      <c r="P56">
+        <v>0.2</v>
+      </c>
+      <c r="Q56">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="R56">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="S56">
+        <v>0.39598100000000003</v>
+      </c>
+      <c r="T56">
+        <v>1.5729660000000001</v>
+      </c>
+      <c r="U56">
+        <v>1.820811</v>
+      </c>
+      <c r="V56">
+        <v>1.699341</v>
+      </c>
+      <c r="W56">
+        <v>2.5888920000000004</v>
+      </c>
+      <c r="X56">
+        <v>2.2435940000000003</v>
+      </c>
+    </row>
+    <row r="57" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>1</v>
+      </c>
+      <c r="B57">
+        <v>17.207000000000001</v>
+      </c>
+      <c r="C57">
+        <v>19.757000000000001</v>
+      </c>
+      <c r="D57">
+        <v>17.373000000000001</v>
+      </c>
+      <c r="E57">
+        <v>19.462</v>
+      </c>
+      <c r="F57">
+        <v>19.106999999999999</v>
+      </c>
+      <c r="G57">
+        <v>18.625</v>
+      </c>
+      <c r="H57">
+        <v>19.206</v>
+      </c>
+      <c r="I57">
+        <v>22.463000000000001</v>
+      </c>
+      <c r="J57">
+        <v>23.22</v>
+      </c>
+      <c r="K57">
+        <v>21.103000000000002</v>
+      </c>
+      <c r="L57">
+        <v>22.606000000000002</v>
+      </c>
+      <c r="M57">
+        <v>27.536999999999999</v>
+      </c>
+      <c r="N57">
+        <v>22.876000000000001</v>
+      </c>
+      <c r="O57">
+        <v>19.391598000000002</v>
+      </c>
+      <c r="P57">
+        <v>21.305</v>
+      </c>
+      <c r="Q57">
+        <v>22.521999999999998</v>
+      </c>
+      <c r="R57">
+        <v>19.364000000000001</v>
+      </c>
+      <c r="S57">
+        <v>20.914090999999999</v>
+      </c>
+      <c r="T57">
+        <v>18.659473000000002</v>
+      </c>
+      <c r="U57">
+        <v>17.224985</v>
+      </c>
+      <c r="V57">
+        <v>13.53266</v>
+      </c>
+      <c r="W57">
+        <v>17.085889999999999</v>
+      </c>
+      <c r="X57">
+        <v>21.785509999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A58" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58">
+        <v>1.9119999999999999</v>
+      </c>
+      <c r="C58">
+        <v>1.9079999999999999</v>
+      </c>
+      <c r="D58">
+        <v>1.5389999999999999</v>
+      </c>
+      <c r="E58">
+        <v>1.762</v>
+      </c>
+      <c r="F58">
+        <v>1.494</v>
+      </c>
+      <c r="G58">
+        <v>1.7290000000000001</v>
+      </c>
+      <c r="H58">
+        <v>2.1589999999999998</v>
+      </c>
+      <c r="I58">
+        <v>2.3359999999999999</v>
+      </c>
+      <c r="J58">
+        <v>2.36</v>
+      </c>
+      <c r="K58">
+        <v>1.9610000000000001</v>
+      </c>
+      <c r="L58">
+        <v>1.9665680000000001</v>
+      </c>
+      <c r="M58">
+        <v>2.077</v>
+      </c>
+      <c r="N58">
+        <v>2.3559999999999999</v>
+      </c>
+      <c r="O58">
+        <v>2.339</v>
+      </c>
+      <c r="P58">
+        <v>2.1419999999999999</v>
+      </c>
+      <c r="Q58">
+        <v>1.8640000000000001</v>
+      </c>
+      <c r="R58">
+        <v>2.0529999999999999</v>
+      </c>
+      <c r="S58">
+        <v>1.9266459999999999</v>
+      </c>
+      <c r="T58">
+        <v>2.0227580000000001</v>
+      </c>
+      <c r="U58">
+        <v>2.1529029999999998</v>
+      </c>
+      <c r="V58">
+        <v>2.292316</v>
+      </c>
+      <c r="W58">
+        <v>3.0456720000000002</v>
+      </c>
+      <c r="X58">
+        <v>2.0534110000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A59" t="s">
         <v>7</v>
       </c>
-      <c r="B52">
-        <v>1.88</v>
-      </c>
-      <c r="C52">
-        <v>1.7050000000000001</v>
-      </c>
-      <c r="D52">
-        <v>1.948</v>
-      </c>
-      <c r="E52">
-        <v>2.5150000000000001</v>
-      </c>
-      <c r="F52">
-        <v>2.8479999999999999</v>
-      </c>
-      <c r="G52">
-        <v>2.8479999999999999</v>
-      </c>
-      <c r="H52">
-        <v>2.8479999999999999</v>
-      </c>
-      <c r="I52">
-        <v>2.8759999999999999</v>
-      </c>
-      <c r="J52">
-        <v>2.984</v>
-      </c>
-      <c r="K52">
-        <v>3.0009999999999999</v>
-      </c>
-      <c r="L52">
-        <v>3.048</v>
-      </c>
-      <c r="M52">
-        <v>3.1080000000000001</v>
-      </c>
-      <c r="N52">
-        <v>3.181</v>
-      </c>
-      <c r="O52">
-        <v>3.2029999999999998</v>
-      </c>
-      <c r="P52">
-        <v>3.2189999999999999</v>
-      </c>
-      <c r="Q52">
-        <v>3.2189999999999999</v>
-      </c>
-      <c r="R52">
-        <v>3.2229999999999999</v>
-      </c>
-      <c r="S52">
-        <v>3.37155</v>
-      </c>
-      <c r="T52">
-        <v>3.379</v>
-      </c>
-      <c r="U52">
-        <v>3.3783499999999997</v>
-      </c>
-      <c r="V52">
-        <v>3.3764560000000001</v>
-      </c>
-      <c r="W52">
-        <v>3.3692329999999999</v>
-      </c>
-      <c r="X52">
-        <v>3.348185</v>
-      </c>
-      <c r="Y52">
-        <v>3.3502800000000001</v>
-      </c>
-      <c r="Z52">
-        <v>3.3502800000000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
+      <c r="B59">
+        <v>2.9509999999999996</v>
+      </c>
+      <c r="C59">
+        <v>2.1710000000000003</v>
+      </c>
+      <c r="D59">
+        <v>2.7040000000000002</v>
+      </c>
+      <c r="E59">
+        <v>3.3010000000000002</v>
+      </c>
+      <c r="F59">
+        <v>3.3628110000000002</v>
+      </c>
+      <c r="G59">
+        <v>4.7298960000000001</v>
+      </c>
+      <c r="H59">
+        <v>4.5789740000000005</v>
+      </c>
+      <c r="I59">
+        <v>3.2339989999999998</v>
+      </c>
+      <c r="J59">
+        <v>3.2767620000000002</v>
+      </c>
+      <c r="K59">
+        <v>4.0527119999999996</v>
+      </c>
+      <c r="L59">
+        <v>5.6925160000000004</v>
+      </c>
+      <c r="M59">
+        <v>3.6909139999999998</v>
+      </c>
+      <c r="N59">
+        <v>3.9757060000000002</v>
+      </c>
+      <c r="O59">
+        <v>4.7951379999999997</v>
+      </c>
+      <c r="P59">
+        <v>5.1626289999999999</v>
+      </c>
+      <c r="Q59">
+        <v>6.1465419999999993</v>
+      </c>
+      <c r="R59">
+        <v>4.5678419999999997</v>
+      </c>
+      <c r="S59">
+        <v>3.4929449999999997</v>
+      </c>
+      <c r="T59">
+        <v>5.4227320000000008</v>
+      </c>
+      <c r="U59">
+        <v>3.3827449999999999</v>
+      </c>
+      <c r="V59">
+        <v>3.3202579999999999</v>
+      </c>
+      <c r="W59">
+        <v>5.0671330000000001</v>
+      </c>
+      <c r="X59">
+        <v>3.833256</v>
+      </c>
+    </row>
+    <row r="60" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A60" t="s">
         <v>8</v>
       </c>
-      <c r="B53">
-        <v>3.532</v>
-      </c>
-      <c r="C53">
-        <v>3.532</v>
-      </c>
-      <c r="D53">
-        <v>2.722</v>
-      </c>
-      <c r="E53">
-        <v>2.722</v>
-      </c>
-      <c r="F53">
-        <v>2.722</v>
-      </c>
-      <c r="G53">
-        <v>2.722</v>
-      </c>
-      <c r="H53">
-        <v>2.722</v>
-      </c>
-      <c r="I53">
-        <v>1.8919999999999999</v>
-      </c>
-      <c r="J53">
-        <v>1.8919999999999999</v>
-      </c>
-      <c r="K53">
-        <v>1.8919999999999999</v>
-      </c>
-      <c r="L53">
-        <v>1.8919999999999999</v>
-      </c>
-      <c r="M53">
-        <v>1.8919999999999999</v>
-      </c>
-      <c r="N53">
-        <v>1.9059999999999999</v>
-      </c>
-      <c r="O53">
-        <v>1.982</v>
-      </c>
-      <c r="P53">
-        <v>1.9750000000000001</v>
-      </c>
-      <c r="Q53">
-        <v>1.9750000000000001</v>
-      </c>
-      <c r="R53">
-        <v>1.9670000000000001</v>
-      </c>
-      <c r="S53">
-        <v>1.9670000000000001</v>
-      </c>
-      <c r="T53">
-        <v>2.008</v>
-      </c>
-      <c r="U53">
-        <v>2.0059999999999998</v>
-      </c>
-      <c r="V53">
-        <v>2.0059999999999998</v>
-      </c>
-      <c r="W53">
-        <v>2.0059999999999998</v>
-      </c>
-      <c r="X53">
-        <v>2.0059999999999998</v>
-      </c>
-      <c r="Y53">
-        <v>2.0059999999999998</v>
-      </c>
-      <c r="Z53">
-        <v>2.0059999999999998</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A54" t="s">
+      <c r="B60">
+        <v>18.178000000000001</v>
+      </c>
+      <c r="C60">
+        <v>19.553000000000001</v>
+      </c>
+      <c r="D60">
+        <v>20.222000000000001</v>
+      </c>
+      <c r="E60">
+        <v>17.28</v>
+      </c>
+      <c r="F60">
+        <v>16.815000000000001</v>
+      </c>
+      <c r="G60">
+        <v>18.652999999999999</v>
+      </c>
+      <c r="H60">
+        <v>19.492999999999999</v>
+      </c>
+      <c r="I60">
+        <v>14.643000000000001</v>
+      </c>
+      <c r="J60">
+        <v>15.765000000000001</v>
+      </c>
+      <c r="K60">
+        <v>15.256</v>
+      </c>
+      <c r="L60">
+        <v>15.249000000000001</v>
+      </c>
+      <c r="M60">
+        <v>16.314</v>
+      </c>
+      <c r="N60">
+        <v>15.785</v>
+      </c>
+      <c r="O60">
+        <v>14.170999999999999</v>
+      </c>
+      <c r="P60">
+        <v>15.867000000000001</v>
+      </c>
+      <c r="Q60">
+        <v>15.382999999999999</v>
+      </c>
+      <c r="R60">
+        <v>15.776</v>
+      </c>
+      <c r="S60">
+        <v>15.545499</v>
+      </c>
+      <c r="T60">
+        <v>16.125281000000001</v>
+      </c>
+      <c r="U60">
+        <v>16.555288000000001</v>
+      </c>
+      <c r="V60">
+        <v>16.625764999999998</v>
+      </c>
+      <c r="W60">
+        <v>16.486893999999999</v>
+      </c>
+      <c r="X60">
+        <v>16.462018</v>
+      </c>
+    </row>
+    <row r="61" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A61" t="s">
         <v>3</v>
       </c>
-      <c r="B54">
-        <v>5.6210000000000004</v>
-      </c>
-      <c r="C54">
-        <v>7.4059999999999997</v>
-      </c>
-      <c r="D54">
-        <v>6.8259999999999996</v>
-      </c>
-      <c r="E54">
-        <v>6.7519999999999998</v>
-      </c>
-      <c r="F54">
-        <v>6.6820000000000004</v>
-      </c>
-      <c r="G54">
-        <v>6.6749999999999998</v>
-      </c>
-      <c r="H54">
-        <v>6.4119999999999999</v>
-      </c>
-      <c r="I54">
-        <v>4.8959999999999999</v>
-      </c>
-      <c r="J54">
-        <v>4.641</v>
-      </c>
-      <c r="K54">
-        <v>4.3630000000000004</v>
-      </c>
-      <c r="L54">
-        <v>4.5679999999999996</v>
-      </c>
-      <c r="M54">
-        <v>4.5350000000000001</v>
-      </c>
-      <c r="N54">
-        <v>4.8979999999999997</v>
-      </c>
-      <c r="O54">
-        <v>4.6669999999999998</v>
-      </c>
-      <c r="P54">
-        <v>4.43</v>
-      </c>
-      <c r="Q54">
-        <v>3.9369999999999998</v>
-      </c>
-      <c r="R54">
-        <v>3.7650000000000001</v>
-      </c>
-      <c r="S54">
-        <v>3.7333600000000002</v>
-      </c>
-      <c r="T54">
-        <v>4.1509750000000007</v>
-      </c>
-      <c r="U54">
-        <v>4.040362</v>
-      </c>
-      <c r="V54">
-        <v>3.7584020000000002</v>
-      </c>
-      <c r="W54">
-        <v>3.8066649999999997</v>
-      </c>
-      <c r="X54">
-        <v>3.9745819999999998</v>
-      </c>
-      <c r="Y54">
-        <v>3.9745819999999998</v>
-      </c>
-      <c r="Z54">
-        <v>3.9745819999999998</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A55" t="s">
+      <c r="B61">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="C61">
+        <v>0.57899999999999996</v>
+      </c>
+      <c r="D61">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="E61">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="F61">
+        <v>0.84099999999999997</v>
+      </c>
+      <c r="G61">
+        <v>0.623</v>
+      </c>
+      <c r="H61">
+        <v>0.38600000000000001</v>
+      </c>
+      <c r="I61">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="J61">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="K61">
+        <v>0.34300000000000003</v>
+      </c>
+      <c r="L61">
+        <v>0.40700000000000003</v>
+      </c>
+      <c r="M61">
+        <v>0.16</v>
+      </c>
+      <c r="N61">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="O61">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="P61">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="Q61">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="R61">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="S61">
+        <v>0.43059500000000001</v>
+      </c>
+      <c r="T61">
+        <v>0.37356200000000001</v>
+      </c>
+      <c r="U61">
+        <v>0.40558499999999997</v>
+      </c>
+      <c r="V61">
+        <v>0.33825000000000005</v>
+      </c>
+      <c r="W61">
+        <v>0.39345599999999997</v>
+      </c>
+      <c r="X61">
+        <v>0.52855200000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A62" t="s">
         <v>9</v>
       </c>
-      <c r="I55">
-        <v>2.9999999999999997E-5</v>
-      </c>
-      <c r="J55">
-        <v>1E-4</v>
-      </c>
-      <c r="K55">
-        <v>2E-3</v>
-      </c>
-      <c r="L55">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="M55">
-        <v>0.154</v>
-      </c>
-      <c r="N55">
-        <v>0.92200000000000004</v>
-      </c>
-      <c r="O55">
-        <v>1.0389999999999999</v>
-      </c>
-      <c r="P55">
-        <v>1.0289999999999999</v>
-      </c>
-      <c r="Q55">
-        <v>1.028</v>
-      </c>
-      <c r="R55">
-        <v>1.03</v>
-      </c>
-      <c r="S55">
-        <v>1.0307010000000001</v>
-      </c>
-      <c r="T55">
-        <v>1.033058</v>
-      </c>
-      <c r="U55">
-        <v>1.0443900000000002</v>
-      </c>
-      <c r="V55">
-        <v>1.1002110000000001</v>
-      </c>
-      <c r="W55">
-        <v>1.274713</v>
-      </c>
-      <c r="X55">
-        <v>1.736537</v>
-      </c>
-      <c r="Y55">
-        <v>2.9081269999999999</v>
-      </c>
-      <c r="Z55">
-        <v>3.9081269999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
+      <c r="I62">
+        <v>5.9999999999999995E-5</v>
+      </c>
+      <c r="J62">
+        <v>1.6700000000000002E-4</v>
+      </c>
+      <c r="K62">
+        <v>3.2669999999999999E-3</v>
+      </c>
+      <c r="L62">
+        <v>1.4865E-2</v>
+      </c>
+      <c r="M62">
+        <v>0.10086199999999999</v>
+      </c>
+      <c r="N62">
+        <v>0.77869600000000005</v>
+      </c>
+      <c r="O62">
+        <v>1.3919870000000001</v>
+      </c>
+      <c r="P62">
+        <v>1.256651</v>
+      </c>
+      <c r="Q62">
+        <v>1.381661</v>
+      </c>
+      <c r="R62">
+        <v>1.3879900000000001</v>
+      </c>
+      <c r="S62">
+        <v>1.4029700000000001</v>
+      </c>
+      <c r="T62">
+        <v>1.3427880000000001</v>
+      </c>
+      <c r="U62">
+        <v>1.417286</v>
+      </c>
+      <c r="V62">
+        <v>1.46872</v>
+      </c>
+      <c r="W62">
+        <v>1.4665979999999998</v>
+      </c>
+      <c r="X62">
+        <v>2.0938380000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
         <v>10</v>
       </c>
-      <c r="F56">
+      <c r="F63">
         <v>1E-3</v>
       </c>
-      <c r="G56">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="H56">
-        <v>2.7E-2</v>
-      </c>
-      <c r="I56">
-        <v>0.03</v>
-      </c>
-      <c r="J56">
-        <v>0.114</v>
-      </c>
-      <c r="K56">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="L56">
-        <v>0.48799999999999999</v>
-      </c>
-      <c r="M56">
-        <v>0.54100000000000004</v>
-      </c>
-      <c r="N56">
-        <v>0.67700000000000005</v>
-      </c>
-      <c r="O56">
-        <v>0.68300000000000005</v>
-      </c>
-      <c r="P56">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="Q56">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="R56">
-        <v>0.69899999999999995</v>
-      </c>
-      <c r="S56">
-        <v>0.69838999999999996</v>
-      </c>
-      <c r="T56">
-        <v>0.69891999999999999</v>
-      </c>
-      <c r="U56">
-        <v>0.70311999999999997</v>
-      </c>
-      <c r="V56">
-        <v>0.70279999999999998</v>
-      </c>
-      <c r="W56">
-        <v>0.70437499999999997</v>
-      </c>
-      <c r="X56">
-        <v>0.70430999999999999</v>
-      </c>
-      <c r="Y56">
-        <v>0.70430999999999999</v>
-      </c>
-      <c r="Z56">
-        <v>0.70430999999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>4</v>
-      </c>
-      <c r="B60">
-        <v>2000</v>
-      </c>
-      <c r="C60">
-        <v>2001</v>
-      </c>
-      <c r="D60">
-        <v>2002</v>
-      </c>
-      <c r="E60">
-        <v>2003</v>
-      </c>
-      <c r="F60">
-        <v>2004</v>
-      </c>
-      <c r="G60">
-        <v>2005</v>
-      </c>
-      <c r="H60">
-        <v>2006</v>
-      </c>
-      <c r="I60">
-        <v>2007</v>
-      </c>
-      <c r="J60">
-        <v>2008</v>
-      </c>
-      <c r="K60">
-        <v>2009</v>
-      </c>
-      <c r="L60">
-        <v>2010</v>
-      </c>
-      <c r="M60">
-        <v>2011</v>
-      </c>
-      <c r="N60">
-        <v>2012</v>
-      </c>
-      <c r="O60">
-        <v>2013</v>
-      </c>
-      <c r="P60">
-        <v>2014</v>
-      </c>
-      <c r="Q60">
-        <v>2015</v>
-      </c>
-      <c r="R60">
-        <v>2016</v>
-      </c>
-      <c r="S60">
-        <v>2017</v>
-      </c>
-      <c r="T60">
-        <v>2018</v>
-      </c>
-      <c r="U60">
-        <v>2019</v>
-      </c>
-      <c r="V60">
-        <v>2020</v>
-      </c>
-      <c r="W60">
-        <v>2021</v>
-      </c>
-      <c r="X60">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>0</v>
-      </c>
-      <c r="J61">
-        <v>1.6E-2</v>
-      </c>
-      <c r="K61">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="L61">
-        <v>3.5431999999999998E-2</v>
-      </c>
-      <c r="M61">
-        <v>5.5999999999999994E-2</v>
-      </c>
-      <c r="N61">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="O61">
-        <v>0.110402</v>
-      </c>
-      <c r="P61">
-        <v>0.2</v>
-      </c>
-      <c r="Q61">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="R61">
-        <v>0.35299999999999998</v>
-      </c>
-      <c r="S61">
-        <v>0.39598100000000003</v>
-      </c>
-      <c r="T61">
-        <v>1.5729660000000001</v>
-      </c>
-      <c r="U61">
-        <v>1.820811</v>
-      </c>
-      <c r="V61">
-        <v>1.699341</v>
-      </c>
-      <c r="W61">
-        <v>2.5888920000000004</v>
-      </c>
-      <c r="X61">
-        <v>2.2435940000000003</v>
-      </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B62">
-        <v>17.207000000000001</v>
-      </c>
-      <c r="C62">
-        <v>19.757000000000001</v>
-      </c>
-      <c r="D62">
-        <v>17.373000000000001</v>
-      </c>
-      <c r="E62">
-        <v>19.462</v>
-      </c>
-      <c r="F62">
-        <v>19.106999999999999</v>
-      </c>
-      <c r="G62">
-        <v>18.625</v>
-      </c>
-      <c r="H62">
-        <v>19.206</v>
-      </c>
-      <c r="I62">
-        <v>22.463000000000001</v>
-      </c>
-      <c r="J62">
-        <v>23.22</v>
-      </c>
-      <c r="K62">
-        <v>21.103000000000002</v>
-      </c>
-      <c r="L62">
-        <v>22.606000000000002</v>
-      </c>
-      <c r="M62">
-        <v>27.536999999999999</v>
-      </c>
-      <c r="N62">
-        <v>22.876000000000001</v>
-      </c>
-      <c r="O62">
-        <v>19.391598000000002</v>
-      </c>
-      <c r="P62">
-        <v>21.305</v>
-      </c>
-      <c r="Q62">
-        <v>22.521999999999998</v>
-      </c>
-      <c r="R62">
-        <v>19.364000000000001</v>
-      </c>
-      <c r="S62">
-        <v>20.914090999999999</v>
-      </c>
-      <c r="T62">
-        <v>18.659473000000002</v>
-      </c>
-      <c r="U62">
-        <v>17.224985</v>
-      </c>
-      <c r="V62">
-        <v>13.53266</v>
-      </c>
-      <c r="W62">
-        <v>17.085889999999999</v>
-      </c>
-      <c r="X62">
-        <v>21.785509999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>2</v>
-      </c>
-      <c r="B63">
-        <v>1.9119999999999999</v>
-      </c>
-      <c r="C63">
-        <v>1.9079999999999999</v>
-      </c>
-      <c r="D63">
-        <v>1.5389999999999999</v>
-      </c>
-      <c r="E63">
-        <v>1.762</v>
-      </c>
-      <c r="F63">
-        <v>1.494</v>
-      </c>
       <c r="G63">
-        <v>1.7290000000000001</v>
+        <v>4.5869999999999999E-3</v>
       </c>
       <c r="H63">
-        <v>2.1589999999999998</v>
+        <v>2.0047000000000002E-2</v>
       </c>
       <c r="I63">
-        <v>2.3359999999999999</v>
+        <v>4.6801999999999996E-2</v>
       </c>
       <c r="J63">
-        <v>2.36</v>
+        <v>0.12175799999999999</v>
       </c>
       <c r="K63">
-        <v>1.9610000000000001</v>
+        <v>0.237009</v>
       </c>
       <c r="L63">
-        <v>1.9665680000000001</v>
+        <v>0.681369</v>
       </c>
       <c r="M63">
-        <v>2.077</v>
+        <v>0.86109500000000005</v>
       </c>
       <c r="N63">
-        <v>2.3559999999999999</v>
+        <v>1.2208979999999998</v>
       </c>
       <c r="O63">
-        <v>2.339</v>
+        <v>1.3735119999999998</v>
       </c>
       <c r="P63">
-        <v>2.1419999999999999</v>
+        <v>1.3305769999999999</v>
       </c>
       <c r="Q63">
-        <v>1.8640000000000001</v>
+        <v>1.451511</v>
       </c>
       <c r="R63">
-        <v>2.0529999999999999</v>
+        <v>1.4249700000000001</v>
       </c>
       <c r="S63">
-        <v>1.9266459999999999</v>
+        <v>1.5040640000000001</v>
       </c>
       <c r="T63">
-        <v>2.0227580000000001</v>
+        <v>1.3181230000000002</v>
       </c>
       <c r="U63">
-        <v>2.1529029999999998</v>
+        <v>1.316988</v>
       </c>
       <c r="V63">
-        <v>2.292316</v>
+        <v>1.4771310000000002</v>
       </c>
       <c r="W63">
-        <v>3.0456720000000002</v>
+        <v>1.4335609999999999</v>
       </c>
       <c r="X63">
-        <v>2.0534110000000001</v>
-      </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>7</v>
-      </c>
-      <c r="B64">
-        <v>2.9509999999999996</v>
-      </c>
-      <c r="C64">
-        <v>2.1710000000000003</v>
-      </c>
-      <c r="D64">
-        <v>2.7040000000000002</v>
-      </c>
-      <c r="E64">
-        <v>3.3010000000000002</v>
-      </c>
-      <c r="F64">
-        <v>3.3628110000000002</v>
-      </c>
-      <c r="G64">
-        <v>4.7298960000000001</v>
-      </c>
-      <c r="H64">
-        <v>4.5789740000000005</v>
-      </c>
-      <c r="I64">
-        <v>3.2339989999999998</v>
-      </c>
-      <c r="J64">
-        <v>3.2767620000000002</v>
-      </c>
-      <c r="K64">
-        <v>4.0527119999999996</v>
-      </c>
-      <c r="L64">
-        <v>5.6925160000000004</v>
-      </c>
-      <c r="M64">
-        <v>3.6909139999999998</v>
-      </c>
-      <c r="N64">
-        <v>3.9757060000000002</v>
-      </c>
-      <c r="O64">
-        <v>4.7951379999999997</v>
-      </c>
-      <c r="P64">
-        <v>5.1626289999999999</v>
-      </c>
-      <c r="Q64">
-        <v>6.1465419999999993</v>
-      </c>
-      <c r="R64">
-        <v>4.5678419999999997</v>
-      </c>
-      <c r="S64">
-        <v>3.4929449999999997</v>
-      </c>
-      <c r="T64">
-        <v>5.4227320000000008</v>
-      </c>
-      <c r="U64">
-        <v>3.3827449999999999</v>
-      </c>
-      <c r="V64">
-        <v>3.3202579999999999</v>
-      </c>
-      <c r="W64">
-        <v>5.0671330000000001</v>
-      </c>
-      <c r="X64">
-        <v>3.833256</v>
-      </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>8</v>
-      </c>
-      <c r="B65">
-        <v>18.178000000000001</v>
-      </c>
-      <c r="C65">
-        <v>19.553000000000001</v>
-      </c>
-      <c r="D65">
-        <v>20.222000000000001</v>
-      </c>
-      <c r="E65">
-        <v>17.28</v>
-      </c>
-      <c r="F65">
-        <v>16.815000000000001</v>
-      </c>
-      <c r="G65">
-        <v>18.652999999999999</v>
-      </c>
-      <c r="H65">
-        <v>19.492999999999999</v>
-      </c>
-      <c r="I65">
-        <v>14.643000000000001</v>
-      </c>
-      <c r="J65">
-        <v>15.765000000000001</v>
-      </c>
-      <c r="K65">
-        <v>15.256</v>
-      </c>
-      <c r="L65">
-        <v>15.249000000000001</v>
-      </c>
-      <c r="M65">
-        <v>16.314</v>
-      </c>
-      <c r="N65">
-        <v>15.785</v>
-      </c>
-      <c r="O65">
-        <v>14.170999999999999</v>
-      </c>
-      <c r="P65">
-        <v>15.867000000000001</v>
-      </c>
-      <c r="Q65">
-        <v>15.382999999999999</v>
-      </c>
-      <c r="R65">
-        <v>15.776</v>
-      </c>
-      <c r="S65">
-        <v>15.545499</v>
-      </c>
-      <c r="T65">
-        <v>16.125281000000001</v>
-      </c>
-      <c r="U65">
-        <v>16.555288000000001</v>
-      </c>
-      <c r="V65">
-        <v>16.625764999999998</v>
-      </c>
-      <c r="W65">
-        <v>16.486893999999999</v>
-      </c>
-      <c r="X65">
-        <v>16.462018</v>
+        <v>1.499125</v>
       </c>
     </row>
     <row r="66" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66">
-        <v>0.67600000000000005</v>
-      </c>
-      <c r="C66">
-        <v>0.57899999999999996</v>
-      </c>
-      <c r="D66">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="E66">
-        <v>0.79500000000000004</v>
-      </c>
-      <c r="F66">
-        <v>0.84099999999999997</v>
-      </c>
-      <c r="G66">
-        <v>0.623</v>
-      </c>
-      <c r="H66">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="I66">
-        <v>0.57399999999999995</v>
-      </c>
-      <c r="J66">
-        <v>0.27700000000000002</v>
-      </c>
-      <c r="K66">
-        <v>0.34300000000000003</v>
-      </c>
-      <c r="L66">
-        <v>0.40700000000000003</v>
-      </c>
-      <c r="M66">
-        <v>0.16</v>
-      </c>
-      <c r="N66">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="O66">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="P66">
-        <v>0.22500000000000001</v>
-      </c>
-      <c r="Q66">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="R66">
-        <v>0.35199999999999998</v>
-      </c>
-      <c r="S66">
-        <v>0.43059500000000001</v>
-      </c>
-      <c r="T66">
-        <v>0.37356200000000001</v>
-      </c>
-      <c r="U66">
-        <v>0.40558499999999997</v>
-      </c>
-      <c r="V66">
-        <v>0.33825000000000005</v>
-      </c>
-      <c r="W66">
-        <v>0.39345599999999997</v>
-      </c>
-      <c r="X66">
-        <v>0.52855200000000002</v>
+        <v>84</v>
       </c>
     </row>
     <row r="67" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B67">
+        <v>2000</v>
+      </c>
+      <c r="C67">
+        <v>2001</v>
+      </c>
+      <c r="D67">
+        <v>2002</v>
+      </c>
+      <c r="E67">
+        <v>2003</v>
+      </c>
+      <c r="F67">
+        <v>2004</v>
+      </c>
+      <c r="G67">
+        <v>2005</v>
+      </c>
+      <c r="H67">
+        <v>2006</v>
       </c>
       <c r="I67">
-        <v>5.9999999999999995E-5</v>
+        <v>2007</v>
       </c>
       <c r="J67">
-        <v>1.6700000000000002E-4</v>
+        <v>2008</v>
       </c>
       <c r="K67">
-        <v>3.2669999999999999E-3</v>
+        <v>2009</v>
       </c>
       <c r="L67">
-        <v>1.4865E-2</v>
+        <v>2010</v>
       </c>
       <c r="M67">
-        <v>0.10086199999999999</v>
+        <v>2011</v>
       </c>
       <c r="N67">
-        <v>0.77869600000000005</v>
+        <v>2012</v>
       </c>
       <c r="O67">
-        <v>1.3919870000000001</v>
+        <v>2013</v>
       </c>
       <c r="P67">
-        <v>1.256651</v>
+        <v>2014</v>
       </c>
       <c r="Q67">
-        <v>1.381661</v>
+        <v>2015</v>
       </c>
       <c r="R67">
-        <v>1.3879900000000001</v>
+        <v>2016</v>
       </c>
       <c r="S67">
-        <v>1.4029700000000001</v>
+        <v>2017</v>
       </c>
       <c r="T67">
-        <v>1.3427880000000001</v>
+        <v>2018</v>
       </c>
       <c r="U67">
-        <v>1.417286</v>
+        <v>2019</v>
       </c>
       <c r="V67">
-        <v>1.46872</v>
+        <v>2020</v>
       </c>
       <c r="W67">
-        <v>1.4665979999999998</v>
+        <v>2021</v>
       </c>
       <c r="X67">
-        <v>2.0938380000000003</v>
+        <v>2022</v>
+      </c>
+      <c r="Y67">
+        <v>2023</v>
+      </c>
+      <c r="Z67">
+        <v>2024</v>
       </c>
     </row>
     <row r="68" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
-        <v>10</v>
+        <v>0</v>
+      </c>
+      <c r="B68">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="C68">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D68">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E68">
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="F68">
-        <v>1E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="G68">
-        <v>4.5869999999999999E-3</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="H68">
-        <v>2.0047000000000002E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="I68">
-        <v>4.6801999999999996E-2</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="J68">
-        <v>0.12175799999999999</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="K68">
-        <v>0.237009</v>
+        <v>9.0000000000000011E-3</v>
       </c>
       <c r="L68">
-        <v>0.681369</v>
+        <v>0.01</v>
       </c>
       <c r="M68">
-        <v>0.86109500000000005</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="N68">
-        <v>1.2208979999999998</v>
+        <v>1.4E-2</v>
       </c>
       <c r="O68">
-        <v>1.3735119999999998</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="P68">
-        <v>1.3305769999999999</v>
+        <v>0.04</v>
       </c>
       <c r="Q68">
-        <v>1.451511</v>
+        <v>5.4000000000000006E-2</v>
       </c>
       <c r="R68">
-        <v>1.4249700000000001</v>
+        <v>5.6999999999999995E-2</v>
       </c>
       <c r="S68">
-        <v>1.5040640000000001</v>
+        <v>5.2003000000000001E-2</v>
       </c>
       <c r="T68">
-        <v>1.3181230000000002</v>
+        <v>6.942799999999999E-2</v>
       </c>
       <c r="U68">
-        <v>1.316988</v>
+        <v>5.6869000000000003E-2</v>
       </c>
       <c r="V68">
-        <v>1.4771310000000002</v>
+        <v>4.8054000000000006E-2</v>
       </c>
       <c r="W68">
-        <v>1.4335609999999999</v>
+        <v>4.7321000000000002E-2</v>
       </c>
       <c r="X68">
-        <v>1.499125</v>
+        <v>7.8688999999999995E-2</v>
+      </c>
+      <c r="Y68">
+        <v>7.8688999999999995E-2</v>
+      </c>
+      <c r="Z68">
+        <v>7.8688999999999995E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A69" t="s">
+        <v>7</v>
+      </c>
+      <c r="B69">
+        <v>1.88</v>
+      </c>
+      <c r="C69">
+        <v>1.7050000000000001</v>
+      </c>
+      <c r="D69">
+        <v>1.948</v>
+      </c>
+      <c r="E69">
+        <v>2.5150000000000001</v>
+      </c>
+      <c r="F69">
+        <v>2.8479999999999999</v>
+      </c>
+      <c r="G69">
+        <v>2.8479999999999999</v>
+      </c>
+      <c r="H69">
+        <v>2.8479999999999999</v>
+      </c>
+      <c r="I69">
+        <v>2.8759999999999999</v>
+      </c>
+      <c r="J69">
+        <v>2.984</v>
+      </c>
+      <c r="K69">
+        <v>3.0009999999999999</v>
+      </c>
+      <c r="L69">
+        <v>3.048</v>
+      </c>
+      <c r="M69">
+        <v>3.1080000000000001</v>
+      </c>
+      <c r="N69">
+        <v>3.181</v>
+      </c>
+      <c r="O69">
+        <v>3.2029999999999998</v>
+      </c>
+      <c r="P69">
+        <v>3.2189999999999999</v>
+      </c>
+      <c r="Q69">
+        <v>3.2189999999999999</v>
+      </c>
+      <c r="R69">
+        <v>3.2229999999999999</v>
+      </c>
+      <c r="S69">
+        <v>3.37155</v>
+      </c>
+      <c r="T69">
+        <v>3.379</v>
+      </c>
+      <c r="U69">
+        <v>3.3783499999999997</v>
+      </c>
+      <c r="V69">
+        <v>3.3764560000000001</v>
+      </c>
+      <c r="W69">
+        <v>3.3692329999999999</v>
+      </c>
+      <c r="X69">
+        <v>3.348185</v>
+      </c>
+      <c r="Y69">
+        <v>3.3502800000000001</v>
+      </c>
+      <c r="Z69">
+        <v>3.3502800000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A70" t="s">
+        <v>8</v>
+      </c>
+      <c r="B70">
+        <v>3.532</v>
+      </c>
+      <c r="C70">
+        <v>3.532</v>
+      </c>
+      <c r="D70">
+        <v>2.722</v>
+      </c>
+      <c r="E70">
+        <v>2.722</v>
+      </c>
+      <c r="F70">
+        <v>2.722</v>
+      </c>
+      <c r="G70">
+        <v>2.722</v>
+      </c>
+      <c r="H70">
+        <v>2.722</v>
+      </c>
+      <c r="I70">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="J70">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="K70">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="L70">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="M70">
+        <v>1.8919999999999999</v>
+      </c>
+      <c r="N70">
+        <v>1.9059999999999999</v>
+      </c>
+      <c r="O70">
+        <v>1.982</v>
+      </c>
+      <c r="P70">
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="Q70">
+        <v>1.9750000000000001</v>
+      </c>
+      <c r="R70">
+        <v>1.9670000000000001</v>
+      </c>
+      <c r="S70">
+        <v>1.9670000000000001</v>
+      </c>
+      <c r="T70">
+        <v>2.008</v>
+      </c>
+      <c r="U70">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="V70">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="W70">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="X70">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="Y70">
+        <v>2.0059999999999998</v>
+      </c>
+      <c r="Z70">
+        <v>2.0059999999999998</v>
       </c>
     </row>
     <row r="71" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
-        <v>85</v>
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>5.6210000000000004</v>
+      </c>
+      <c r="C71">
+        <v>7.4059999999999997</v>
+      </c>
+      <c r="D71">
+        <v>6.8259999999999996</v>
+      </c>
+      <c r="E71">
+        <v>6.7519999999999998</v>
+      </c>
+      <c r="F71">
+        <v>6.6820000000000004</v>
+      </c>
+      <c r="G71">
+        <v>6.6749999999999998</v>
+      </c>
+      <c r="H71">
+        <v>6.4119999999999999</v>
+      </c>
+      <c r="I71">
+        <v>4.8959999999999999</v>
+      </c>
+      <c r="J71">
+        <v>4.641</v>
+      </c>
+      <c r="K71">
+        <v>4.3630000000000004</v>
+      </c>
+      <c r="L71">
+        <v>4.5679999999999996</v>
+      </c>
+      <c r="M71">
+        <v>4.5350000000000001</v>
+      </c>
+      <c r="N71">
+        <v>4.8979999999999997</v>
+      </c>
+      <c r="O71">
+        <v>4.6669999999999998</v>
+      </c>
+      <c r="P71">
+        <v>4.43</v>
+      </c>
+      <c r="Q71">
+        <v>3.9369999999999998</v>
+      </c>
+      <c r="R71">
+        <v>3.7650000000000001</v>
+      </c>
+      <c r="S71">
+        <v>3.7333600000000002</v>
+      </c>
+      <c r="T71">
+        <v>4.1509750000000007</v>
+      </c>
+      <c r="U71">
+        <v>4.040362</v>
+      </c>
+      <c r="V71">
+        <v>3.7584020000000002</v>
+      </c>
+      <c r="W71">
+        <v>3.8066649999999997</v>
+      </c>
+      <c r="X71">
+        <v>3.9745819999999998</v>
+      </c>
+      <c r="Y71">
+        <v>3.9745819999999998</v>
+      </c>
+      <c r="Z71">
+        <v>3.9745819999999998</v>
       </c>
     </row>
     <row r="72" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
-        <v>86</v>
-      </c>
-      <c r="B72" t="s">
-        <v>17</v>
-      </c>
-      <c r="C72">
-        <v>2000</v>
-      </c>
-      <c r="D72">
-        <v>2001</v>
-      </c>
-      <c r="E72">
-        <v>2002</v>
-      </c>
-      <c r="F72">
-        <v>2003</v>
-      </c>
-      <c r="G72">
-        <v>2004</v>
-      </c>
-      <c r="H72">
-        <v>2005</v>
+        <v>9</v>
       </c>
       <c r="I72">
-        <v>2006</v>
+        <v>2.9999999999999997E-5</v>
       </c>
       <c r="J72">
-        <v>2007</v>
+        <v>1E-4</v>
       </c>
       <c r="K72">
-        <v>2008</v>
+        <v>2E-3</v>
       </c>
       <c r="L72">
-        <v>2009</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M72">
-        <v>2010</v>
+        <v>0.154</v>
       </c>
       <c r="N72">
-        <v>2011</v>
+        <v>0.92200000000000004</v>
       </c>
       <c r="O72">
-        <v>2012</v>
+        <v>1.0389999999999999</v>
       </c>
       <c r="P72">
-        <v>2013</v>
+        <v>1.0289999999999999</v>
       </c>
       <c r="Q72">
-        <v>2014</v>
+        <v>1.028</v>
       </c>
       <c r="R72">
-        <v>2015</v>
+        <v>1.03</v>
       </c>
       <c r="S72">
-        <v>2016</v>
+        <v>1.0307010000000001</v>
       </c>
       <c r="T72">
-        <v>2017</v>
+        <v>1.033058</v>
       </c>
       <c r="U72">
-        <v>2018</v>
+        <v>1.0443900000000002</v>
       </c>
       <c r="V72">
-        <v>2019</v>
+        <v>1.1002110000000001</v>
       </c>
       <c r="W72">
-        <v>2020</v>
+        <v>1.274713</v>
       </c>
       <c r="X72">
-        <v>2021</v>
+        <v>1.736537</v>
       </c>
       <c r="Y72">
-        <v>2022</v>
+        <v>2.9081269999999999</v>
       </c>
       <c r="Z72">
-        <v>2023</v>
+        <v>3.9081269999999999</v>
       </c>
     </row>
     <row r="73" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
+        <v>10</v>
+      </c>
+      <c r="F73">
+        <v>1E-3</v>
+      </c>
+      <c r="G73">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H73">
+        <v>2.7E-2</v>
+      </c>
+      <c r="I73">
+        <v>0.03</v>
+      </c>
+      <c r="J73">
+        <v>0.114</v>
+      </c>
+      <c r="K73">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="L73">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="M73">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="N73">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="O73">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="P73">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="Q73">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="R73">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="S73">
+        <v>0.69838999999999996</v>
+      </c>
+      <c r="T73">
+        <v>0.69891999999999999</v>
+      </c>
+      <c r="U73">
+        <v>0.70311999999999997</v>
+      </c>
+      <c r="V73">
+        <v>0.70279999999999998</v>
+      </c>
+      <c r="W73">
+        <v>0.70437499999999997</v>
+      </c>
+      <c r="X73">
+        <v>0.70430999999999999</v>
+      </c>
+      <c r="Y73">
+        <v>0.70430999999999999</v>
+      </c>
+      <c r="Z73">
+        <v>0.70430999999999999</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A76" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A77" t="s">
+        <v>86</v>
+      </c>
+      <c r="B77" t="s">
+        <v>17</v>
+      </c>
+      <c r="C77">
+        <v>2000</v>
+      </c>
+      <c r="D77">
+        <v>2001</v>
+      </c>
+      <c r="E77">
+        <v>2002</v>
+      </c>
+      <c r="F77">
+        <v>2003</v>
+      </c>
+      <c r="G77">
+        <v>2004</v>
+      </c>
+      <c r="H77">
+        <v>2005</v>
+      </c>
+      <c r="I77">
+        <v>2006</v>
+      </c>
+      <c r="J77">
+        <v>2007</v>
+      </c>
+      <c r="K77">
+        <v>2008</v>
+      </c>
+      <c r="L77">
+        <v>2009</v>
+      </c>
+      <c r="M77">
+        <v>2010</v>
+      </c>
+      <c r="N77">
+        <v>2011</v>
+      </c>
+      <c r="O77">
+        <v>2012</v>
+      </c>
+      <c r="P77">
+        <v>2013</v>
+      </c>
+      <c r="Q77">
+        <v>2014</v>
+      </c>
+      <c r="R77">
+        <v>2015</v>
+      </c>
+      <c r="S77">
+        <v>2016</v>
+      </c>
+      <c r="T77">
+        <v>2017</v>
+      </c>
+      <c r="U77">
+        <v>2018</v>
+      </c>
+      <c r="V77">
+        <v>2019</v>
+      </c>
+      <c r="W77">
+        <v>2020</v>
+      </c>
+      <c r="X77">
+        <v>2021</v>
+      </c>
+      <c r="Y77">
+        <v>2022</v>
+      </c>
+      <c r="Z77">
+        <v>2023</v>
+      </c>
+    </row>
+    <row r="78" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A78" t="s">
         <v>87</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B78" t="s">
         <v>88</v>
       </c>
-      <c r="C73">
+      <c r="C78">
         <v>5.6</v>
       </c>
-      <c r="D73">
+      <c r="D78">
         <v>8</v>
       </c>
-      <c r="E73">
+      <c r="E78">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F73">
+      <c r="F78">
         <v>6.8</v>
       </c>
-      <c r="G73">
+      <c r="G78">
         <v>6.6</v>
       </c>
-      <c r="H73">
+      <c r="H78">
         <v>8.4</v>
       </c>
-      <c r="I73">
+      <c r="I78">
         <v>8.9</v>
       </c>
-      <c r="J73">
+      <c r="J78">
         <v>7.5</v>
       </c>
-      <c r="K73">
+      <c r="K78">
         <v>8.4</v>
       </c>
-      <c r="L73">
+      <c r="L78">
         <v>7.7</v>
       </c>
-      <c r="M73">
+      <c r="M78">
         <v>9.6</v>
       </c>
-      <c r="N73">
+      <c r="N78">
         <v>12.1</v>
       </c>
-      <c r="O73">
+      <c r="O78">
         <v>10.7</v>
       </c>
-      <c r="P73">
+      <c r="P78">
         <v>9.5</v>
       </c>
-      <c r="Q73">
+      <c r="Q78">
         <v>13.8</v>
       </c>
-      <c r="R73">
+      <c r="R78">
         <v>14.8</v>
       </c>
-      <c r="S73">
+      <c r="S78">
         <v>10.9</v>
       </c>
-      <c r="T73">
+      <c r="T78">
         <v>9.1999999999999993</v>
       </c>
-      <c r="U73">
+      <c r="U78">
         <v>10</v>
       </c>
-      <c r="V73">
+      <c r="V78">
         <v>8.9</v>
       </c>
-      <c r="W73">
+      <c r="W78">
         <v>7.1</v>
       </c>
-      <c r="X73">
+      <c r="X78">
         <v>10.6</v>
       </c>
-      <c r="Y73">
+      <c r="Y78">
         <v>13.7</v>
       </c>
-      <c r="Z73">
+      <c r="Z78">
         <v>7.7</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.45">
-      <c r="A74" t="s">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.45">
+      <c r="A79" t="s">
         <v>87</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B79" t="s">
         <v>89</v>
       </c>
-      <c r="C74">
+      <c r="C79">
         <v>1</v>
       </c>
-      <c r="D74">
+      <c r="D79">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E74">
+      <c r="E79">
         <v>2</v>
       </c>
-      <c r="F74">
+      <c r="F79">
         <v>1.3</v>
       </c>
-      <c r="G74">
+      <c r="G79">
         <v>0.7</v>
       </c>
-      <c r="H74">
+      <c r="H79">
         <v>0.8</v>
       </c>
-      <c r="I74">
+      <c r="I79">
         <v>1.1000000000000001</v>
       </c>
-      <c r="J74">
+      <c r="J79">
         <v>3.1</v>
       </c>
-      <c r="K74">
+      <c r="K79">
         <v>3.1</v>
       </c>
-      <c r="L74">
+      <c r="L79">
         <v>2.7</v>
       </c>
-      <c r="M74">
+      <c r="M79">
         <v>1.2</v>
       </c>
-      <c r="N74">
+      <c r="N79">
         <v>1.4</v>
       </c>
-      <c r="O74">
+      <c r="O79">
         <v>2.4</v>
       </c>
-      <c r="P74">
+      <c r="P79">
         <v>3.4</v>
       </c>
-      <c r="Q74">
+      <c r="Q79">
         <v>4.3</v>
       </c>
-      <c r="R74">
+      <c r="R79">
         <v>4.3</v>
       </c>
-      <c r="S74">
+      <c r="S79">
         <v>4.5999999999999996</v>
       </c>
-      <c r="T74">
+      <c r="T79">
         <v>3.7</v>
       </c>
-      <c r="U74">
+      <c r="U79">
         <v>2.2000000000000002</v>
       </c>
-      <c r="V74">
+      <c r="V79">
         <v>3</v>
       </c>
-      <c r="W74">
+      <c r="W79">
         <v>3.7</v>
       </c>
-      <c r="X74">
+      <c r="X79">
         <v>1.9</v>
       </c>
-      <c r="Y74">
+      <c r="Y79">
         <v>1.5</v>
       </c>
-      <c r="Z74">
+      <c r="Z79">
         <v>4.4000000000000004</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated BGR model - 2025-07-29 10:14
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -1292,10 +1292,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z83"/>
+  <dimension ref="A1:Z88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:Z83"/>
+      <selection activeCell="A1" sqref="A1:Z88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
@@ -5305,266 +5305,266 @@
         <v>0.70431</v>
       </c>
     </row>
-    <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="7" t="inlineStr">
+    <row r="84" ht="15.75" customHeight="1"/>
+    <row r="85" ht="15.75" customHeight="1">
+      <c r="A85" s="7" t="inlineStr">
         <is>
           <t>Electricity Trade Data (TWh) - Source: UNSD</t>
         </is>
       </c>
     </row>
-    <row r="81">
-      <c r="A81" s="8" t="inlineStr">
+    <row r="86">
+      <c r="A86" s="8" t="inlineStr">
         <is>
           <t>ISO</t>
         </is>
       </c>
-      <c r="B81" s="8" t="inlineStr">
+      <c r="B86" s="8" t="inlineStr">
         <is>
           <t>attribute</t>
         </is>
       </c>
-      <c r="C81" s="8" t="n">
+      <c r="C86" s="8" t="n">
         <v>2000</v>
       </c>
-      <c r="D81" s="8" t="n">
+      <c r="D86" s="8" t="n">
         <v>2001</v>
       </c>
-      <c r="E81" s="8" t="n">
+      <c r="E86" s="8" t="n">
         <v>2002</v>
       </c>
-      <c r="F81" s="8" t="n">
+      <c r="F86" s="8" t="n">
         <v>2003</v>
       </c>
-      <c r="G81" s="8" t="n">
+      <c r="G86" s="8" t="n">
         <v>2004</v>
       </c>
-      <c r="H81" s="8" t="n">
+      <c r="H86" s="8" t="n">
         <v>2005</v>
       </c>
-      <c r="I81" s="8" t="n">
+      <c r="I86" s="8" t="n">
         <v>2006</v>
       </c>
-      <c r="J81" s="8" t="n">
+      <c r="J86" s="8" t="n">
         <v>2007</v>
       </c>
-      <c r="K81" s="8" t="n">
+      <c r="K86" s="8" t="n">
         <v>2008</v>
       </c>
-      <c r="L81" s="8" t="n">
+      <c r="L86" s="8" t="n">
         <v>2009</v>
       </c>
-      <c r="M81" s="8" t="n">
+      <c r="M86" s="8" t="n">
         <v>2010</v>
       </c>
-      <c r="N81" s="8" t="n">
+      <c r="N86" s="8" t="n">
         <v>2011</v>
       </c>
-      <c r="O81" s="8" t="n">
+      <c r="O86" s="8" t="n">
         <v>2012</v>
       </c>
-      <c r="P81" s="8" t="n">
+      <c r="P86" s="8" t="n">
         <v>2013</v>
       </c>
-      <c r="Q81" s="8" t="n">
+      <c r="Q86" s="8" t="n">
         <v>2014</v>
       </c>
-      <c r="R81" s="8" t="n">
+      <c r="R86" s="8" t="n">
         <v>2015</v>
       </c>
-      <c r="S81" s="8" t="n">
+      <c r="S86" s="8" t="n">
         <v>2016</v>
       </c>
-      <c r="T81" s="8" t="n">
+      <c r="T86" s="8" t="n">
         <v>2017</v>
       </c>
-      <c r="U81" s="8" t="n">
+      <c r="U86" s="8" t="n">
         <v>2018</v>
       </c>
-      <c r="V81" s="8" t="n">
+      <c r="V86" s="8" t="n">
         <v>2019</v>
       </c>
-      <c r="W81" s="8" t="n">
+      <c r="W86" s="8" t="n">
         <v>2020</v>
       </c>
-      <c r="X81" s="8" t="n">
+      <c r="X86" s="8" t="n">
         <v>2021</v>
       </c>
-      <c r="Y81" s="8" t="n">
+      <c r="Y86" s="8" t="n">
         <v>2022</v>
       </c>
-      <c r="Z81" s="8" t="n">
+      <c r="Z86" s="8" t="n">
         <v>2023</v>
       </c>
     </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
+    <row r="87">
+      <c r="A87" t="inlineStr">
         <is>
           <t>BGR</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B87" t="inlineStr">
         <is>
           <t>Export</t>
         </is>
       </c>
-      <c r="C82" s="10" t="n">
+      <c r="C87" s="10" t="n">
         <v>5.6</v>
       </c>
-      <c r="D82" s="10" t="n">
+      <c r="D87" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E82" s="10" t="n">
+      <c r="E87" s="10" t="n">
         <v>8.300000000000001</v>
       </c>
-      <c r="F82" s="10" t="n">
+      <c r="F87" s="10" t="n">
         <v>6.8</v>
       </c>
-      <c r="G82" s="10" t="n">
+      <c r="G87" s="10" t="n">
         <v>6.6</v>
       </c>
-      <c r="H82" s="10" t="n">
+      <c r="H87" s="10" t="n">
         <v>8.4</v>
       </c>
-      <c r="I82" s="10" t="n">
+      <c r="I87" s="10" t="n">
         <v>8.9</v>
       </c>
-      <c r="J82" s="10" t="n">
+      <c r="J87" s="10" t="n">
         <v>7.5</v>
       </c>
-      <c r="K82" s="10" t="n">
+      <c r="K87" s="10" t="n">
         <v>8.4</v>
       </c>
-      <c r="L82" s="10" t="n">
+      <c r="L87" s="10" t="n">
         <v>7.7</v>
       </c>
-      <c r="M82" s="10" t="n">
+      <c r="M87" s="10" t="n">
         <v>9.6</v>
       </c>
-      <c r="N82" s="10" t="n">
+      <c r="N87" s="10" t="n">
         <v>12.1</v>
       </c>
-      <c r="O82" s="10" t="n">
+      <c r="O87" s="10" t="n">
         <v>10.7</v>
       </c>
-      <c r="P82" s="10" t="n">
+      <c r="P87" s="10" t="n">
         <v>9.5</v>
       </c>
-      <c r="Q82" s="10" t="n">
+      <c r="Q87" s="10" t="n">
         <v>13.8</v>
       </c>
-      <c r="R82" s="10" t="n">
+      <c r="R87" s="10" t="n">
         <v>14.8</v>
       </c>
-      <c r="S82" s="10" t="n">
+      <c r="S87" s="10" t="n">
         <v>10.9</v>
       </c>
-      <c r="T82" s="10" t="n">
+      <c r="T87" s="10" t="n">
         <v>9.199999999999999</v>
       </c>
-      <c r="U82" s="10" t="n">
+      <c r="U87" s="10" t="n">
         <v>10</v>
       </c>
-      <c r="V82" s="10" t="n">
+      <c r="V87" s="10" t="n">
         <v>8.9</v>
       </c>
-      <c r="W82" s="10" t="n">
+      <c r="W87" s="10" t="n">
         <v>7.1</v>
       </c>
-      <c r="X82" s="10" t="n">
+      <c r="X87" s="10" t="n">
         <v>10.6</v>
       </c>
-      <c r="Y82" s="10" t="n">
+      <c r="Y87" s="10" t="n">
         <v>13.7</v>
       </c>
-      <c r="Z82" s="10" t="n">
+      <c r="Z87" s="10" t="n">
         <v>7.7</v>
       </c>
     </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
+    <row r="88">
+      <c r="A88" t="inlineStr">
         <is>
           <t>BGR</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B88" t="inlineStr">
         <is>
           <t>Import</t>
         </is>
       </c>
-      <c r="C83" s="10" t="n">
+      <c r="C88" s="10" t="n">
         <v>1</v>
       </c>
-      <c r="D83" s="10" t="n">
+      <c r="D88" s="10" t="n">
         <v>1.1</v>
       </c>
-      <c r="E83" s="10" t="n">
+      <c r="E88" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="F83" s="10" t="n">
+      <c r="F88" s="10" t="n">
         <v>1.3</v>
       </c>
-      <c r="G83" s="10" t="n">
+      <c r="G88" s="10" t="n">
         <v>0.7</v>
       </c>
-      <c r="H83" s="10" t="n">
+      <c r="H88" s="10" t="n">
         <v>0.8</v>
       </c>
-      <c r="I83" s="10" t="n">
+      <c r="I88" s="10" t="n">
         <v>1.1</v>
       </c>
-      <c r="J83" s="10" t="n">
+      <c r="J88" s="10" t="n">
         <v>3.1</v>
       </c>
-      <c r="K83" s="10" t="n">
+      <c r="K88" s="10" t="n">
         <v>3.1</v>
       </c>
-      <c r="L83" s="10" t="n">
+      <c r="L88" s="10" t="n">
         <v>2.7</v>
       </c>
-      <c r="M83" s="10" t="n">
+      <c r="M88" s="10" t="n">
         <v>1.2</v>
       </c>
-      <c r="N83" s="10" t="n">
+      <c r="N88" s="10" t="n">
         <v>1.4</v>
       </c>
-      <c r="O83" s="10" t="n">
+      <c r="O88" s="10" t="n">
         <v>2.4</v>
       </c>
-      <c r="P83" s="10" t="n">
+      <c r="P88" s="10" t="n">
         <v>3.4</v>
       </c>
-      <c r="Q83" s="10" t="n">
+      <c r="Q88" s="10" t="n">
         <v>4.3</v>
       </c>
-      <c r="R83" s="10" t="n">
+      <c r="R88" s="10" t="n">
         <v>4.3</v>
       </c>
-      <c r="S83" s="10" t="n">
+      <c r="S88" s="10" t="n">
         <v>4.6</v>
       </c>
-      <c r="T83" s="10" t="n">
+      <c r="T88" s="10" t="n">
         <v>3.7</v>
       </c>
-      <c r="U83" s="10" t="n">
+      <c r="U88" s="10" t="n">
         <v>2.2</v>
       </c>
-      <c r="V83" s="10" t="n">
+      <c r="V88" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="W83" s="10" t="n">
+      <c r="W88" s="10" t="n">
         <v>3.7</v>
       </c>
-      <c r="X83" s="10" t="n">
+      <c r="X88" s="10" t="n">
         <v>1.9</v>
       </c>
-      <c r="Y83" s="10" t="n">
+      <c r="Y88" s="10" t="n">
         <v>1.5</v>
       </c>
-      <c r="Z83" s="10" t="n">
+      <c r="Z88" s="10" t="n">
         <v>4.4</v>
       </c>
     </row>
-    <row r="84" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated BGR model - 2025-08-14 19:09
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97E58345-7FC0-42E5-8D1D-E1B9BC6223BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9866754A-9A2F-4AA0-8786-75061248B271}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1513" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="80">
   <si>
     <t>~TFM_INS-AT</t>
   </si>
@@ -327,6 +327,15 @@
   </si>
   <si>
     <t>UC_RHSRT~2050</t>
+  </si>
+  <si>
+    <t>life</t>
+  </si>
+  <si>
+    <t>g[_]*</t>
+  </si>
+  <si>
+    <t>prc_capact</t>
   </si>
 </sst>
 </file>
@@ -814,8 +823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1355,6 +1364,9 @@
       <c r="F21" t="s">
         <v>14</v>
       </c>
+      <c r="G21" t="s">
+        <v>3</v>
+      </c>
       <c r="L21" t="s">
         <v>38</v>
       </c>
@@ -1475,8 +1487,28 @@
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28">
+        <v>50</v>
+      </c>
+      <c r="G28" t="s">
+        <v>78</v>
+      </c>
       <c r="L28" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29">
+        <v>8.76</v>
+      </c>
+      <c r="G29" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Updated DEU model - 2025-08-19 15:00
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A414CAD-60F2-447D-A730-0DFD90DA9BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0012C232-CE69-41C0-A6A6-F23299436421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Veda" sheetId="1" r:id="rId1"/>
@@ -547,7 +547,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -564,13 +564,10 @@
     <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="9" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
@@ -1698,7 +1695,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1711,16 +1708,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="9" spans="1:10" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B9" s="10" t="s">
@@ -1728,60 +1725,60 @@
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C10" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="E10" s="17" t="s">
+      <c r="E10" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="F10" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="17" t="s">
+      <c r="I10" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="J10" s="17" t="s">
+      <c r="J10" s="11" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="19">
+      <c r="C11" s="13">
         <v>1.2</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="13">
         <v>1.8</v>
       </c>
-      <c r="E11" s="20">
+      <c r="E11" s="16">
         <v>0.8</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="13">
         <v>1.2</v>
       </c>
-      <c r="G11" s="20">
+      <c r="G11" s="16">
         <v>0.05</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="16">
         <v>0.1</v>
       </c>
-      <c r="I11" s="20">
+      <c r="I11" s="16">
         <v>0.5</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="13">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated BGR model - 2025-08-21 22:55
</commit_message>
<xml_diff>
--- a/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
+++ b/VerveStacks_BGR/SuppXLS/Scen_Base_VS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_BGR\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DFA32418-A3A0-4B86-94B1-7985EAE1613A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{406B7773-B018-4A38-9B8E-FA561BF012C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -611,7 +611,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59926F54-1552-0240-90E7-D91C79D653FD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76C42756-2440-482D-8F33-CC47E5832B28}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>

</xml_diff>